<commit_message>
fill some gaps and colorize benchmark results
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B1B8C158-F198-4A76-95B0-04D6417EFFDD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8F24B6B6-5987-4738-8ABA-4D0C7ED40AEB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t> 29</t>
   </si>
   <si>
-    <t xml:space="preserve"> Manufacturer</t>
-  </si>
-  <si>
     <t>CPU Model</t>
   </si>
   <si>
@@ -160,12 +157,18 @@
   </si>
   <si>
     <t>Atom E3815</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,19 +218,1435 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="181">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC2A6A6"/>
+      <color rgb="FFFF9966"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -243,14 +1662,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:R1048576" totalsRowShown="0">
   <autoFilter ref="A1:R1048576" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name=" Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#"/>
+    <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="180"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="124"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="125"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="161"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -567,20 +1986,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R20" sqref="R20"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
     <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -589,67 +2008,67 @@
     <col min="15" max="18" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -661,13 +2080,13 @@
       <c r="E2">
         <v>8</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>3.6</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>4</v>
       </c>
       <c r="I2" t="s">
@@ -703,24 +2122,27 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
+      <c r="D3">
+        <v>65</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>3.6</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>4.2</v>
       </c>
       <c r="I3" t="s">
@@ -753,24 +2175,27 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>1.6</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>3.4</v>
       </c>
       <c r="I4" t="s">
@@ -803,13 +2228,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>45</v>
@@ -817,13 +2242,13 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>2.8</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>3.4</v>
       </c>
       <c r="I5" t="s">
@@ -858,11 +2283,11 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>280</v>
@@ -870,13 +2295,13 @@
       <c r="E6">
         <v>32</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
         <v>2.6</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>2.9</v>
       </c>
       <c r="I6" t="s">
@@ -892,7 +2317,7 @@
         <v>8</v>
       </c>
       <c r="M6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N6">
         <v>1333</v>
@@ -912,24 +2337,27 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>77</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
         <v>3.4</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>3.8</v>
       </c>
       <c r="I7" t="s">
@@ -942,7 +2370,7 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N7">
         <v>1600</v>
@@ -964,25 +2392,25 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E8">
         <v>8</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
         <v>3.6</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>4</v>
       </c>
       <c r="I8" t="s">
@@ -998,7 +2426,7 @@
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N8">
         <v>1600</v>
@@ -1018,24 +2446,27 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>2.9</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>3.5</v>
       </c>
       <c r="I9" t="s">
@@ -1068,24 +2499,27 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="D10">
+        <v>51</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
         <v>2.8</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>2.8</v>
       </c>
       <c r="I10" t="s">
@@ -1120,11 +2554,11 @@
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11">
         <v>280</v>
@@ -1132,20 +2566,20 @@
       <c r="E11">
         <v>32</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
         <v>1.3</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>1.3</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K11">
         <v>64</v>
@@ -1154,7 +2588,7 @@
         <v>8</v>
       </c>
       <c r="M11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N11">
         <v>1333</v>
@@ -1169,29 +2603,32 @@
         <v>5.2</v>
       </c>
       <c r="R11">
-        <v>109</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <v>95</v>
       </c>
       <c r="E12">
         <v>6</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
         <v>3.5</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>3.5</v>
       </c>
       <c r="I12" t="s">
@@ -1204,7 +2641,7 @@
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N12">
         <v>1333</v>
@@ -1226,32 +2663,32 @@
       <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E13">
         <v>8</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
         <v>3.6</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>3.6</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K13">
         <v>24</v>
@@ -1260,7 +2697,7 @@
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N13">
         <v>1600</v>
@@ -1282,11 +2719,11 @@
       <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14">
         <v>25</v>
@@ -1294,13 +2731,13 @@
       <c r="E14">
         <v>4</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
         <v>2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>2</v>
       </c>
       <c r="I14" t="s">
@@ -1313,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N14">
         <v>1600</v>
@@ -1333,24 +2770,27 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
         <v>1.6</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>2.1</v>
       </c>
       <c r="I15" t="s">
@@ -1366,7 +2806,7 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N15">
         <v>1600</v>
@@ -1386,24 +2826,27 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="D16">
+        <v>34</v>
       </c>
       <c r="E16">
         <v>2</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
         <v>2</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>2</v>
       </c>
       <c r="I16" t="s">
@@ -1416,7 +2859,7 @@
         <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N16">
         <v>667</v>
@@ -1430,19 +2873,19 @@
       <c r="Q16">
         <v>15.9</v>
       </c>
-      <c r="R16" s="2" t="s">
-        <v>40</v>
+      <c r="R16" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1450,17 +2893,17 @@
       <c r="E17">
         <v>4</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
         <v>1.3</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>1.8</v>
       </c>
       <c r="I17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K17">
         <v>2</v>
@@ -1469,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N17">
         <v>1333</v>
@@ -1483,19 +2926,19 @@
       <c r="Q17">
         <v>62</v>
       </c>
-      <c r="R17" s="2" t="s">
-        <v>40</v>
+      <c r="R17" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1503,17 +2946,17 @@
       <c r="E18">
         <v>4</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
         <v>1.3</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>1.8</v>
       </c>
       <c r="I18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1522,7 +2965,7 @@
         <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N18">
         <v>1333</v>
@@ -1533,22 +2976,22 @@
       <c r="P18">
         <v>30.5</v>
       </c>
-      <c r="Q18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>40</v>
+      <c r="Q18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -1556,13 +2999,13 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
         <v>1.4</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>1.4</v>
       </c>
       <c r="I19" t="s">
@@ -1578,7 +3021,7 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N19">
         <v>1600</v>
@@ -1597,9 +3040,222 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I1048576">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+      <formula>"x86-32"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:R1048576">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+      <formula>"OOM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K1048576">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0367AC6D-DDF3-42AF-AC1A-A8D437802C33}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{769BD0BC-E3E0-4DCC-B1ED-8FCB849998EF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4F31A67C-5F53-4BA7-A05C-64FCDA72461D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:H1048576">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B3B407FB-2D4D-463A-AD8A-DEC691552228}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F1048576 L2:L1048576">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M1048576">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"DDR2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"DDR4"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N1048576">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{463BE009-64FC-4160-9507-16F4AF063486}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0367AC6D-DDF3-42AF-AC1A-A8D437802C33}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0" direction="leftToRight">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{769BD0BC-E3E0-4DCC-B1ED-8FCB849998EF}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4F31A67C-5F53-4BA7-A05C-64FCDA72461D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B3B407FB-2D4D-463A-AD8A-DEC691552228}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G1:H1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{463BE009-64FC-4160-9507-16F4AF063486}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N1:N1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added benchmark results for Ryzen 5 3600X
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35486363-EC5D-424E-BCEE-E527252073ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758E6DBB-FC84-40C7-B6B1-CBB158862FFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
+    <workbookView xWindow="3225" yWindow="1463" windowWidth="25035" windowHeight="13027" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Cores</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>x86-32 (emu)</t>
+  </si>
+  <si>
+    <t>Ryzen 5 3600X</t>
   </si>
 </sst>
 </file>
@@ -350,7 +353,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:R1048576" totalsRowShown="0">
   <autoFilter ref="A1:R1048576" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState ref="A2:R21">
+  <sortState ref="A2:R22">
     <sortCondition ref="O1:O1048576"/>
   </sortState>
   <tableColumns count="18">
@@ -674,11 +677,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -814,28 +817,28 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="D3">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="3">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="H3" s="3">
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -850,19 +853,19 @@
         <v>13</v>
       </c>
       <c r="N3">
-        <v>2366</v>
+        <v>3200</v>
       </c>
       <c r="O3">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="P3">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>2.2999999999999998</v>
+        <v>1.8</v>
       </c>
       <c r="R3">
-        <v>4.5999999999999996</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
@@ -873,10 +876,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -885,37 +888,37 @@
         <v>2</v>
       </c>
       <c r="G4" s="3">
-        <v>1.6</v>
+        <v>3.6</v>
       </c>
       <c r="H4" s="3">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" t="s">
         <v>13</v>
       </c>
       <c r="N4">
-        <v>2400</v>
+        <v>2366</v>
       </c>
       <c r="O4">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="P4">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q4">
-        <v>3.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R4">
-        <v>6.5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
@@ -926,10 +929,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -938,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="3">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="H5" s="3">
         <v>3.4</v>
@@ -947,7 +950,7 @@
         <v>11</v>
       </c>
       <c r="K5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -962,60 +965,57 @@
         <v>0.8</v>
       </c>
       <c r="P5">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q5">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R5">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H6" s="3">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
       </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
       <c r="K6">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N6">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O6">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P6">
         <v>1.7</v>
@@ -1024,130 +1024,130 @@
         <v>3.3</v>
       </c>
       <c r="R6">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7">
-        <v>77</v>
+        <v>280</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="3">
-        <v>3.4</v>
+        <v>2.6</v>
       </c>
       <c r="H7" s="3">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
       <c r="K7">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M7" t="s">
         <v>27</v>
       </c>
       <c r="N7">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O7">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="P7">
         <v>1.7</v>
       </c>
       <c r="Q7">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="R7">
-        <v>8</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="1">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>77</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8">
+        <v>1600</v>
+      </c>
+      <c r="O8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P8">
+        <v>1.7</v>
+      </c>
+      <c r="Q8">
         <v>3.5</v>
       </c>
-      <c r="E8">
+      <c r="R8">
         <v>8</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8">
-        <v>6</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N8">
-        <v>1866</v>
-      </c>
-      <c r="O8">
-        <v>1.2</v>
-      </c>
-      <c r="P8">
-        <v>2.5</v>
-      </c>
-      <c r="Q8">
-        <v>5</v>
-      </c>
-      <c r="R8">
-        <v>10.3</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9">
-        <v>125</v>
+        <v>45</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3.5</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1156,93 +1156,96 @@
         <v>1</v>
       </c>
       <c r="G9" s="3">
-        <v>3.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H9" s="3">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K9">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N9">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O9">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="P9">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="Q9">
-        <v>4.5999999999999996</v>
+        <v>5</v>
       </c>
       <c r="R9">
-        <v>8.8000000000000007</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>2.9</v>
+        <v>3.6</v>
       </c>
       <c r="H10" s="3">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
       <c r="K10">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="L10">
         <v>2</v>
       </c>
       <c r="M10" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N10">
-        <v>2133</v>
+        <v>1600</v>
       </c>
       <c r="O10">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="P10">
-        <v>2.9</v>
+        <v>2.6</v>
       </c>
       <c r="Q10">
-        <v>5.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="R10">
-        <v>10.6</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
@@ -1253,28 +1256,28 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="3">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="H11" s="3">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
       <c r="K11">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -1283,7 +1286,7 @@
         <v>13</v>
       </c>
       <c r="N11">
-        <v>2800</v>
+        <v>2133</v>
       </c>
       <c r="O11">
         <v>1.5</v>
@@ -1292,66 +1295,63 @@
         <v>2.9</v>
       </c>
       <c r="Q11">
-        <v>6.2</v>
+        <v>5.7</v>
       </c>
       <c r="R11">
-        <v>12.4</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D12">
-        <v>280</v>
+        <v>51</v>
       </c>
       <c r="E12">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="3">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="H12" s="3">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
-      <c r="J12" t="s">
-        <v>32</v>
-      </c>
       <c r="K12">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="L12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N12">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O12">
         <v>1.5</v>
       </c>
       <c r="P12">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q12">
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="R12">
-        <v>10.9</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
@@ -1359,34 +1359,37 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="H13" s="3">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
       <c r="K13">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M13" t="s">
         <v>27</v>
@@ -1395,16 +1398,16 @@
         <v>1333</v>
       </c>
       <c r="O13">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P13">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Q13">
-        <v>6.6</v>
+        <v>5.2</v>
       </c>
       <c r="R13">
-        <v>13.6</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
@@ -1415,31 +1418,28 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D14">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
       <c r="G14" s="3">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="H14" s="3">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
-      <c r="J14" t="s">
-        <v>34</v>
-      </c>
       <c r="K14">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="L14">
         <v>2</v>
@@ -1448,19 +1448,19 @@
         <v>27</v>
       </c>
       <c r="N14">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O14">
-        <v>2.7</v>
+        <v>1.7</v>
       </c>
       <c r="P14">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="Q14">
-        <v>10.1</v>
+        <v>6.6</v>
       </c>
       <c r="R14">
-        <v>22.4</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
@@ -1471,28 +1471,31 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D15">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="H15" s="3">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
       <c r="K15">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="L15">
         <v>2</v>
@@ -1507,27 +1510,27 @@
         <v>2.7</v>
       </c>
       <c r="P15">
-        <v>5.0999999999999996</v>
+        <v>5</v>
       </c>
       <c r="Q15">
-        <v>10.8</v>
+        <v>10.1</v>
       </c>
       <c r="R15">
-        <v>21.5</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1536,22 +1539,19 @@
         <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="H16" s="3">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
-        <v>12</v>
-      </c>
       <c r="K16">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" t="s">
         <v>27</v>
@@ -1560,16 +1560,16 @@
         <v>1600</v>
       </c>
       <c r="O16">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="P16">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q16">
-        <v>12.3</v>
+        <v>10.8</v>
       </c>
       <c r="R16">
-        <v>23.9</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
@@ -1580,102 +1580,102 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="H17" s="3">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
       <c r="K17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="N17">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O17">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="P17">
-        <v>7.8</v>
+        <v>6.4</v>
       </c>
       <c r="Q17">
-        <v>15.9</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>39</v>
+        <v>12.3</v>
+      </c>
+      <c r="R17">
+        <v>23.9</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="1">
-        <v>3.5</v>
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>34</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H18" s="3">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>48</v>
-      </c>
-      <c r="J18" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N18">
-        <v>1866</v>
+        <v>667</v>
       </c>
       <c r="O18">
-        <v>8.3000000000000007</v>
+        <v>3.8</v>
       </c>
       <c r="P18">
-        <v>16.100000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="Q18">
-        <v>33.799999999999997</v>
+        <v>15.9</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>39</v>
@@ -1683,52 +1683,55 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.5</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H19" s="3">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I19" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L19">
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N19">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O19">
-        <v>11.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P19">
-        <v>30.5</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>39</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q19">
+        <v>33.799999999999997</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>39</v>
@@ -1763,7 +1766,7 @@
         <v>41</v>
       </c>
       <c r="K20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -1775,13 +1778,13 @@
         <v>1333</v>
       </c>
       <c r="O20">
-        <v>11.8</v>
+        <v>11.3</v>
       </c>
       <c r="P20">
-        <v>23.2</v>
-      </c>
-      <c r="Q20">
-        <v>62</v>
+        <v>30.5</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="R20" s="1" t="s">
         <v>39</v>
@@ -1795,31 +1798,28 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H21" s="3">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K21">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -1828,18 +1828,74 @@
         <v>27</v>
       </c>
       <c r="N21">
+        <v>1333</v>
+      </c>
+      <c r="O21">
+        <v>11.8</v>
+      </c>
+      <c r="P21">
+        <v>23.2</v>
+      </c>
+      <c r="Q21">
+        <v>62</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22">
+        <v>8</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22">
         <v>1600</v>
       </c>
-      <c r="O21">
+      <c r="O22">
         <v>13.1</v>
       </c>
-      <c r="P21">
+      <c r="P22">
         <v>27.2</v>
       </c>
-      <c r="Q21">
+      <c r="Q22">
         <v>56.8</v>
       </c>
-      <c r="R21">
+      <c r="R22">
         <v>117.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reruns for more precise results
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758E6DBB-FC84-40C7-B6B1-CBB158862FFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED75DCFF-DC9B-4173-ADDD-FCBCC2878825}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="1463" windowWidth="25035" windowHeight="13027" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t>Cores</t>
   </si>
@@ -178,6 +178,34 @@
   </si>
   <si>
     <t>Ryzen 5 3600X</t>
+  </si>
+  <si>
+    <t>Xeon E5-2630 v4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Intel</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -187,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +228,22 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -259,20 +303,63 @@
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -331,6 +418,20 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -351,20 +452,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:R1048576" totalsRowShown="0">
-  <autoFilter ref="A1:R1048576" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:R1048575" totalsRowShown="0">
+  <autoFilter ref="A1:R1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
   <sortState ref="A2:R22">
-    <sortCondition ref="O1:O1048576"/>
+    <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="14"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -681,7 +782,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S15" sqref="S15"/>
+      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -803,16 +904,16 @@
         <v>3333</v>
       </c>
       <c r="O2">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P2">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="Q2">
         <v>1.8</v>
       </c>
       <c r="R2">
-        <v>3.6</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
@@ -1085,34 +1186,34 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="H8" s="3">
         <v>4</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="H8" s="3">
-        <v>3.8</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="L8">
         <v>2</v>
@@ -1124,86 +1225,83 @@
         <v>1600</v>
       </c>
       <c r="O8">
-        <v>1.1000000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P8">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="Q8">
-        <v>3.5</v>
+        <v>4.09</v>
       </c>
       <c r="R8">
-        <v>8</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="1">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>77</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9">
+        <v>1600</v>
+      </c>
+      <c r="O9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P9">
+        <v>1.7</v>
+      </c>
+      <c r="Q9">
         <v>3.5</v>
       </c>
-      <c r="E9">
+      <c r="R9">
         <v>8</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9">
-        <v>6</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9">
-        <v>1866</v>
-      </c>
-      <c r="O9">
-        <v>1.2</v>
-      </c>
-      <c r="P9">
-        <v>2.5</v>
-      </c>
-      <c r="Q9">
-        <v>5</v>
-      </c>
-      <c r="R9">
-        <v>10.3</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10">
-        <v>125</v>
+        <v>45</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3.5</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -1212,40 +1310,40 @@
         <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>3.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H10" s="3">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K10">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N10">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O10">
-        <v>1.3</v>
+        <v>1.26</v>
       </c>
       <c r="P10">
-        <v>2.6</v>
+        <v>2.57</v>
       </c>
       <c r="Q10">
-        <v>4.5999999999999996</v>
+        <v>5.16</v>
       </c>
       <c r="R10">
-        <v>8.8000000000000007</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
@@ -1471,31 +1569,28 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D15">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="H15" s="3">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
-      <c r="J15" t="s">
-        <v>34</v>
-      </c>
       <c r="K15">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L15">
         <v>2</v>
@@ -1510,27 +1605,27 @@
         <v>2.7</v>
       </c>
       <c r="P15">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q15">
-        <v>10.1</v>
+        <v>10.8</v>
       </c>
       <c r="R15">
-        <v>22.4</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1539,19 +1634,22 @@
         <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="H16" s="3">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
+      <c r="J16" t="s">
+        <v>12</v>
+      </c>
       <c r="K16">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M16" t="s">
         <v>27</v>
@@ -1560,72 +1658,69 @@
         <v>1600</v>
       </c>
       <c r="O16">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="P16">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="Q16">
-        <v>10.8</v>
+        <v>12.3</v>
       </c>
       <c r="R16">
-        <v>21.5</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H17" s="3">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
       <c r="K17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N17">
         <v>1600</v>
       </c>
       <c r="O17">
-        <v>2.9</v>
+        <v>3.56</v>
       </c>
       <c r="P17">
-        <v>6.4</v>
+        <v>8.07</v>
       </c>
       <c r="Q17">
-        <v>12.3</v>
+        <v>15.55</v>
       </c>
       <c r="R17">
-        <v>23.9</v>
+        <v>34.93</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
@@ -1778,10 +1873,10 @@
         <v>1333</v>
       </c>
       <c r="O20">
-        <v>11.3</v>
+        <v>10.45</v>
       </c>
       <c r="P20">
-        <v>30.5</v>
+        <v>23.55</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>39</v>
@@ -1900,27 +1995,28 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="greaterThan">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B2:B1048575">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I1048576">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+  <conditionalFormatting sqref="I2:I1048575">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>"x86-32"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:R1048576">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+  <conditionalFormatting sqref="O2:R1048575">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>"OOM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="F2:F1048575">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K1048576">
+  <conditionalFormatting sqref="K2:K1048575">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
@@ -1934,7 +2030,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D1048575">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
@@ -1948,7 +2044,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E1:E1048575">
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
@@ -1962,7 +2058,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1048576">
+  <conditionalFormatting sqref="G1:H1048575">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="min"/>
@@ -1976,20 +2072,20 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048576 L2:L1048576">
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="greaterThan">
+  <conditionalFormatting sqref="F2:F1048575 L2:L1048575">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+  <conditionalFormatting sqref="M1:M1048575">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"DDR4"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"DDR2"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576">
+  <conditionalFormatting sqref="N1:N1048575">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
@@ -2003,7 +2099,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
+  <conditionalFormatting sqref="P1:P1048575">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2015,7 +2111,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048576">
+  <conditionalFormatting sqref="O1:O1048575">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2027,7 +2123,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1048576">
+  <conditionalFormatting sqref="Q1:Q1048575">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2039,7 +2135,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1048576">
+  <conditionalFormatting sqref="R1:R1048575">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2068,7 +2164,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>K2:K1048575</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{769BD0BC-E3E0-4DCC-B1ED-8FCB849998EF}">
@@ -2079,7 +2175,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D1:D1048576</xm:sqref>
+          <xm:sqref>D1:D1048575</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4F31A67C-5F53-4BA7-A05C-64FCDA72461D}">
@@ -2090,7 +2186,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>E1:E1048575</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B3B407FB-2D4D-463A-AD8A-DEC691552228}">
@@ -2101,7 +2197,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G1:H1048576</xm:sqref>
+          <xm:sqref>G1:H1048575</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{463BE009-64FC-4160-9507-16F4AF063486}">
@@ -2112,7 +2208,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N1:N1048576</xm:sqref>
+          <xm:sqref>N1:N1048575</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
add results for 12-core Opteron 6180 SE
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED75DCFF-DC9B-4173-ADDD-FCBCC2878825}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62ED8AD-B1CE-468B-ABA4-A7A262C08F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
   <si>
     <t>Cores</t>
   </si>
@@ -206,6 +206,9 @@
       </rPr>
       <t xml:space="preserve"> Intel</t>
     </r>
+  </si>
+  <si>
+    <t>Opteron 6180 SE</t>
   </si>
 </sst>
 </file>
@@ -303,63 +306,20 @@
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="11">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2A6A6"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -418,20 +378,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -454,18 +400,18 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:R1048575" totalsRowShown="0">
   <autoFilter ref="A1:R1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState ref="A2:R22">
+  <sortState ref="A2:R23">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -778,11 +724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1292,111 +1238,114 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3.5</v>
+        <v>52</v>
+      </c>
+      <c r="D10">
+        <v>140</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="H10" s="3">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K10">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N10">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O10">
-        <v>1.26</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P10">
-        <v>2.57</v>
+        <v>2.17</v>
       </c>
       <c r="Q10">
-        <v>5.16</v>
+        <v>4.16</v>
       </c>
       <c r="R10">
-        <v>10.47</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.5</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="3">
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H11" s="3">
-        <v>3.5</v>
+        <v>2.4</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
       </c>
       <c r="K11">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N11">
-        <v>2133</v>
+        <v>1866</v>
       </c>
       <c r="O11">
-        <v>1.5</v>
+        <v>1.26</v>
       </c>
       <c r="P11">
-        <v>2.9</v>
+        <v>2.57</v>
       </c>
       <c r="Q11">
-        <v>5.7</v>
+        <v>5.16</v>
       </c>
       <c r="R11">
-        <v>10.6</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
@@ -1407,28 +1356,28 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="3">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="H12" s="3">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
       <c r="K12">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L12">
         <v>2</v>
@@ -1437,7 +1386,7 @@
         <v>13</v>
       </c>
       <c r="N12">
-        <v>2800</v>
+        <v>2133</v>
       </c>
       <c r="O12">
         <v>1.5</v>
@@ -1446,66 +1395,63 @@
         <v>2.9</v>
       </c>
       <c r="Q12">
-        <v>6.2</v>
+        <v>5.7</v>
       </c>
       <c r="R12">
-        <v>12.4</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D13">
-        <v>280</v>
+        <v>51</v>
       </c>
       <c r="E13">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="H13" s="3">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
-      <c r="J13" t="s">
-        <v>32</v>
-      </c>
       <c r="K13">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="L13">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N13">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O13">
         <v>1.5</v>
       </c>
       <c r="P13">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q13">
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="R13">
-        <v>10.9</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
@@ -1513,34 +1459,37 @@
         <v>5</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
       <c r="G14" s="3">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="H14" s="3">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
+      <c r="J14" t="s">
+        <v>32</v>
+      </c>
       <c r="K14">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M14" t="s">
         <v>27</v>
@@ -1549,16 +1498,16 @@
         <v>1333</v>
       </c>
       <c r="O14">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P14">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Q14">
-        <v>6.6</v>
+        <v>5.2</v>
       </c>
       <c r="R14">
-        <v>13.6</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
@@ -1569,28 +1518,28 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="H15" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
       <c r="K15">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L15">
         <v>2</v>
@@ -1599,33 +1548,33 @@
         <v>27</v>
       </c>
       <c r="N15">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O15">
-        <v>2.7</v>
+        <v>1.7</v>
       </c>
       <c r="P15">
-        <v>5.0999999999999996</v>
+        <v>3.2</v>
       </c>
       <c r="Q15">
-        <v>10.8</v>
+        <v>6.6</v>
       </c>
       <c r="R15">
-        <v>21.5</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1634,22 +1583,19 @@
         <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="H16" s="3">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
-        <v>12</v>
-      </c>
       <c r="K16">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" t="s">
         <v>27</v>
@@ -1658,83 +1604,86 @@
         <v>1600</v>
       </c>
       <c r="O16">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="P16">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q16">
-        <v>12.3</v>
+        <v>10.8</v>
       </c>
       <c r="R16">
-        <v>23.9</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D17">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>2.2000000000000002</v>
+        <v>1.6</v>
       </c>
       <c r="H17" s="3">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
       <c r="K17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N17">
         <v>1600</v>
       </c>
       <c r="O17">
-        <v>3.56</v>
+        <v>2.9</v>
       </c>
       <c r="P17">
-        <v>8.07</v>
+        <v>6.4</v>
       </c>
       <c r="Q17">
-        <v>15.55</v>
+        <v>12.3</v>
       </c>
       <c r="R17">
-        <v>34.93</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D18">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -1743,90 +1692,87 @@
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H18" s="3">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
       </c>
       <c r="K18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L18">
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="N18">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O18">
-        <v>3.8</v>
+        <v>3.56</v>
       </c>
       <c r="P18">
-        <v>7.8</v>
+        <v>8.07</v>
       </c>
       <c r="Q18">
-        <v>15.9</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>39</v>
+        <v>15.55</v>
+      </c>
+      <c r="R18">
+        <v>34.93</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="1">
-        <v>3.5</v>
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>34</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H19" s="3">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>48</v>
-      </c>
-      <c r="J19" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M19" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N19">
-        <v>1866</v>
+        <v>667</v>
       </c>
       <c r="O19">
-        <v>8.3000000000000007</v>
+        <v>3.8</v>
       </c>
       <c r="P19">
-        <v>16.100000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="Q19">
-        <v>33.799999999999997</v>
+        <v>15.9</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>39</v>
@@ -1834,52 +1780,55 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3.5</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H20" s="3">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N20">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O20">
-        <v>10.45</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P20">
-        <v>23.55</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>39</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q20">
+        <v>33.799999999999997</v>
       </c>
       <c r="R20" s="1" t="s">
         <v>39</v>
@@ -1914,7 +1863,7 @@
         <v>41</v>
       </c>
       <c r="K21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -1926,13 +1875,13 @@
         <v>1333</v>
       </c>
       <c r="O21">
-        <v>11.8</v>
+        <v>10.45</v>
       </c>
       <c r="P21">
-        <v>23.2</v>
-      </c>
-      <c r="Q21">
-        <v>62</v>
+        <v>23.55</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>39</v>
@@ -1946,31 +1895,28 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H22" s="3">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K22">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -1979,40 +1925,96 @@
         <v>27</v>
       </c>
       <c r="N22">
+        <v>1333</v>
+      </c>
+      <c r="O22">
+        <v>11.8</v>
+      </c>
+      <c r="P22">
+        <v>23.2</v>
+      </c>
+      <c r="Q22">
+        <v>62</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23">
+        <v>8</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23">
         <v>1600</v>
       </c>
-      <c r="O22">
+      <c r="O23">
         <v>13.1</v>
       </c>
-      <c r="P22">
+      <c r="P23">
         <v>27.2</v>
       </c>
-      <c r="Q22">
+      <c r="Q23">
         <v>56.8</v>
       </c>
-      <c r="R22">
+      <c r="R23">
         <v>117.2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:B1048575">
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1048575">
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>"x86-32"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:R1048575">
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"OOM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2073,15 +2075,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575 L2:L1048575">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048575">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"DDR4"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"DDR2"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add emulated x64 benchmark results for Qualcomm Snapdragon 835
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62ED8AD-B1CE-468B-ABA4-A7A262C08F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0A3F6C-8809-4FFD-95E4-367DD076556F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="54">
   <si>
     <t>Cores</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Opteron 6180 SE</t>
+  </si>
+  <si>
+    <t>x86-64 (emu)</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:R1048575" totalsRowShown="0">
   <autoFilter ref="A1:R1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState ref="A2:R23">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R24">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="18">
@@ -724,11 +727,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1565,69 +1568,72 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D16">
-        <v>25</v>
+        <v>3.5</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H16" s="3">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
       </c>
       <c r="K16">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N16">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O16">
-        <v>2.7</v>
+        <v>2.41</v>
       </c>
       <c r="P16">
-        <v>5.0999999999999996</v>
+        <v>4.97</v>
       </c>
       <c r="Q16">
-        <v>10.8</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R16">
-        <v>21.5</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1636,22 +1642,19 @@
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="H17" s="3">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
       <c r="K17">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" t="s">
         <v>27</v>
@@ -1660,83 +1663,86 @@
         <v>1600</v>
       </c>
       <c r="O17">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="P17">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q17">
-        <v>12.3</v>
+        <v>10.8</v>
       </c>
       <c r="R17">
-        <v>23.9</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D18">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>2.2000000000000002</v>
+        <v>1.6</v>
       </c>
       <c r="H18" s="3">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
       </c>
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
       <c r="K18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N18">
         <v>1600</v>
       </c>
       <c r="O18">
-        <v>3.56</v>
+        <v>2.9</v>
       </c>
       <c r="P18">
-        <v>8.07</v>
+        <v>6.4</v>
       </c>
       <c r="Q18">
-        <v>15.55</v>
+        <v>12.3</v>
       </c>
       <c r="R18">
-        <v>34.93</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D19">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -1745,90 +1751,87 @@
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H19" s="3">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
       </c>
       <c r="K19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L19">
         <v>2</v>
       </c>
       <c r="M19" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="N19">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O19">
-        <v>3.8</v>
+        <v>3.56</v>
       </c>
       <c r="P19">
-        <v>7.8</v>
+        <v>8.07</v>
       </c>
       <c r="Q19">
-        <v>15.9</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>39</v>
+        <v>15.55</v>
+      </c>
+      <c r="R19">
+        <v>34.93</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="1">
-        <v>3.5</v>
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>34</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H20" s="3">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N20">
-        <v>1866</v>
+        <v>667</v>
       </c>
       <c r="O20">
-        <v>8.3000000000000007</v>
+        <v>3.8</v>
       </c>
       <c r="P20">
-        <v>16.100000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="Q20">
-        <v>33.799999999999997</v>
+        <v>15.9</v>
       </c>
       <c r="R20" s="1" t="s">
         <v>39</v>
@@ -1836,52 +1839,55 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3.5</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H21" s="3">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I21" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L21">
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N21">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O21">
-        <v>10.45</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P21">
-        <v>23.55</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>39</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q21">
+        <v>33.799999999999997</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>39</v>
@@ -1916,7 +1922,7 @@
         <v>41</v>
       </c>
       <c r="K22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -1928,13 +1934,13 @@
         <v>1333</v>
       </c>
       <c r="O22">
-        <v>11.8</v>
+        <v>10.45</v>
       </c>
       <c r="P22">
-        <v>23.2</v>
-      </c>
-      <c r="Q22">
-        <v>62</v>
+        <v>23.55</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>39</v>
@@ -1948,31 +1954,28 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H23" s="3">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -1981,18 +1984,74 @@
         <v>27</v>
       </c>
       <c r="N23">
+        <v>1333</v>
+      </c>
+      <c r="O23">
+        <v>11.8</v>
+      </c>
+      <c r="P23">
+        <v>23.2</v>
+      </c>
+      <c r="Q23">
+        <v>62</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H24" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24">
+        <v>8</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24">
         <v>1600</v>
       </c>
-      <c r="O23">
+      <c r="O24">
         <v>13.1</v>
       </c>
-      <c r="P23">
+      <c r="P24">
         <v>27.2</v>
       </c>
-      <c r="Q23">
+      <c r="Q24">
         <v>56.8</v>
       </c>
-      <c r="R23">
+      <c r="R24">
         <v>117.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add results for Xeon Phi 7250 (68c), MCDRAM @ 7200 MHz, HT on/off
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0A3F6C-8809-4FFD-95E4-367DD076556F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB72FD4A-5D54-4EFA-AF74-650CBF9CFC3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="59">
   <si>
     <t>Cores</t>
   </si>
@@ -183,35 +183,28 @@
     <t>Xeon E5-2630 v4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>VM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Intel</t>
-    </r>
-  </si>
-  <si>
     <t>Opteron 6180 SE</t>
   </si>
   <si>
     <t>x86-64 (emu)</t>
+  </si>
+  <si>
+    <t>Xeon Phi 7250</t>
+  </si>
+  <si>
+    <t>MCDRAM</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>HT/SMT disabled</t>
+  </si>
+  <si>
+    <t>limited to 1st group = first 64 HW threads = 16 cores</t>
+  </si>
+  <si>
+    <t>VM on Azure, 2 cores provisioned</t>
   </si>
 </sst>
 </file>
@@ -221,7 +214,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,15 +227,6 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -286,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -304,6 +288,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
@@ -401,12 +386,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:R1048575" totalsRowShown="0">
-  <autoFilter ref="A1:R1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
+  <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R26">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
-  <tableColumns count="18">
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
     <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
@@ -425,6 +410,7 @@
     <tableColumn id="15" xr3:uid="{F47BAEEA-393D-4793-8520-847D6349F6D6}" name=" 27"/>
     <tableColumn id="16" xr3:uid="{C553BC33-B4AA-43F8-AB27-68198CB52E16}" name=" 28"/>
     <tableColumn id="17" xr3:uid="{DD355127-DC45-4F05-94FC-A4E0C5EAC951}" name=" 29"/>
+    <tableColumn id="18" xr3:uid="{5E580592-2D6E-4FF1-8BBC-7D1DE24945D0}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -727,11 +713,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -751,9 +737,10 @@
     <col min="13" max="13" width="9.265625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="42.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
@@ -808,8 +795,11 @@
       <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="S1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -865,7 +855,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -918,7 +908,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -926,52 +916,58 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D4">
-        <v>65</v>
+        <v>280</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="3">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="H4" s="3">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
       </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
       <c r="K4">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M4" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="N4">
-        <v>2366</v>
+        <v>7200</v>
       </c>
       <c r="O4">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P4">
-        <v>1.1000000000000001</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q4">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="R4">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+        <v>3.57</v>
+      </c>
+      <c r="S4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -979,10 +975,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -991,40 +987,40 @@
         <v>2</v>
       </c>
       <c r="G5" s="3">
-        <v>1.6</v>
+        <v>3.6</v>
       </c>
       <c r="H5" s="3">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5" t="s">
         <v>13</v>
       </c>
       <c r="N5">
-        <v>2400</v>
+        <v>2366</v>
       </c>
       <c r="O5">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="P5">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q5">
-        <v>3.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R5">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1032,10 +1028,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1044,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="H6" s="3">
         <v>3.4</v>
@@ -1053,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="K6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -1068,60 +1064,57 @@
         <v>0.8</v>
       </c>
       <c r="P6">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q6">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R6">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="E7">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H7" s="3">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
       <c r="K7">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N7">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O7">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P7">
         <v>1.7</v>
@@ -1130,63 +1123,66 @@
         <v>3.3</v>
       </c>
       <c r="R7">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>125</v>
+        <v>280</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="3">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="H8" s="3">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
       <c r="K8">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="L8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M8" t="s">
         <v>27</v>
       </c>
       <c r="N8">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O8">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="P8">
-        <v>1.95</v>
+        <v>1.7</v>
       </c>
       <c r="Q8">
-        <v>4.09</v>
+        <v>3.3</v>
       </c>
       <c r="R8">
-        <v>8.27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1194,52 +1190,58 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D9">
-        <v>77</v>
+        <v>215</v>
       </c>
       <c r="E9">
+        <v>68</v>
+      </c>
+      <c r="F9" s="2">
         <v>4</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
       <c r="G9" s="3">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="H9" s="3">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
       <c r="K9">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M9" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N9">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O9">
-        <v>1.1000000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="P9">
-        <v>1.7</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q9">
-        <v>3.5</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+        <v>7.92</v>
+      </c>
+      <c r="S9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1247,31 +1249,28 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="D10">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="H10" s="3">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
-      <c r="J10" t="s">
-        <v>12</v>
-      </c>
       <c r="K10">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -1280,349 +1279,349 @@
         <v>27</v>
       </c>
       <c r="N10">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O10">
-        <v>1.1200000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P10">
-        <v>2.17</v>
+        <v>1.95</v>
       </c>
       <c r="Q10">
-        <v>4.16</v>
+        <v>4.09</v>
       </c>
       <c r="R10">
-        <v>8.32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+        <v>8.27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>77</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11">
+        <v>1600</v>
+      </c>
+      <c r="O11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P11">
+        <v>1.7</v>
+      </c>
+      <c r="Q11">
         <v>3.5</v>
       </c>
-      <c r="E11">
+      <c r="R11">
         <v>8</v>
       </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H11" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11">
-        <v>6</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N11">
-        <v>1866</v>
-      </c>
-      <c r="O11">
-        <v>1.26</v>
-      </c>
-      <c r="P11">
-        <v>2.57</v>
-      </c>
-      <c r="Q11">
-        <v>5.16</v>
-      </c>
-      <c r="R11">
-        <v>10.47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="3">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="H12" s="3">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
       <c r="K12">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L12">
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N12">
-        <v>2133</v>
+        <v>1333</v>
       </c>
       <c r="O12">
-        <v>1.5</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P12">
+        <v>2.17</v>
+      </c>
+      <c r="Q12">
+        <v>4.16</v>
+      </c>
+      <c r="R12">
+        <v>8.32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13">
+        <v>1866</v>
+      </c>
+      <c r="O13">
+        <v>1.26</v>
+      </c>
+      <c r="P13">
+        <v>2.57</v>
+      </c>
+      <c r="Q13">
+        <v>5.16</v>
+      </c>
+      <c r="R13">
+        <v>10.47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
         <v>2.9</v>
       </c>
-      <c r="Q12">
-        <v>5.7</v>
-      </c>
-      <c r="R12">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13">
-        <v>51</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="H13" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13">
-        <v>20</v>
-      </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
-      <c r="M13" t="s">
-        <v>13</v>
-      </c>
-      <c r="N13">
-        <v>2800</v>
-      </c>
-      <c r="O13">
-        <v>1.5</v>
-      </c>
-      <c r="P13">
-        <v>2.9</v>
-      </c>
-      <c r="Q13">
-        <v>6.2</v>
-      </c>
-      <c r="R13">
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14">
-        <v>280</v>
-      </c>
-      <c r="E14">
-        <v>32</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1.3</v>
-      </c>
       <c r="H14" s="3">
-        <v>1.3</v>
+        <v>3.5</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
-      <c r="J14" t="s">
-        <v>32</v>
-      </c>
       <c r="K14">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N14">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O14">
         <v>1.5</v>
       </c>
       <c r="P14">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q14">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="R14">
-        <v>10.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="H15" s="3">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
       <c r="K15">
+        <v>20</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15">
+        <v>2800</v>
+      </c>
+      <c r="O15">
+        <v>1.5</v>
+      </c>
+      <c r="P15">
+        <v>2.9</v>
+      </c>
+      <c r="Q15">
+        <v>6.2</v>
+      </c>
+      <c r="R15">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>280</v>
+      </c>
+      <c r="E16">
         <v>32</v>
       </c>
-      <c r="L15">
-        <v>2</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16">
+        <v>64</v>
+      </c>
+      <c r="L16">
+        <v>8</v>
+      </c>
+      <c r="M16" t="s">
         <v>27</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>1333</v>
       </c>
-      <c r="O15">
-        <v>1.7</v>
-      </c>
-      <c r="P15">
-        <v>3.2</v>
-      </c>
-      <c r="Q15">
-        <v>6.6</v>
-      </c>
-      <c r="R15">
-        <v>13.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16">
-        <v>3.5</v>
-      </c>
-      <c r="E16">
-        <v>8</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H16" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I16" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16">
-        <v>6</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>46</v>
-      </c>
-      <c r="N16">
-        <v>1866</v>
-      </c>
       <c r="O16">
-        <v>2.41</v>
+        <v>1.5</v>
       </c>
       <c r="P16">
-        <v>4.97</v>
+        <v>3</v>
       </c>
       <c r="Q16">
-        <v>10.050000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="R16">
-        <v>21.07</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1630,28 +1629,28 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="H17" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
       <c r="K17">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L17">
         <v>2</v>
@@ -1660,131 +1659,131 @@
         <v>27</v>
       </c>
       <c r="N17">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O17">
-        <v>2.7</v>
+        <v>1.7</v>
       </c>
       <c r="P17">
-        <v>5.0999999999999996</v>
+        <v>3.2</v>
       </c>
       <c r="Q17">
-        <v>10.8</v>
+        <v>6.6</v>
       </c>
       <c r="R17">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D18">
+        <v>3.5</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18">
         <v>6</v>
       </c>
-      <c r="E18">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18">
+        <v>1866</v>
+      </c>
+      <c r="O18">
+        <v>2.41</v>
+      </c>
+      <c r="P18">
+        <v>4.97</v>
+      </c>
+      <c r="Q18">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="R18">
+        <v>21.07</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="E19">
         <v>4</v>
       </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="H18" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18">
-        <v>8</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>27</v>
-      </c>
-      <c r="N18">
-        <v>1600</v>
-      </c>
-      <c r="O18">
-        <v>2.9</v>
-      </c>
-      <c r="P18">
-        <v>6.4</v>
-      </c>
-      <c r="Q18">
-        <v>12.3</v>
-      </c>
-      <c r="R18">
-        <v>23.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19">
-        <v>85</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H19" s="3">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
       </c>
       <c r="K19">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L19">
         <v>2</v>
       </c>
       <c r="M19" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N19">
         <v>1600</v>
       </c>
       <c r="O19">
-        <v>3.56</v>
+        <v>2.7</v>
       </c>
       <c r="P19">
-        <v>8.07</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q19">
-        <v>15.55</v>
+        <v>10.8</v>
       </c>
       <c r="R19">
-        <v>34.93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1792,66 +1791,69 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="H20" s="3">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
+      <c r="J20" t="s">
+        <v>12</v>
+      </c>
       <c r="K20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="N20">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O20">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="P20">
-        <v>7.8</v>
+        <v>6.4</v>
       </c>
       <c r="Q20">
-        <v>15.9</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>44</v>
+        <v>12.3</v>
+      </c>
+      <c r="R20">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A21" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="1">
-        <v>3.5</v>
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>85</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -1860,40 +1862,40 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H21" s="3">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="I21" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M21" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="N21">
-        <v>1866</v>
+        <v>1600</v>
       </c>
       <c r="O21">
-        <v>8.3000000000000007</v>
+        <v>3.56</v>
       </c>
       <c r="P21">
-        <v>16.100000000000001</v>
+        <v>8.07</v>
       </c>
       <c r="Q21">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+        <v>15.55</v>
+      </c>
+      <c r="R21">
+        <v>34.93</v>
+      </c>
+      <c r="S21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1901,105 +1903,108 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="H22" s="3">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="N22">
-        <v>1333</v>
+        <v>667</v>
       </c>
       <c r="O22">
-        <v>10.45</v>
+        <v>3.8</v>
       </c>
       <c r="P22">
-        <v>23.55</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>39</v>
+        <v>7.8</v>
+      </c>
+      <c r="Q22">
+        <v>15.9</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.5</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H23" s="3">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I23" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J23" t="s">
+        <v>34</v>
       </c>
       <c r="K23">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L23">
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N23">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O23">
-        <v>11.8</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P23">
-        <v>23.2</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="Q23">
-        <v>62</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -2007,31 +2012,28 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
       </c>
       <c r="G24" s="3">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H24" s="3">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I24" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K24">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -2040,23 +2042,132 @@
         <v>27</v>
       </c>
       <c r="N24">
+        <v>1333</v>
+      </c>
+      <c r="O24">
+        <v>10.45</v>
+      </c>
+      <c r="P24">
+        <v>23.55</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
+        <v>27</v>
+      </c>
+      <c r="N25">
+        <v>1333</v>
+      </c>
+      <c r="O25">
+        <v>11.8</v>
+      </c>
+      <c r="P25">
+        <v>23.2</v>
+      </c>
+      <c r="Q25">
+        <v>62</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26">
+        <v>8</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26">
         <v>1600</v>
       </c>
-      <c r="O24">
+      <c r="O26">
         <v>13.1</v>
       </c>
-      <c r="P24">
+      <c r="P26">
         <v>27.2</v>
       </c>
-      <c r="Q24">
+      <c r="Q26">
         <v>56.8</v>
       </c>
-      <c r="R24">
+      <c r="R26">
         <v>117.2</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B1048575">
     <cfRule type="cellIs" dxfId="10" priority="18" operator="greaterThan">
       <formula>1</formula>

</xml_diff>

<commit_message>
add results for Ryzen 5 1600 AF
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB72FD4A-5D54-4EFA-AF74-650CBF9CFC3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4300020-EE67-4898-802E-0B3066134783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>Cores</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>VM on Azure, 2 cores provisioned</t>
+  </si>
+  <si>
+    <t>Ryzen 5 1600 AF</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S27">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
@@ -713,11 +716,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -910,61 +913,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D4">
-        <v>280</v>
+        <v>65</v>
       </c>
       <c r="E4">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="3">
-        <v>1.4</v>
+        <v>3.2</v>
       </c>
       <c r="H4" s="3">
-        <v>1.5</v>
+        <v>3.46</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K4">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N4">
-        <v>7200</v>
+        <v>3066</v>
       </c>
       <c r="O4">
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="P4">
-        <v>1.1599999999999999</v>
+        <v>1.03</v>
       </c>
       <c r="Q4">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="R4">
-        <v>3.57</v>
-      </c>
-      <c r="S4" t="s">
-        <v>56</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
@@ -975,49 +975,55 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D5">
-        <v>65</v>
+        <v>280</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="3">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="H5" s="3">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
       </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
       <c r="K5">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M5" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="N5">
-        <v>2366</v>
+        <v>7200</v>
       </c>
       <c r="O5">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P5">
-        <v>1.1000000000000001</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q5">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="R5">
-        <v>4.5999999999999996</v>
+        <v>3.57</v>
+      </c>
+      <c r="S5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
@@ -1028,10 +1034,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1040,37 +1046,37 @@
         <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>1.6</v>
+        <v>3.6</v>
       </c>
       <c r="H6" s="3">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" t="s">
         <v>13</v>
       </c>
       <c r="N6">
-        <v>2400</v>
+        <v>2366</v>
       </c>
       <c r="O6">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="P6">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q6">
-        <v>3.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R6">
-        <v>6.5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
@@ -1081,10 +1087,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1093,7 +1099,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="3">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="H7" s="3">
         <v>3.4</v>
@@ -1102,7 +1108,7 @@
         <v>11</v>
       </c>
       <c r="K7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -1117,60 +1123,57 @@
         <v>0.8</v>
       </c>
       <c r="P7">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q7">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R7">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="E8">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H8" s="3">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
       <c r="K8">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N8">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O8">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P8">
         <v>1.7</v>
@@ -1179,151 +1182,154 @@
         <v>3.3</v>
       </c>
       <c r="R8">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D9">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="E9">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="F9" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="H9" s="3">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K9">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L9">
         <v>8</v>
       </c>
       <c r="M9" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N9">
-        <v>7200</v>
+        <v>1333</v>
       </c>
       <c r="O9">
-        <v>1.02</v>
+        <v>0.9</v>
       </c>
       <c r="P9">
-        <v>2.0699999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="Q9">
-        <v>4.8899999999999997</v>
+        <v>3.3</v>
       </c>
       <c r="R9">
-        <v>7.92</v>
-      </c>
-      <c r="S9" t="s">
-        <v>57</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D10">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G10" s="3">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="H10" s="3">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
       <c r="K10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M10" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N10">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O10">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="P10">
-        <v>1.95</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q10">
-        <v>4.09</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R10">
-        <v>8.27</v>
+        <v>7.92</v>
+      </c>
+      <c r="S10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="H11" s="3">
         <v>4</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3.8</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
       <c r="K11">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -1335,51 +1341,48 @@
         <v>1600</v>
       </c>
       <c r="O11">
-        <v>1.1000000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P11">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="Q11">
-        <v>3.5</v>
+        <v>4.09</v>
       </c>
       <c r="R11">
-        <v>8</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="E12">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="3">
-        <v>2.5</v>
+        <v>3.4</v>
       </c>
       <c r="H12" s="3">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
-      <c r="J12" t="s">
-        <v>12</v>
-      </c>
       <c r="K12">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L12">
         <v>2</v>
@@ -1388,128 +1391,131 @@
         <v>27</v>
       </c>
       <c r="N12">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O12">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P12">
-        <v>2.17</v>
+        <v>1.7</v>
       </c>
       <c r="Q12">
-        <v>4.16</v>
+        <v>3.5</v>
       </c>
       <c r="R12">
-        <v>8.32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3.5</v>
+        <v>51</v>
+      </c>
+      <c r="D13">
+        <v>140</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="H13" s="3">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K13">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N13">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O13">
-        <v>1.26</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P13">
-        <v>2.57</v>
+        <v>2.17</v>
       </c>
       <c r="Q13">
-        <v>5.16</v>
+        <v>4.16</v>
       </c>
       <c r="R13">
-        <v>10.47</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.5</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3">
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H14" s="3">
-        <v>3.5</v>
+        <v>2.4</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
       </c>
       <c r="K14">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N14">
-        <v>2133</v>
+        <v>1866</v>
       </c>
       <c r="O14">
-        <v>1.5</v>
+        <v>1.26</v>
       </c>
       <c r="P14">
-        <v>2.9</v>
+        <v>2.57</v>
       </c>
       <c r="Q14">
-        <v>5.7</v>
+        <v>5.16</v>
       </c>
       <c r="R14">
-        <v>10.6</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
@@ -1520,28 +1526,28 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="3">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="H15" s="3">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
       <c r="K15">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L15">
         <v>2</v>
@@ -1550,7 +1556,7 @@
         <v>13</v>
       </c>
       <c r="N15">
-        <v>2800</v>
+        <v>2133</v>
       </c>
       <c r="O15">
         <v>1.5</v>
@@ -1559,66 +1565,63 @@
         <v>2.9</v>
       </c>
       <c r="Q15">
-        <v>6.2</v>
+        <v>5.7</v>
       </c>
       <c r="R15">
-        <v>12.4</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D16">
-        <v>280</v>
+        <v>51</v>
       </c>
       <c r="E16">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="H16" s="3">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
-        <v>32</v>
-      </c>
       <c r="K16">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="L16">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N16">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O16">
         <v>1.5</v>
       </c>
       <c r="P16">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q16">
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="R16">
-        <v>10.9</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
@@ -1626,34 +1629,37 @@
         <v>5</v>
       </c>
       <c r="B17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D17">
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="H17" s="3">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
+      <c r="J17" t="s">
+        <v>32</v>
+      </c>
       <c r="K17">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M17" t="s">
         <v>27</v>
@@ -1662,139 +1668,139 @@
         <v>1333</v>
       </c>
       <c r="O17">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P17">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Q17">
-        <v>6.6</v>
+        <v>5.2</v>
       </c>
       <c r="R17">
-        <v>13.6</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D18">
+        <v>95</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
         <v>3.5</v>
       </c>
-      <c r="E18">
-        <v>8</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="H18" s="3">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="I18" t="s">
-        <v>52</v>
-      </c>
-      <c r="J18" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K18">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N18">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O18">
-        <v>2.41</v>
+        <v>1.7</v>
       </c>
       <c r="P18">
-        <v>4.97</v>
+        <v>3.2</v>
       </c>
       <c r="Q18">
-        <v>10.050000000000001</v>
+        <v>6.6</v>
       </c>
       <c r="R18">
-        <v>21.07</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D19">
-        <v>25</v>
+        <v>3.5</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H19" s="3">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
       </c>
       <c r="K19">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N19">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O19">
-        <v>2.7</v>
+        <v>2.41</v>
       </c>
       <c r="P19">
-        <v>5.0999999999999996</v>
+        <v>4.97</v>
       </c>
       <c r="Q19">
-        <v>10.8</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R19">
-        <v>21.5</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1803,22 +1809,19 @@
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="H20" s="3">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
-      <c r="J20" t="s">
-        <v>12</v>
-      </c>
       <c r="K20">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" t="s">
         <v>27</v>
@@ -1827,86 +1830,86 @@
         <v>1600</v>
       </c>
       <c r="O20">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="P20">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q20">
-        <v>12.3</v>
+        <v>10.8</v>
       </c>
       <c r="R20">
-        <v>23.9</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A21" s="7" t="s">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D21">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>2.2000000000000002</v>
+        <v>1.6</v>
       </c>
       <c r="H21" s="3">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
+      <c r="J21" t="s">
+        <v>12</v>
+      </c>
       <c r="K21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N21">
         <v>1600</v>
       </c>
       <c r="O21">
-        <v>3.56</v>
+        <v>2.9</v>
       </c>
       <c r="P21">
-        <v>8.07</v>
+        <v>6.4</v>
       </c>
       <c r="Q21">
-        <v>15.55</v>
+        <v>12.3</v>
       </c>
       <c r="R21">
-        <v>34.93</v>
-      </c>
-      <c r="S21" t="s">
-        <v>58</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D22">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1915,90 +1918,90 @@
         <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H22" s="3">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
       </c>
       <c r="K22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L22">
         <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="N22">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O22">
-        <v>3.8</v>
+        <v>3.56</v>
       </c>
       <c r="P22">
-        <v>7.8</v>
+        <v>8.07</v>
       </c>
       <c r="Q22">
-        <v>15.9</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>39</v>
+        <v>15.55</v>
+      </c>
+      <c r="R22">
+        <v>34.93</v>
+      </c>
+      <c r="S22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="1">
-        <v>3.5</v>
+        <v>37</v>
+      </c>
+      <c r="D23">
+        <v>34</v>
       </c>
       <c r="E23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H23" s="3">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>48</v>
-      </c>
-      <c r="J23" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N23">
-        <v>1866</v>
+        <v>667</v>
       </c>
       <c r="O23">
-        <v>8.3000000000000007</v>
+        <v>3.8</v>
       </c>
       <c r="P23">
-        <v>16.100000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="Q23">
-        <v>33.799999999999997</v>
+        <v>15.9</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>39</v>
@@ -2006,52 +2009,55 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3.5</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
       </c>
       <c r="G24" s="3">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H24" s="3">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I24" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J24" t="s">
+        <v>34</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L24">
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N24">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O24">
-        <v>10.45</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P24">
-        <v>23.55</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>39</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q24">
+        <v>33.799999999999997</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>39</v>
@@ -2086,7 +2092,7 @@
         <v>41</v>
       </c>
       <c r="K25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -2098,13 +2104,13 @@
         <v>1333</v>
       </c>
       <c r="O25">
-        <v>11.8</v>
+        <v>10.45</v>
       </c>
       <c r="P25">
-        <v>23.2</v>
-      </c>
-      <c r="Q25">
-        <v>62</v>
+        <v>23.55</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="R25" s="1" t="s">
         <v>39</v>
@@ -2118,31 +2124,28 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="3">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H26" s="3">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K26">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -2151,18 +2154,74 @@
         <v>27</v>
       </c>
       <c r="N26">
+        <v>1333</v>
+      </c>
+      <c r="O26">
+        <v>11.8</v>
+      </c>
+      <c r="P26">
+        <v>23.2</v>
+      </c>
+      <c r="Q26">
+        <v>62</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27">
+        <v>8</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>27</v>
+      </c>
+      <c r="N27">
         <v>1600</v>
       </c>
-      <c r="O26">
+      <c r="O27">
         <v>13.1</v>
       </c>
-      <c r="P26">
+      <c r="P27">
         <v>27.2</v>
       </c>
-      <c r="Q26">
+      <c r="Q27">
         <v>56.8</v>
       </c>
-      <c r="R26">
+      <c r="R27">
         <v>117.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add results for Ryzen 9 5900X, Ryzen 7 2700, and some cloud VMs
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4300020-EE67-4898-802E-0B3066134783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98A0422-7C4C-4687-98C8-6FE58AF56A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="65">
   <si>
     <t>Cores</t>
   </si>
@@ -208,6 +208,21 @@
   </si>
   <si>
     <t>Ryzen 5 1600 AF</t>
+  </si>
+  <si>
+    <t>VM on Red Hat, 2 cores provisioned</t>
+  </si>
+  <si>
+    <t>Epyc 7452</t>
+  </si>
+  <si>
+    <t>Ryzen 7 2700</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Ryzen 9 5900X</t>
   </si>
 </sst>
 </file>
@@ -391,7 +406,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S31">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
@@ -716,11 +731,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -810,29 +825,26 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D2">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2">
         <v>2</v>
       </c>
       <c r="G2" s="3">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="H2" s="3">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
       <c r="K2">
         <v>16</v>
       </c>
@@ -843,19 +855,19 @@
         <v>13</v>
       </c>
       <c r="N2">
-        <v>3333</v>
+        <v>3600</v>
       </c>
       <c r="O2">
-        <v>0.46</v>
+        <v>0.24</v>
       </c>
       <c r="P2">
-        <v>0.91</v>
+        <v>0.52</v>
       </c>
       <c r="Q2">
-        <v>1.8</v>
+        <v>0.98</v>
       </c>
       <c r="R2">
-        <v>3.59</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
@@ -866,28 +878,28 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D3">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="3">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="H3" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
       </c>
       <c r="K3">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -896,19 +908,22 @@
         <v>13</v>
       </c>
       <c r="N3">
-        <v>3200</v>
+        <v>2400</v>
       </c>
       <c r="O3">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.76</v>
       </c>
       <c r="Q3">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="R3">
-        <v>3.7</v>
+        <v>3.03</v>
+      </c>
+      <c r="S3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
@@ -919,22 +934,22 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D4">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="3">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="H4" s="3">
-        <v>3.46</v>
+        <v>4</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -943,7 +958,7 @@
         <v>12</v>
       </c>
       <c r="K4">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -952,108 +967,105 @@
         <v>13</v>
       </c>
       <c r="N4">
-        <v>3066</v>
+        <v>3333</v>
       </c>
       <c r="O4">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P4">
-        <v>1.03</v>
+        <v>0.91</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R4">
-        <v>4.05</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D5">
-        <v>280</v>
+        <v>95</v>
       </c>
       <c r="E5">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3">
-        <v>1.4</v>
+        <v>3.8</v>
       </c>
       <c r="H5" s="3">
-        <v>1.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
       </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
       <c r="K5">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N5">
-        <v>7200</v>
+        <v>3200</v>
       </c>
       <c r="O5">
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="P5">
-        <v>1.1599999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="R5">
-        <v>3.57</v>
-      </c>
-      <c r="S5" t="s">
-        <v>56</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <v>65</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2">
         <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="H6" s="3">
-        <v>4.2</v>
+        <v>3.46</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
       </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
       <c r="K6">
         <v>32</v>
       </c>
@@ -1064,19 +1076,19 @@
         <v>13</v>
       </c>
       <c r="N6">
-        <v>2366</v>
+        <v>3066</v>
       </c>
       <c r="O6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="P6">
-        <v>1.1000000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="Q6">
-        <v>2.2999999999999998</v>
+        <v>2</v>
       </c>
       <c r="R6">
-        <v>4.5999999999999996</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
@@ -1087,49 +1099,55 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D7">
-        <v>15</v>
+        <v>280</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="H7" s="3">
-        <v>3.4</v>
+        <v>1.5</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
       <c r="K7">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M7" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="N7">
-        <v>2400</v>
+        <v>7200</v>
       </c>
       <c r="O7">
-        <v>0.8</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P7">
-        <v>1.5</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q7">
-        <v>3.1</v>
+        <v>1.9</v>
       </c>
       <c r="R7">
-        <v>6.5</v>
+        <v>3.57</v>
+      </c>
+      <c r="S7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -1140,10 +1158,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -1152,93 +1170,90 @@
         <v>2</v>
       </c>
       <c r="G8" s="3">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="H8" s="3">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
       <c r="K8">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8" t="s">
         <v>13</v>
       </c>
       <c r="N8">
-        <v>2400</v>
+        <v>2366</v>
       </c>
       <c r="O8">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="P8">
-        <v>1.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q8">
-        <v>3.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R8">
-        <v>6.7</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E9">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="3">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="H9" s="3">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" t="s">
-        <v>12</v>
-      </c>
       <c r="K9">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="L9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N9">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O9">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P9">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q9">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R9">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
@@ -1249,55 +1264,49 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="D10">
-        <v>215</v>
+        <v>45</v>
       </c>
       <c r="E10">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="F10" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G10" s="3">
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="H10" s="3">
-        <v>1.5</v>
+        <v>3.4</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
-      <c r="J10" t="s">
-        <v>34</v>
-      </c>
       <c r="K10">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L10">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N10">
-        <v>7200</v>
+        <v>2400</v>
       </c>
       <c r="O10">
-        <v>1.02</v>
+        <v>0.8</v>
       </c>
       <c r="P10">
-        <v>2.0699999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="Q10">
-        <v>4.8899999999999997</v>
+        <v>3.3</v>
       </c>
       <c r="R10">
-        <v>7.92</v>
-      </c>
-      <c r="S10" t="s">
-        <v>57</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
@@ -1305,52 +1314,55 @@
         <v>5</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D11">
-        <v>125</v>
+        <v>280</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
       </c>
       <c r="G11" s="3">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="H11" s="3">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
       <c r="K11">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M11" t="s">
         <v>27</v>
       </c>
       <c r="N11">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O11">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="P11">
-        <v>1.95</v>
+        <v>1.7</v>
       </c>
       <c r="Q11">
-        <v>4.09</v>
+        <v>3.3</v>
       </c>
       <c r="R11">
-        <v>8.27</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
@@ -1361,49 +1373,55 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D12">
-        <v>77</v>
+        <v>215</v>
       </c>
       <c r="E12">
+        <v>68</v>
+      </c>
+      <c r="F12" s="2">
         <v>4</v>
       </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
       <c r="G12" s="3">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="H12" s="3">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
       <c r="K12">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M12" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N12">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O12">
-        <v>1.1000000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="P12">
-        <v>1.7</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q12">
-        <v>3.5</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R12">
-        <v>8</v>
+        <v>7.92</v>
+      </c>
+      <c r="S12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
@@ -1414,31 +1432,28 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D13">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E13">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="H13" s="3">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
-      <c r="J13" t="s">
-        <v>12</v>
-      </c>
       <c r="K13">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -1447,346 +1462,346 @@
         <v>27</v>
       </c>
       <c r="N13">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O13">
-        <v>1.1200000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P13">
-        <v>2.17</v>
+        <v>1.95</v>
       </c>
       <c r="Q13">
-        <v>4.16</v>
+        <v>4.09</v>
       </c>
       <c r="R13">
-        <v>8.32</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="1">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>77</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14">
+        <v>1600</v>
+      </c>
+      <c r="O14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P14">
+        <v>1.7</v>
+      </c>
+      <c r="Q14">
         <v>3.5</v>
       </c>
-      <c r="E14">
+      <c r="R14">
         <v>8</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H14" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14">
-        <v>6</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14">
-        <v>1866</v>
-      </c>
-      <c r="O14">
-        <v>1.26</v>
-      </c>
-      <c r="P14">
-        <v>2.57</v>
-      </c>
-      <c r="Q14">
-        <v>5.16</v>
-      </c>
-      <c r="R14">
-        <v>10.47</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D15">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="H15" s="3">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
       <c r="K15">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L15">
         <v>2</v>
       </c>
       <c r="M15" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N15">
-        <v>2133</v>
+        <v>1333</v>
       </c>
       <c r="O15">
-        <v>1.5</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P15">
-        <v>2.9</v>
+        <v>2.17</v>
       </c>
       <c r="Q15">
-        <v>5.7</v>
+        <v>4.16</v>
       </c>
       <c r="R15">
-        <v>10.6</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.5</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>2.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H16" s="3">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
       </c>
       <c r="K16">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N16">
-        <v>2800</v>
+        <v>1866</v>
       </c>
       <c r="O16">
-        <v>1.5</v>
+        <v>1.26</v>
       </c>
       <c r="P16">
-        <v>2.9</v>
+        <v>2.57</v>
       </c>
       <c r="Q16">
-        <v>6.2</v>
+        <v>5.16</v>
       </c>
       <c r="R16">
-        <v>12.4</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D17">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E17">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" s="3">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="H17" s="3">
-        <v>1.3</v>
+        <v>3.5</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
-      <c r="J17" t="s">
-        <v>32</v>
-      </c>
       <c r="K17">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N17">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O17">
         <v>1.5</v>
       </c>
       <c r="P17">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q17">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="R17">
-        <v>10.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="H18" s="3">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
       </c>
       <c r="K18">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L18">
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N18">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O18">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P18">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q18">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="R18">
-        <v>13.6</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D19">
-        <v>3.5</v>
+        <v>280</v>
       </c>
       <c r="E19">
+        <v>32</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19">
+        <v>64</v>
+      </c>
+      <c r="L19">
         <v>8</v>
       </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H19" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I19" t="s">
-        <v>52</v>
-      </c>
-      <c r="J19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19">
-        <v>6</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
       <c r="M19" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N19">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O19">
-        <v>2.41</v>
+        <v>1.5</v>
       </c>
       <c r="P19">
-        <v>4.97</v>
+        <v>3</v>
       </c>
       <c r="Q19">
-        <v>10.050000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="R19">
-        <v>21.07</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
@@ -1797,28 +1812,28 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="H20" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
       <c r="K20">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -1827,92 +1842,89 @@
         <v>27</v>
       </c>
       <c r="N20">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O20">
-        <v>2.7</v>
+        <v>1.7</v>
       </c>
       <c r="P20">
-        <v>5.0999999999999996</v>
+        <v>3.2</v>
       </c>
       <c r="Q20">
-        <v>10.8</v>
+        <v>6.6</v>
       </c>
       <c r="R20">
-        <v>21.5</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>1.6</v>
+        <v>2.35</v>
       </c>
       <c r="H21" s="3">
-        <v>2.1</v>
+        <v>3.35</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
-      <c r="J21" t="s">
-        <v>12</v>
-      </c>
       <c r="K21">
         <v>8</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M21" t="s">
-        <v>27</v>
-      </c>
-      <c r="N21">
-        <v>1600</v>
+        <v>13</v>
       </c>
       <c r="O21">
-        <v>2.9</v>
+        <v>2.16</v>
       </c>
       <c r="P21">
-        <v>6.4</v>
+        <v>4.42</v>
       </c>
       <c r="Q21">
-        <v>12.3</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R21">
-        <v>23.9</v>
+        <v>18.75</v>
+      </c>
+      <c r="S21" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A22" s="7" t="s">
-        <v>21</v>
+      <c r="A22" t="s">
+        <v>44</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D22">
-        <v>85</v>
+        <v>3.5</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
@@ -1921,37 +1933,37 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H22" s="3">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
       </c>
       <c r="K22">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N22">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O22">
-        <v>3.56</v>
+        <v>2.41</v>
       </c>
       <c r="P22">
-        <v>8.07</v>
+        <v>4.97</v>
       </c>
       <c r="Q22">
-        <v>15.55</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R22">
-        <v>34.93</v>
-      </c>
-      <c r="S22" t="s">
-        <v>58</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
@@ -1962,10 +1974,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D23">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1974,93 +1986,93 @@
         <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H23" s="3">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
       </c>
       <c r="K23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L23">
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="N23">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O23">
-        <v>3.8</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P23">
-        <v>7.8</v>
+        <v>5.28</v>
       </c>
       <c r="Q23">
-        <v>15.9</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>39</v>
+        <v>10.6</v>
+      </c>
+      <c r="R23">
+        <v>25.18</v>
+      </c>
+      <c r="S23" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="1">
-        <v>3.5</v>
+        <v>35</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
       </c>
       <c r="G24" s="3">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H24" s="3">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K24">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M24" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N24">
-        <v>1866</v>
+        <v>1600</v>
       </c>
       <c r="O24">
-        <v>8.3000000000000007</v>
+        <v>2.7</v>
       </c>
       <c r="P24">
-        <v>16.100000000000001</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q24">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>39</v>
+        <v>10.8</v>
+      </c>
+      <c r="R24">
+        <v>21.5</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
@@ -2071,10 +2083,10 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -2083,16 +2095,19 @@
         <v>1</v>
       </c>
       <c r="G25" s="3">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="H25" s="3">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="I25" t="s">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -2101,72 +2116,75 @@
         <v>27</v>
       </c>
       <c r="N25">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O25">
-        <v>10.45</v>
+        <v>2.9</v>
       </c>
       <c r="P25">
-        <v>23.55</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>39</v>
+        <v>6.4</v>
+      </c>
+      <c r="Q25">
+        <v>12.3</v>
+      </c>
+      <c r="R25">
+        <v>23.9</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="A26" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26">
         <v>4</v>
       </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="I26" t="s">
-        <v>41</v>
-      </c>
-      <c r="K26">
-        <v>2</v>
-      </c>
       <c r="L26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M26" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N26">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O26">
-        <v>11.8</v>
+        <v>3.56</v>
       </c>
       <c r="P26">
-        <v>23.2</v>
+        <v>8.07</v>
       </c>
       <c r="Q26">
-        <v>62</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>39</v>
+        <v>15.55</v>
+      </c>
+      <c r="R26">
+        <v>34.93</v>
+      </c>
+      <c r="S26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
@@ -2177,51 +2195,266 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
       </c>
       <c r="G27" s="3">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="H27" s="3">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27" t="s">
+        <v>38</v>
+      </c>
+      <c r="N27">
+        <v>667</v>
+      </c>
+      <c r="O27">
+        <v>3.8</v>
+      </c>
+      <c r="P27">
+        <v>7.8</v>
+      </c>
+      <c r="Q27">
+        <v>15.9</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H28" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I28" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28">
+        <v>6</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>46</v>
+      </c>
+      <c r="N28">
+        <v>1866</v>
+      </c>
+      <c r="O28">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P28">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q28">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H29" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I29" t="s">
+        <v>41</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29">
+        <v>1333</v>
+      </c>
+      <c r="O29">
+        <v>10.45</v>
+      </c>
+      <c r="P29">
+        <v>23.55</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I30" t="s">
+        <v>41</v>
+      </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30" t="s">
+        <v>27</v>
+      </c>
+      <c r="N30">
+        <v>1333</v>
+      </c>
+      <c r="O30">
+        <v>11.8</v>
+      </c>
+      <c r="P30">
+        <v>23.2</v>
+      </c>
+      <c r="Q30">
+        <v>62</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
         <v>12</v>
       </c>
-      <c r="K27">
+      <c r="K31">
         <v>8</v>
       </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
         <v>27</v>
       </c>
-      <c r="N27">
+      <c r="N31">
         <v>1600</v>
       </c>
-      <c r="O27">
+      <c r="O31">
         <v>13.1</v>
       </c>
-      <c r="P27">
+      <c r="P31">
         <v>27.2</v>
       </c>
-      <c r="Q27">
+      <c r="Q31">
         <v>56.8</v>
       </c>
-      <c r="R27">
+      <c r="R31">
         <v>117.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add results for a couple of ThinkPads
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98A0422-7C4C-4687-98C8-6FE58AF56A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9719BB7-44D4-4AC9-B5CE-3CACAA8DD766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="71">
   <si>
     <t>Cores</t>
   </si>
@@ -223,6 +223,24 @@
   </si>
   <si>
     <t>Ryzen 9 5900X</t>
+  </si>
+  <si>
+    <t>i5-3320M</t>
+  </si>
+  <si>
+    <t>ThinkPad T430s</t>
+  </si>
+  <si>
+    <t>ThinkPad W530</t>
+  </si>
+  <si>
+    <t>i7-3840QM</t>
+  </si>
+  <si>
+    <t>Ryzen 5 PRO 3500U</t>
+  </si>
+  <si>
+    <t>ThinkPad X395</t>
   </si>
 </sst>
 </file>
@@ -406,7 +424,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S34">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
@@ -731,11 +749,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1211,10 +1229,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -1223,51 +1241,54 @@
         <v>2</v>
       </c>
       <c r="G9" s="3">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="H9" s="3">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N9">
-        <v>2400</v>
+        <v>1866</v>
       </c>
       <c r="O9">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="P9">
-        <v>1.5</v>
+        <v>1.32</v>
       </c>
       <c r="Q9">
-        <v>3.1</v>
+        <v>2.68</v>
       </c>
       <c r="R9">
-        <v>6.5</v>
+        <v>5.38</v>
+      </c>
+      <c r="S9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D10">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -1276,19 +1297,19 @@
         <v>2</v>
       </c>
       <c r="G10" s="3">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
       <c r="H10" s="3">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
       <c r="K10">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" t="s">
         <v>13</v>
@@ -1297,72 +1318,72 @@
         <v>2400</v>
       </c>
       <c r="O10">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P10">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="Q10">
-        <v>3.3</v>
+        <v>3.17</v>
       </c>
       <c r="R10">
-        <v>6.7</v>
+        <v>6.53</v>
+      </c>
+      <c r="S10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E11">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="3">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="H11" s="3">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
-      <c r="J11" t="s">
-        <v>12</v>
-      </c>
       <c r="K11">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="L11">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N11">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O11">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P11">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q11">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R11">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
@@ -1373,55 +1394,49 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>215</v>
+        <v>45</v>
       </c>
       <c r="E12">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="F12" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G12" s="3">
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="H12" s="3">
-        <v>1.5</v>
+        <v>3.4</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
-      <c r="J12" t="s">
-        <v>34</v>
-      </c>
       <c r="K12">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N12">
-        <v>7200</v>
+        <v>2400</v>
       </c>
       <c r="O12">
-        <v>1.02</v>
+        <v>0.8</v>
       </c>
       <c r="P12">
-        <v>2.0699999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="Q12">
-        <v>4.8899999999999997</v>
+        <v>3.3</v>
       </c>
       <c r="R12">
-        <v>7.92</v>
-      </c>
-      <c r="S12" t="s">
-        <v>57</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
@@ -1429,52 +1444,55 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>125</v>
+        <v>280</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="H13" s="3">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
       <c r="K13">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M13" t="s">
         <v>27</v>
       </c>
       <c r="N13">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O13">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="P13">
-        <v>1.95</v>
+        <v>1.7</v>
       </c>
       <c r="Q13">
-        <v>4.09</v>
+        <v>3.3</v>
       </c>
       <c r="R13">
-        <v>8.27</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
@@ -1485,49 +1503,55 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D14">
-        <v>77</v>
+        <v>215</v>
       </c>
       <c r="E14">
+        <v>68</v>
+      </c>
+      <c r="F14" s="2">
         <v>4</v>
       </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
       <c r="G14" s="3">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="H14" s="3">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
       <c r="K14">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M14" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N14">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O14">
-        <v>1.1000000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="P14">
-        <v>1.7</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q14">
-        <v>3.5</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R14">
-        <v>8</v>
+        <v>7.92</v>
+      </c>
+      <c r="S14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
@@ -1538,31 +1562,28 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D15">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="H15" s="3">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
-      <c r="J15" t="s">
-        <v>12</v>
-      </c>
       <c r="K15">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L15">
         <v>2</v>
@@ -1571,290 +1592,290 @@
         <v>27</v>
       </c>
       <c r="N15">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O15">
-        <v>1.1200000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P15">
-        <v>2.17</v>
+        <v>1.95</v>
       </c>
       <c r="Q15">
-        <v>4.16</v>
+        <v>4.09</v>
       </c>
       <c r="R15">
-        <v>8.32</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>77</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16">
+        <v>1600</v>
+      </c>
+      <c r="O16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P16">
+        <v>1.7</v>
+      </c>
+      <c r="Q16">
         <v>3.5</v>
       </c>
-      <c r="E16">
+      <c r="R16">
         <v>8</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H16" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16">
-        <v>6</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>46</v>
-      </c>
-      <c r="N16">
-        <v>1866</v>
-      </c>
-      <c r="O16">
-        <v>1.26</v>
-      </c>
-      <c r="P16">
-        <v>2.57</v>
-      </c>
-      <c r="Q16">
-        <v>5.16</v>
-      </c>
-      <c r="R16">
-        <v>10.47</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D17">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="H17" s="3">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
       <c r="K17">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L17">
         <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N17">
-        <v>2133</v>
+        <v>1333</v>
       </c>
       <c r="O17">
-        <v>1.5</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P17">
-        <v>2.9</v>
+        <v>2.17</v>
       </c>
       <c r="Q17">
-        <v>5.7</v>
+        <v>4.16</v>
       </c>
       <c r="R17">
-        <v>10.6</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3.5</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>2.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H18" s="3">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="J18" t="s">
+        <v>34</v>
       </c>
       <c r="K18">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N18">
-        <v>2800</v>
+        <v>1866</v>
       </c>
       <c r="O18">
-        <v>1.5</v>
+        <v>1.26</v>
       </c>
       <c r="P18">
-        <v>2.9</v>
+        <v>2.57</v>
       </c>
       <c r="Q18">
-        <v>6.2</v>
+        <v>5.16</v>
       </c>
       <c r="R18">
-        <v>12.4</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D19">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E19">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="3">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="H19" s="3">
-        <v>1.3</v>
+        <v>3.5</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
       </c>
-      <c r="J19" t="s">
-        <v>32</v>
-      </c>
       <c r="K19">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L19">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M19" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N19">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O19">
         <v>1.5</v>
       </c>
       <c r="P19">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q19">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="R19">
-        <v>10.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="H20" s="3">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
       <c r="K20">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L20">
         <v>2</v>
       </c>
       <c r="M20" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N20">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O20">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P20">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q20">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="R20">
-        <v>13.6</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
@@ -1862,108 +1883,108 @@
         <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="D21">
-        <v>155</v>
+        <v>280</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>2.35</v>
+        <v>1.3</v>
       </c>
       <c r="H21" s="3">
-        <v>3.35</v>
+        <v>1.3</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
+      <c r="J21" t="s">
+        <v>32</v>
+      </c>
       <c r="K21">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="L21">
         <v>8</v>
       </c>
       <c r="M21" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N21">
+        <v>1333</v>
       </c>
       <c r="O21">
-        <v>2.16</v>
+        <v>1.5</v>
       </c>
       <c r="P21">
-        <v>4.42</v>
+        <v>3</v>
       </c>
       <c r="Q21">
-        <v>9.2899999999999991</v>
+        <v>5.2</v>
       </c>
       <c r="R21">
-        <v>18.75</v>
-      </c>
-      <c r="S21" t="s">
-        <v>58</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D22">
+        <v>95</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
         <v>3.5</v>
       </c>
-      <c r="E22">
-        <v>8</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="H22" s="3">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="I22" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K22">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N22">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O22">
-        <v>2.41</v>
+        <v>1.7</v>
       </c>
       <c r="P22">
-        <v>4.97</v>
+        <v>3.2</v>
       </c>
       <c r="Q22">
-        <v>10.050000000000001</v>
+        <v>6.6</v>
       </c>
       <c r="R22">
-        <v>21.07</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
@@ -1974,10 +1995,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D23">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1986,40 +2007,40 @@
         <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="H23" s="3">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
       </c>
       <c r="K23">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L23">
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N23">
         <v>1600</v>
       </c>
       <c r="O23">
-        <v>2.4900000000000002</v>
+        <v>1.76</v>
       </c>
       <c r="P23">
-        <v>5.28</v>
+        <v>3.53</v>
       </c>
       <c r="Q23">
-        <v>10.6</v>
+        <v>7.34</v>
       </c>
       <c r="R23">
-        <v>25.18</v>
+        <v>14.74</v>
       </c>
       <c r="S23" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
@@ -2030,109 +2051,109 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D24">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
       </c>
       <c r="G24" s="3">
-        <v>2</v>
+        <v>2.35</v>
       </c>
       <c r="H24" s="3">
-        <v>2</v>
+        <v>3.35</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
       </c>
       <c r="K24">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M24" t="s">
-        <v>27</v>
-      </c>
-      <c r="N24">
-        <v>1600</v>
+        <v>13</v>
       </c>
       <c r="O24">
-        <v>2.7</v>
+        <v>2.16</v>
       </c>
       <c r="P24">
-        <v>5.0999999999999996</v>
+        <v>4.42</v>
       </c>
       <c r="Q24">
-        <v>10.8</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R24">
-        <v>21.5</v>
+        <v>18.75</v>
+      </c>
+      <c r="S24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D25">
+        <v>3.5</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H25" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25">
         <v>6</v>
       </c>
-      <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="H25" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="I25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J25" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25">
-        <v>8</v>
-      </c>
       <c r="L25">
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N25">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O25">
-        <v>2.9</v>
+        <v>2.41</v>
       </c>
       <c r="P25">
-        <v>6.4</v>
+        <v>4.97</v>
       </c>
       <c r="Q25">
-        <v>12.3</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R25">
-        <v>23.9</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A26" s="7" t="s">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="2">
@@ -2172,36 +2193,36 @@
         <v>1600</v>
       </c>
       <c r="O26">
-        <v>3.56</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P26">
-        <v>8.07</v>
+        <v>5.28</v>
       </c>
       <c r="Q26">
-        <v>15.55</v>
+        <v>10.6</v>
       </c>
       <c r="R26">
-        <v>34.93</v>
+        <v>25.18</v>
       </c>
       <c r="S26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D27">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
@@ -2216,137 +2237,140 @@
         <v>11</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="L27">
         <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="N27">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O27">
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
       <c r="P27">
-        <v>7.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q27">
-        <v>15.9</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>39</v>
+        <v>10.8</v>
+      </c>
+      <c r="R27">
+        <v>21.5</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="1">
-        <v>3.5</v>
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
       </c>
       <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="H28" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28">
         <v>8</v>
       </c>
-      <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3">
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>27</v>
+      </c>
+      <c r="N28">
+        <v>1600</v>
+      </c>
+      <c r="O28">
+        <v>2.9</v>
+      </c>
+      <c r="P28">
+        <v>6.4</v>
+      </c>
+      <c r="Q28">
+        <v>12.3</v>
+      </c>
+      <c r="R28">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29">
+        <v>85</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H28" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I28" t="s">
-        <v>48</v>
-      </c>
-      <c r="J28" t="s">
-        <v>34</v>
-      </c>
-      <c r="K28">
-        <v>6</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-      <c r="M28" t="s">
-        <v>46</v>
-      </c>
-      <c r="N28">
-        <v>1866</v>
-      </c>
-      <c r="O28">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="P28">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="Q28">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="E29">
+      <c r="H29" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29">
         <v>4</v>
       </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="H29" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="I29" t="s">
-        <v>41</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
       <c r="L29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N29">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O29">
-        <v>10.45</v>
+        <v>3.56</v>
       </c>
       <c r="P29">
-        <v>23.55</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>39</v>
+        <v>8.07</v>
+      </c>
+      <c r="Q29">
+        <v>15.55</v>
+      </c>
+      <c r="R29">
+        <v>34.93</v>
+      </c>
+      <c r="S29" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
@@ -2357,46 +2381,46 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F30" s="2">
         <v>1</v>
       </c>
       <c r="G30" s="3">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="H30" s="3">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="K30">
         <v>2</v>
       </c>
       <c r="L30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="N30">
-        <v>1333</v>
+        <v>667</v>
       </c>
       <c r="O30">
-        <v>11.8</v>
+        <v>3.8</v>
       </c>
       <c r="P30">
-        <v>23.2</v>
+        <v>7.8</v>
       </c>
       <c r="Q30">
-        <v>62</v>
+        <v>15.9</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>39</v>
@@ -2404,57 +2428,219 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31">
+        <v>6</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
+        <v>46</v>
+      </c>
+      <c r="N31">
+        <v>1866</v>
+      </c>
+      <c r="O31">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P31">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q31">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H32" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
+        <v>27</v>
+      </c>
+      <c r="N32">
+        <v>1333</v>
+      </c>
+      <c r="O32">
+        <v>10.45</v>
+      </c>
+      <c r="P32">
+        <v>23.55</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I33" t="s">
+        <v>41</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33" t="s">
+        <v>27</v>
+      </c>
+      <c r="N33">
+        <v>1333</v>
+      </c>
+      <c r="O33">
+        <v>11.8</v>
+      </c>
+      <c r="P33">
+        <v>23.2</v>
+      </c>
+      <c r="Q33">
+        <v>62</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>42</v>
       </c>
-      <c r="D31">
+      <c r="D34">
         <v>5</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2">
-        <v>1</v>
-      </c>
-      <c r="G31" s="3">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
         <v>1.4</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H34" s="3">
         <v>1.4</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I34" t="s">
         <v>11</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J34" t="s">
         <v>12</v>
       </c>
-      <c r="K31">
+      <c r="K34">
         <v>8</v>
       </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-      <c r="M31" t="s">
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34" t="s">
         <v>27</v>
       </c>
-      <c r="N31">
+      <c r="N34">
         <v>1600</v>
       </c>
-      <c r="O31">
+      <c r="O34">
         <v>13.1</v>
       </c>
-      <c r="P31">
+      <c r="P34">
         <v>27.2</v>
       </c>
-      <c r="Q31">
+      <c r="Q34">
         <v>56.8</v>
       </c>
-      <c r="R31">
+      <c r="R34">
         <v>117.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add results for Ryzen 7 5800H and AMD A8-3850
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9719BB7-44D4-4AC9-B5CE-3CACAA8DD766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B4B0DC-F292-4589-93A8-F0136F0E012B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="73">
   <si>
     <t>Cores</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>ThinkPad X395</t>
+  </si>
+  <si>
+    <t>Ryzen 7 5800H</t>
+  </si>
+  <si>
+    <t>A8-3850</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S37">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
@@ -749,11 +755,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -896,10 +902,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D3">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -911,11 +917,14 @@
         <v>3.2</v>
       </c>
       <c r="H3" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
       </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
       <c r="K3">
         <v>16</v>
       </c>
@@ -926,22 +935,19 @@
         <v>13</v>
       </c>
       <c r="N3">
-        <v>2400</v>
+        <v>3200</v>
       </c>
       <c r="O3">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="P3">
-        <v>0.76</v>
+        <v>0.63</v>
       </c>
       <c r="Q3">
-        <v>1.5</v>
+        <v>1.24</v>
       </c>
       <c r="R3">
-        <v>3.03</v>
-      </c>
-      <c r="S3" t="s">
-        <v>63</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
@@ -952,10 +958,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="D4">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -964,16 +970,16 @@
         <v>2</v>
       </c>
       <c r="G4" s="3">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="H4" s="3">
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="K4">
         <v>16</v>
@@ -985,19 +991,19 @@
         <v>13</v>
       </c>
       <c r="N4">
-        <v>3333</v>
+        <v>3200</v>
       </c>
       <c r="O4">
-        <v>0.46</v>
+        <v>0.32</v>
       </c>
       <c r="P4">
-        <v>0.91</v>
+        <v>0.66</v>
       </c>
       <c r="Q4">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
       <c r="R4">
-        <v>3.59</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
@@ -1008,28 +1014,28 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D5">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
       </c>
       <c r="G5" s="3">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="H5" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
       </c>
       <c r="K5">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L5">
         <v>2</v>
@@ -1038,19 +1044,22 @@
         <v>13</v>
       </c>
       <c r="N5">
-        <v>3200</v>
+        <v>2400</v>
       </c>
       <c r="O5">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.76</v>
       </c>
       <c r="Q5">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="R5">
-        <v>3.7</v>
+        <v>3.03</v>
+      </c>
+      <c r="S5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
@@ -1061,22 +1070,22 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2">
         <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="H6" s="3">
-        <v>3.46</v>
+        <v>4</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
@@ -1085,7 +1094,7 @@
         <v>12</v>
       </c>
       <c r="K6">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -1094,108 +1103,105 @@
         <v>13</v>
       </c>
       <c r="N6">
-        <v>3066</v>
+        <v>3333</v>
       </c>
       <c r="O6">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P6">
-        <v>1.03</v>
+        <v>0.91</v>
       </c>
       <c r="Q6">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R6">
-        <v>4.05</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D7">
-        <v>280</v>
+        <v>95</v>
       </c>
       <c r="E7">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3">
-        <v>1.4</v>
+        <v>3.8</v>
       </c>
       <c r="H7" s="3">
-        <v>1.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
       <c r="K7">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N7">
-        <v>7200</v>
+        <v>3200</v>
       </c>
       <c r="O7">
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="P7">
-        <v>1.1599999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="R7">
-        <v>3.57</v>
-      </c>
-      <c r="S7" t="s">
-        <v>56</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>65</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
       </c>
       <c r="G8" s="3">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="H8" s="3">
-        <v>4.2</v>
+        <v>3.46</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
       <c r="K8">
         <v>32</v>
       </c>
@@ -1206,19 +1212,19 @@
         <v>13</v>
       </c>
       <c r="N8">
-        <v>2366</v>
+        <v>3066</v>
       </c>
       <c r="O8">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="P8">
-        <v>1.1000000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="Q8">
-        <v>2.2999999999999998</v>
+        <v>2</v>
       </c>
       <c r="R8">
-        <v>4.5999999999999996</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
@@ -1229,66 +1235,69 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>280</v>
+      </c>
+      <c r="E9">
         <v>68</v>
       </c>
-      <c r="D9">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
-        <v>2.8</v>
+        <v>1.4</v>
       </c>
       <c r="H9" s="3">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
       <c r="K9">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M9" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N9">
-        <v>1866</v>
+        <v>7200</v>
       </c>
       <c r="O9">
-        <v>0.65</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P9">
-        <v>1.32</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q9">
-        <v>2.68</v>
+        <v>1.9</v>
       </c>
       <c r="R9">
-        <v>5.38</v>
+        <v>3.57</v>
       </c>
       <c r="S9" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -1297,16 +1306,16 @@
         <v>2</v>
       </c>
       <c r="G10" s="3">
-        <v>2.1</v>
+        <v>3.6</v>
       </c>
       <c r="H10" s="3">
-        <v>3.7</v>
+        <v>4.2</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
       <c r="K10">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -1315,22 +1324,19 @@
         <v>13</v>
       </c>
       <c r="N10">
-        <v>2400</v>
+        <v>2366</v>
       </c>
       <c r="O10">
-        <v>0.74</v>
+        <v>0.6</v>
       </c>
       <c r="P10">
-        <v>1.53</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q10">
-        <v>3.17</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R10">
-        <v>6.53</v>
-      </c>
-      <c r="S10" t="s">
-        <v>70</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
@@ -1341,10 +1347,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -1353,51 +1359,54 @@
         <v>2</v>
       </c>
       <c r="G11" s="3">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
       <c r="H11" s="3">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
       <c r="K11">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N11">
-        <v>2400</v>
+        <v>1866</v>
       </c>
       <c r="O11">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="P11">
-        <v>1.5</v>
+        <v>1.32</v>
       </c>
       <c r="Q11">
-        <v>3.1</v>
+        <v>2.68</v>
       </c>
       <c r="R11">
-        <v>6.5</v>
+        <v>5.38</v>
+      </c>
+      <c r="S11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D12">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1406,19 +1415,19 @@
         <v>2</v>
       </c>
       <c r="G12" s="3">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
       <c r="H12" s="3">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
       <c r="K12">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" t="s">
         <v>13</v>
@@ -1427,72 +1436,72 @@
         <v>2400</v>
       </c>
       <c r="O12">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P12">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="Q12">
-        <v>3.3</v>
+        <v>3.17</v>
       </c>
       <c r="R12">
-        <v>6.7</v>
+        <v>6.53</v>
+      </c>
+      <c r="S12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D13">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E13">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="3">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="H13" s="3">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
-      <c r="J13" t="s">
-        <v>12</v>
-      </c>
       <c r="K13">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="L13">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N13">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O13">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P13">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q13">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R13">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
@@ -1503,55 +1512,49 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="D14">
-        <v>215</v>
+        <v>45</v>
       </c>
       <c r="E14">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="F14" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14" s="3">
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="H14" s="3">
-        <v>1.5</v>
+        <v>3.4</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
-      <c r="J14" t="s">
-        <v>34</v>
-      </c>
       <c r="K14">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L14">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N14">
-        <v>7200</v>
+        <v>2400</v>
       </c>
       <c r="O14">
-        <v>1.02</v>
+        <v>0.8</v>
       </c>
       <c r="P14">
-        <v>2.0699999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="Q14">
-        <v>4.8899999999999997</v>
+        <v>3.3</v>
       </c>
       <c r="R14">
-        <v>7.92</v>
-      </c>
-      <c r="S14" t="s">
-        <v>57</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
@@ -1559,52 +1562,55 @@
         <v>5</v>
       </c>
       <c r="B15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>125</v>
+        <v>280</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="H15" s="3">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
       <c r="K15">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M15" t="s">
         <v>27</v>
       </c>
       <c r="N15">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O15">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="P15">
-        <v>1.95</v>
+        <v>1.7</v>
       </c>
       <c r="Q15">
-        <v>4.09</v>
+        <v>3.3</v>
       </c>
       <c r="R15">
-        <v>8.27</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
@@ -1615,49 +1621,55 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D16">
-        <v>77</v>
+        <v>215</v>
       </c>
       <c r="E16">
+        <v>68</v>
+      </c>
+      <c r="F16" s="2">
         <v>4</v>
       </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
       <c r="G16" s="3">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="H16" s="3">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
       <c r="K16">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M16" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N16">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O16">
-        <v>1.1000000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="P16">
-        <v>1.7</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q16">
-        <v>3.5</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R16">
-        <v>8</v>
+        <v>7.92</v>
+      </c>
+      <c r="S16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
@@ -1668,31 +1680,28 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E17">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="H17" s="3">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
       <c r="K17">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L17">
         <v>2</v>
@@ -1701,181 +1710,184 @@
         <v>27</v>
       </c>
       <c r="N17">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O17">
-        <v>1.1200000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P17">
-        <v>2.17</v>
+        <v>1.95</v>
       </c>
       <c r="Q17">
-        <v>4.16</v>
+        <v>4.09</v>
       </c>
       <c r="R17">
-        <v>8.32</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="1">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>77</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18">
+        <v>1600</v>
+      </c>
+      <c r="O18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P18">
+        <v>1.7</v>
+      </c>
+      <c r="Q18">
         <v>3.5</v>
       </c>
-      <c r="E18">
+      <c r="R18">
         <v>8</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H18" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K18">
-        <v>6</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>46</v>
-      </c>
-      <c r="N18">
-        <v>1866</v>
-      </c>
-      <c r="O18">
-        <v>1.26</v>
-      </c>
-      <c r="P18">
-        <v>2.57</v>
-      </c>
-      <c r="Q18">
-        <v>5.16</v>
-      </c>
-      <c r="R18">
-        <v>10.47</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D19">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="H19" s="3">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
       </c>
+      <c r="J19" t="s">
+        <v>12</v>
+      </c>
       <c r="K19">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L19">
         <v>2</v>
       </c>
       <c r="M19" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N19">
-        <v>2133</v>
+        <v>1333</v>
       </c>
       <c r="O19">
-        <v>1.5</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P19">
-        <v>2.9</v>
+        <v>2.17</v>
       </c>
       <c r="Q19">
-        <v>5.7</v>
+        <v>4.16</v>
       </c>
       <c r="R19">
-        <v>10.6</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3.5</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>2.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H20" s="3">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
       </c>
       <c r="K20">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="L20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N20">
-        <v>2800</v>
+        <v>1866</v>
       </c>
       <c r="O20">
-        <v>1.5</v>
+        <v>1.26</v>
       </c>
       <c r="P20">
-        <v>2.9</v>
+        <v>2.57</v>
       </c>
       <c r="Q20">
-        <v>6.2</v>
+        <v>5.16</v>
       </c>
       <c r="R20">
-        <v>12.4</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
@@ -1883,78 +1895,78 @@
         <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="D21">
-        <v>280</v>
+        <v>100</v>
       </c>
       <c r="E21">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="H21" s="3">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
       <c r="J21" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="K21">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L21">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M21" t="s">
         <v>27</v>
       </c>
       <c r="N21">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O21">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="P21">
-        <v>3</v>
+        <v>2.78</v>
       </c>
       <c r="Q21">
-        <v>5.2</v>
+        <v>5.76</v>
       </c>
       <c r="R21">
-        <v>10.9</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D22">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22" s="3">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="H22" s="3">
         <v>3.5</v>
@@ -1963,28 +1975,28 @@
         <v>11</v>
       </c>
       <c r="K22">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L22">
         <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N22">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O22">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P22">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q22">
-        <v>6.6</v>
+        <v>5.7</v>
       </c>
       <c r="R22">
-        <v>13.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
@@ -1995,10 +2007,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D23">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -2007,40 +2019,37 @@
         <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H23" s="3">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
       </c>
       <c r="K23">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L23">
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N23">
-        <v>1600</v>
+        <v>2800</v>
       </c>
       <c r="O23">
-        <v>1.76</v>
+        <v>1.5</v>
       </c>
       <c r="P23">
-        <v>3.53</v>
+        <v>2.9</v>
       </c>
       <c r="Q23">
-        <v>7.34</v>
+        <v>6.2</v>
       </c>
       <c r="R23">
-        <v>14.74</v>
-      </c>
-      <c r="S23" t="s">
-        <v>66</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
@@ -2048,108 +2057,108 @@
         <v>5</v>
       </c>
       <c r="B24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="D24">
-        <v>155</v>
+        <v>280</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
       </c>
       <c r="G24" s="3">
-        <v>2.35</v>
+        <v>1.3</v>
       </c>
       <c r="H24" s="3">
-        <v>3.35</v>
+        <v>1.3</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
       </c>
+      <c r="J24" t="s">
+        <v>32</v>
+      </c>
       <c r="K24">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="L24">
         <v>8</v>
       </c>
       <c r="M24" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N24">
+        <v>1333</v>
       </c>
       <c r="O24">
-        <v>2.16</v>
+        <v>1.5</v>
       </c>
       <c r="P24">
-        <v>4.42</v>
+        <v>3</v>
       </c>
       <c r="Q24">
-        <v>9.2899999999999991</v>
+        <v>5.2</v>
       </c>
       <c r="R24">
-        <v>18.75</v>
-      </c>
-      <c r="S24" t="s">
-        <v>58</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D25">
+        <v>95</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
         <v>3.5</v>
       </c>
-      <c r="E25">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="H25" s="3">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="I25" t="s">
-        <v>52</v>
-      </c>
-      <c r="J25" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K25">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M25" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N25">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O25">
-        <v>2.41</v>
+        <v>1.7</v>
       </c>
       <c r="P25">
-        <v>4.97</v>
+        <v>3.2</v>
       </c>
       <c r="Q25">
-        <v>10.050000000000001</v>
+        <v>6.6</v>
       </c>
       <c r="R25">
-        <v>21.07</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
@@ -2160,10 +2169,10 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D26">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -2172,40 +2181,40 @@
         <v>1</v>
       </c>
       <c r="G26" s="3">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="H26" s="3">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
       </c>
       <c r="K26">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L26">
         <v>2</v>
       </c>
       <c r="M26" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N26">
         <v>1600</v>
       </c>
       <c r="O26">
-        <v>2.4900000000000002</v>
+        <v>1.76</v>
       </c>
       <c r="P26">
-        <v>5.28</v>
+        <v>3.53</v>
       </c>
       <c r="Q26">
-        <v>10.6</v>
+        <v>7.34</v>
       </c>
       <c r="R26">
-        <v>25.18</v>
+        <v>14.74</v>
       </c>
       <c r="S26" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
@@ -2216,109 +2225,109 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D27">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
       </c>
       <c r="G27" s="3">
-        <v>2</v>
+        <v>2.35</v>
       </c>
       <c r="H27" s="3">
-        <v>2</v>
+        <v>3.35</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
       </c>
       <c r="K27">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L27">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M27" t="s">
-        <v>27</v>
-      </c>
-      <c r="N27">
-        <v>1600</v>
+        <v>13</v>
       </c>
       <c r="O27">
-        <v>2.7</v>
+        <v>2.16</v>
       </c>
       <c r="P27">
-        <v>5.0999999999999996</v>
+        <v>4.42</v>
       </c>
       <c r="Q27">
-        <v>10.8</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R27">
-        <v>21.5</v>
+        <v>18.75</v>
+      </c>
+      <c r="S27" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D28">
+        <v>3.5</v>
+      </c>
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H28" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I28" t="s">
+        <v>52</v>
+      </c>
+      <c r="J28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28">
         <v>6</v>
       </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="H28" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="I28" t="s">
-        <v>11</v>
-      </c>
-      <c r="J28" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28">
-        <v>8</v>
-      </c>
       <c r="L28">
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N28">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O28">
-        <v>2.9</v>
+        <v>2.41</v>
       </c>
       <c r="P28">
-        <v>6.4</v>
+        <v>4.97</v>
       </c>
       <c r="Q28">
-        <v>12.3</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R28">
-        <v>23.9</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A29" s="7" t="s">
+      <c r="A29" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="2">
@@ -2358,36 +2367,36 @@
         <v>1600</v>
       </c>
       <c r="O29">
-        <v>3.56</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P29">
-        <v>8.07</v>
+        <v>5.28</v>
       </c>
       <c r="Q29">
-        <v>15.55</v>
+        <v>10.6</v>
       </c>
       <c r="R29">
-        <v>34.93</v>
+        <v>25.18</v>
       </c>
       <c r="S29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D30">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F30" s="2">
         <v>1</v>
@@ -2402,137 +2411,140 @@
         <v>11</v>
       </c>
       <c r="K30">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="L30">
         <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="N30">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O30">
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
       <c r="P30">
-        <v>7.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q30">
-        <v>15.9</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>39</v>
+        <v>10.8</v>
+      </c>
+      <c r="R30">
+        <v>21.5</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="1">
-        <v>3.5</v>
+        <v>36</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
       </c>
       <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31">
         <v>8</v>
       </c>
-      <c r="F31" s="2">
-        <v>1</v>
-      </c>
-      <c r="G31" s="3">
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31">
+        <v>1600</v>
+      </c>
+      <c r="O31">
+        <v>2.9</v>
+      </c>
+      <c r="P31">
+        <v>6.4</v>
+      </c>
+      <c r="Q31">
+        <v>12.3</v>
+      </c>
+      <c r="R31">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32">
+        <v>85</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H31" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I31" t="s">
-        <v>48</v>
-      </c>
-      <c r="J31" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31">
-        <v>6</v>
-      </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-      <c r="M31" t="s">
-        <v>46</v>
-      </c>
-      <c r="N31">
-        <v>1866</v>
-      </c>
-      <c r="O31">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="P31">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="Q31">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32">
+      <c r="H32" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32">
         <v>4</v>
       </c>
-      <c r="F32" s="2">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="H32" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="I32" t="s">
-        <v>41</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
       <c r="L32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N32">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O32">
-        <v>10.45</v>
+        <v>3.56</v>
       </c>
       <c r="P32">
-        <v>23.55</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>39</v>
+        <v>8.07</v>
+      </c>
+      <c r="Q32">
+        <v>15.55</v>
+      </c>
+      <c r="R32">
+        <v>34.93</v>
+      </c>
+      <c r="S32" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.45">
@@ -2543,46 +2555,46 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F33" s="2">
         <v>1</v>
       </c>
       <c r="G33" s="3">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="H33" s="3">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="K33">
         <v>2</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M33" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="N33">
-        <v>1333</v>
+        <v>667</v>
       </c>
       <c r="O33">
-        <v>11.8</v>
+        <v>3.8</v>
       </c>
       <c r="P33">
-        <v>23.2</v>
+        <v>7.8</v>
       </c>
       <c r="Q33">
-        <v>62</v>
+        <v>15.9</v>
       </c>
       <c r="R33" s="1" t="s">
         <v>39</v>
@@ -2590,57 +2602,219 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H34" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I34" t="s">
+        <v>48</v>
+      </c>
+      <c r="J34" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34">
+        <v>6</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34" t="s">
+        <v>46</v>
+      </c>
+      <c r="N34">
+        <v>1866</v>
+      </c>
+      <c r="O34">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P34">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q34">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I35" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35" t="s">
+        <v>27</v>
+      </c>
+      <c r="N35">
+        <v>1333</v>
+      </c>
+      <c r="O35">
+        <v>10.45</v>
+      </c>
+      <c r="P35">
+        <v>23.55</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H36" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I36" t="s">
+        <v>41</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36" t="s">
+        <v>27</v>
+      </c>
+      <c r="N36">
+        <v>1333</v>
+      </c>
+      <c r="O36">
+        <v>11.8</v>
+      </c>
+      <c r="P36">
+        <v>23.2</v>
+      </c>
+      <c r="Q36">
+        <v>62</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
         <v>42</v>
       </c>
-      <c r="D34">
+      <c r="D37">
         <v>5</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="3">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
         <v>1.4</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H37" s="3">
         <v>1.4</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I37" t="s">
         <v>11</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J37" t="s">
         <v>12</v>
       </c>
-      <c r="K34">
+      <c r="K37">
         <v>8</v>
       </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-      <c r="M34" t="s">
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
         <v>27</v>
       </c>
-      <c r="N34">
+      <c r="N37">
         <v>1600</v>
       </c>
-      <c r="O34">
+      <c r="O37">
         <v>13.1</v>
       </c>
-      <c r="P34">
+      <c r="P37">
         <v>27.2</v>
       </c>
-      <c r="Q34">
+      <c r="Q37">
         <v>56.8</v>
       </c>
-      <c r="R34">
+      <c r="R37">
         <v>117.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add result for Ryzen 5950X with overclocked memory
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B4B0DC-F292-4589-93A8-F0136F0E012B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07BA66-8F11-45ED-B748-A01C632E07AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
   <si>
     <t>Cores</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>A8-3850</t>
+  </si>
+  <si>
+    <t>Ryzen 9 5950X</t>
+  </si>
+  <si>
+    <t>16-17-16-34-52-1T</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S38">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
@@ -755,11 +761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -849,28 +855,31 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>105</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2">
         <v>2</v>
       </c>
       <c r="G2" s="3">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="H2" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
       </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
       <c r="K2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -879,19 +888,22 @@
         <v>13</v>
       </c>
       <c r="N2">
-        <v>3600</v>
+        <v>3761</v>
       </c>
       <c r="O2">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="P2">
-        <v>0.52</v>
+        <v>0.42</v>
       </c>
       <c r="Q2">
-        <v>0.98</v>
+        <v>0.72</v>
       </c>
       <c r="R2">
-        <v>2.13</v>
+        <v>1.38</v>
+      </c>
+      <c r="S2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
@@ -902,29 +914,26 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="3">
-        <v>3.2</v>
+        <v>3.7</v>
       </c>
       <c r="H3" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
       <c r="K3">
         <v>16</v>
       </c>
@@ -935,19 +944,19 @@
         <v>13</v>
       </c>
       <c r="N3">
-        <v>3200</v>
+        <v>3600</v>
       </c>
       <c r="O3">
-        <v>0.31</v>
+        <v>0.24</v>
       </c>
       <c r="P3">
-        <v>0.63</v>
+        <v>0.52</v>
       </c>
       <c r="Q3">
-        <v>1.24</v>
+        <v>0.98</v>
       </c>
       <c r="R3">
-        <v>2.5099999999999998</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
@@ -979,7 +988,7 @@
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="K4">
         <v>16</v>
@@ -994,16 +1003,16 @@
         <v>3200</v>
       </c>
       <c r="O4">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="P4">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="Q4">
-        <v>1.3</v>
+        <v>1.24</v>
       </c>
       <c r="R4">
-        <v>2.67</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
@@ -1014,10 +1023,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D5">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -1029,11 +1038,14 @@
         <v>3.2</v>
       </c>
       <c r="H5" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
       </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
       <c r="K5">
         <v>16</v>
       </c>
@@ -1044,22 +1056,19 @@
         <v>13</v>
       </c>
       <c r="N5">
-        <v>2400</v>
+        <v>3200</v>
       </c>
       <c r="O5">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="P5">
-        <v>0.76</v>
+        <v>0.66</v>
       </c>
       <c r="Q5">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="R5">
-        <v>3.03</v>
-      </c>
-      <c r="S5" t="s">
-        <v>63</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
@@ -1070,10 +1079,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D6">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -1082,17 +1091,14 @@
         <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="H6" s="3">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
       </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
       <c r="K6">
         <v>16</v>
       </c>
@@ -1103,19 +1109,22 @@
         <v>13</v>
       </c>
       <c r="N6">
-        <v>3333</v>
+        <v>2400</v>
       </c>
       <c r="O6">
-        <v>0.46</v>
+        <v>0.36</v>
       </c>
       <c r="P6">
-        <v>0.91</v>
+        <v>0.76</v>
       </c>
       <c r="Q6">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="R6">
-        <v>3.59</v>
+        <v>3.03</v>
+      </c>
+      <c r="S6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
@@ -1126,28 +1135,31 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>95</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2">
         <v>2</v>
       </c>
       <c r="G7" s="3">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="H7" s="3">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
       <c r="K7">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -1156,19 +1168,19 @@
         <v>13</v>
       </c>
       <c r="N7">
-        <v>3200</v>
+        <v>3333</v>
       </c>
       <c r="O7">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="Q7">
         <v>1.8</v>
       </c>
       <c r="R7">
-        <v>3.7</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -1179,10 +1191,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -1191,17 +1203,14 @@
         <v>2</v>
       </c>
       <c r="G8" s="3">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="H8" s="3">
-        <v>3.46</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
       <c r="K8">
         <v>32</v>
       </c>
@@ -1212,78 +1221,75 @@
         <v>13</v>
       </c>
       <c r="N8">
-        <v>3066</v>
+        <v>3200</v>
       </c>
       <c r="O8">
         <v>0.5</v>
       </c>
       <c r="P8">
-        <v>1.03</v>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R8">
-        <v>4.05</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D9">
-        <v>280</v>
+        <v>65</v>
       </c>
       <c r="E9">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="3">
-        <v>1.4</v>
+        <v>3.2</v>
       </c>
       <c r="H9" s="3">
-        <v>1.5</v>
+        <v>3.46</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K9">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N9">
-        <v>7200</v>
+        <v>3066</v>
       </c>
       <c r="O9">
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="P9">
-        <v>1.1599999999999999</v>
+        <v>1.03</v>
       </c>
       <c r="Q9">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="R9">
-        <v>3.57</v>
-      </c>
-      <c r="S9" t="s">
-        <v>56</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
@@ -1294,49 +1300,55 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D10">
-        <v>65</v>
+        <v>280</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="H10" s="3">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
       <c r="K10">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M10" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="N10">
-        <v>2366</v>
+        <v>7200</v>
       </c>
       <c r="O10">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P10">
-        <v>1.1000000000000001</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q10">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="R10">
-        <v>4.5999999999999996</v>
+        <v>3.57</v>
+      </c>
+      <c r="S10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
@@ -1347,10 +1359,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="D11">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -1359,10 +1371,10 @@
         <v>2</v>
       </c>
       <c r="G11" s="3">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="H11" s="3">
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -1374,39 +1386,36 @@
         <v>2</v>
       </c>
       <c r="M11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N11">
-        <v>1866</v>
+        <v>2366</v>
       </c>
       <c r="O11">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="P11">
-        <v>1.32</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q11">
-        <v>2.68</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R11">
-        <v>5.38</v>
-      </c>
-      <c r="S11" t="s">
-        <v>67</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1415,51 +1424,51 @@
         <v>2</v>
       </c>
       <c r="G12" s="3">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="H12" s="3">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
       <c r="K12">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L12">
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N12">
-        <v>2400</v>
+        <v>1866</v>
       </c>
       <c r="O12">
-        <v>0.74</v>
+        <v>0.65</v>
       </c>
       <c r="P12">
-        <v>1.53</v>
+        <v>1.32</v>
       </c>
       <c r="Q12">
-        <v>3.17</v>
+        <v>2.68</v>
       </c>
       <c r="R12">
-        <v>6.53</v>
+        <v>5.38</v>
       </c>
       <c r="S12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>15</v>
@@ -1471,19 +1480,19 @@
         <v>2</v>
       </c>
       <c r="G13" s="3">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="H13" s="3">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
       <c r="K13">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" t="s">
         <v>13</v>
@@ -1492,16 +1501,19 @@
         <v>2400</v>
       </c>
       <c r="O13">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P13">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
       <c r="Q13">
-        <v>3.1</v>
+        <v>3.17</v>
       </c>
       <c r="R13">
-        <v>6.5</v>
+        <v>6.53</v>
+      </c>
+      <c r="S13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
@@ -1512,10 +1524,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1524,7 +1536,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="3">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="H14" s="3">
         <v>3.4</v>
@@ -1533,7 +1545,7 @@
         <v>11</v>
       </c>
       <c r="K14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1548,60 +1560,57 @@
         <v>0.8</v>
       </c>
       <c r="P14">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q14">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R14">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="E15">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="3">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H15" s="3">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
-      <c r="J15" t="s">
-        <v>12</v>
-      </c>
       <c r="K15">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N15">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O15">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P15">
         <v>1.7</v>
@@ -1610,151 +1619,154 @@
         <v>3.3</v>
       </c>
       <c r="R15">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D16">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="E16">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="H16" s="3">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K16">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L16">
         <v>8</v>
       </c>
       <c r="M16" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N16">
-        <v>7200</v>
+        <v>1333</v>
       </c>
       <c r="O16">
-        <v>1.02</v>
+        <v>0.9</v>
       </c>
       <c r="P16">
-        <v>2.0699999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="Q16">
-        <v>4.8899999999999997</v>
+        <v>3.3</v>
       </c>
       <c r="R16">
-        <v>7.92</v>
-      </c>
-      <c r="S16" t="s">
-        <v>57</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D17">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G17" s="3">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="H17" s="3">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
+      <c r="J17" t="s">
+        <v>34</v>
+      </c>
       <c r="K17">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M17" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N17">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O17">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="P17">
-        <v>1.95</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q17">
-        <v>4.09</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R17">
-        <v>8.27</v>
+        <v>7.92</v>
+      </c>
+      <c r="S17" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="H18" s="3">
         <v>4</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="H18" s="3">
-        <v>3.8</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
       </c>
       <c r="K18">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="L18">
         <v>2</v>
@@ -1766,51 +1778,48 @@
         <v>1600</v>
       </c>
       <c r="O18">
-        <v>1.1000000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P18">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="Q18">
-        <v>3.5</v>
+        <v>4.09</v>
       </c>
       <c r="R18">
-        <v>8</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D19">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="E19">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>2.5</v>
+        <v>3.4</v>
       </c>
       <c r="H19" s="3">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
       </c>
-      <c r="J19" t="s">
-        <v>12</v>
-      </c>
       <c r="K19">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L19">
         <v>2</v>
@@ -1819,184 +1828,187 @@
         <v>27</v>
       </c>
       <c r="N19">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O19">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P19">
-        <v>2.17</v>
+        <v>1.7</v>
       </c>
       <c r="Q19">
-        <v>4.16</v>
+        <v>3.5</v>
       </c>
       <c r="R19">
-        <v>8.32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="1">
-        <v>3.5</v>
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <v>140</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="H20" s="3">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="I20" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K20">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N20">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O20">
-        <v>1.26</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P20">
-        <v>2.57</v>
+        <v>2.17</v>
       </c>
       <c r="Q20">
-        <v>5.16</v>
+        <v>4.16</v>
       </c>
       <c r="R20">
-        <v>10.47</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3.5</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H21" s="3">
-        <v>2.9</v>
+        <v>2.4</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="J21" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N21">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O21">
-        <v>1.4</v>
+        <v>1.26</v>
       </c>
       <c r="P21">
-        <v>2.78</v>
+        <v>2.57</v>
       </c>
       <c r="Q21">
-        <v>5.76</v>
+        <v>5.16</v>
       </c>
       <c r="R21">
-        <v>11.56</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="D22">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F22" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
         <v>2.9</v>
       </c>
       <c r="H22" s="3">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
       </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
       <c r="K22">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L22">
         <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N22">
-        <v>2133</v>
+        <v>1600</v>
       </c>
       <c r="O22">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="P22">
-        <v>2.9</v>
+        <v>2.78</v>
       </c>
       <c r="Q22">
-        <v>5.7</v>
+        <v>5.76</v>
       </c>
       <c r="R22">
-        <v>10.6</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
@@ -2007,28 +2019,28 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="F23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="3">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="H23" s="3">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
       </c>
       <c r="K23">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -2037,7 +2049,7 @@
         <v>13</v>
       </c>
       <c r="N23">
-        <v>2800</v>
+        <v>2133</v>
       </c>
       <c r="O23">
         <v>1.5</v>
@@ -2046,66 +2058,63 @@
         <v>2.9</v>
       </c>
       <c r="Q23">
-        <v>6.2</v>
+        <v>5.7</v>
       </c>
       <c r="R23">
-        <v>12.4</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D24">
-        <v>280</v>
+        <v>51</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
       </c>
       <c r="G24" s="3">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="H24" s="3">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
       </c>
-      <c r="J24" t="s">
-        <v>32</v>
-      </c>
       <c r="K24">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="L24">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M24" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N24">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O24">
         <v>1.5</v>
       </c>
       <c r="P24">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q24">
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="R24">
-        <v>10.9</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
@@ -2113,34 +2122,37 @@
         <v>5</v>
       </c>
       <c r="B25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D25">
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
       </c>
       <c r="G25" s="3">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="H25" s="3">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
       </c>
+      <c r="J25" t="s">
+        <v>32</v>
+      </c>
       <c r="K25">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M25" t="s">
         <v>27</v>
@@ -2149,48 +2161,48 @@
         <v>1333</v>
       </c>
       <c r="O25">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P25">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Q25">
-        <v>6.6</v>
+        <v>5.2</v>
       </c>
       <c r="R25">
-        <v>13.6</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D26">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="3">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
       <c r="H26" s="3">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
       </c>
       <c r="K26">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L26">
         <v>2</v>
@@ -2199,36 +2211,33 @@
         <v>27</v>
       </c>
       <c r="N26">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O26">
-        <v>1.76</v>
+        <v>1.7</v>
       </c>
       <c r="P26">
-        <v>3.53</v>
+        <v>3.2</v>
       </c>
       <c r="Q26">
-        <v>7.34</v>
+        <v>6.6</v>
       </c>
       <c r="R26">
-        <v>14.74</v>
-      </c>
-      <c r="S26" t="s">
-        <v>66</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D27">
-        <v>155</v>
+        <v>35</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -2237,110 +2246,110 @@
         <v>1</v>
       </c>
       <c r="G27" s="3">
-        <v>2.35</v>
+        <v>2.6</v>
       </c>
       <c r="H27" s="3">
-        <v>3.35</v>
+        <v>3.3</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
       </c>
       <c r="K27">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L27">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N27">
+        <v>1600</v>
       </c>
       <c r="O27">
-        <v>2.16</v>
+        <v>1.76</v>
       </c>
       <c r="P27">
-        <v>4.42</v>
+        <v>3.53</v>
       </c>
       <c r="Q27">
-        <v>9.2899999999999991</v>
+        <v>7.34</v>
       </c>
       <c r="R27">
-        <v>18.75</v>
+        <v>14.74</v>
       </c>
       <c r="S27" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D28">
-        <v>3.5</v>
+        <v>155</v>
       </c>
       <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2.35</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3.35</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28">
         <v>8</v>
       </c>
-      <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H28" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I28" t="s">
-        <v>52</v>
-      </c>
-      <c r="J28" t="s">
-        <v>34</v>
-      </c>
-      <c r="K28">
-        <v>6</v>
-      </c>
       <c r="L28">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M28" t="s">
-        <v>46</v>
-      </c>
-      <c r="N28">
-        <v>1866</v>
+        <v>13</v>
       </c>
       <c r="O28">
-        <v>2.41</v>
+        <v>2.16</v>
       </c>
       <c r="P28">
-        <v>4.97</v>
+        <v>4.42</v>
       </c>
       <c r="Q28">
-        <v>10.050000000000001</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R28">
-        <v>21.07</v>
+        <v>18.75</v>
+      </c>
+      <c r="S28" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D29">
-        <v>85</v>
+        <v>3.5</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F29" s="2">
         <v>1</v>
@@ -2349,104 +2358,107 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H29" s="3">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="I29" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="J29" t="s">
+        <v>34</v>
       </c>
       <c r="K29">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N29">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O29">
-        <v>2.4900000000000002</v>
+        <v>2.41</v>
       </c>
       <c r="P29">
-        <v>5.28</v>
+        <v>4.97</v>
       </c>
       <c r="Q29">
-        <v>10.6</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R29">
-        <v>25.18</v>
-      </c>
-      <c r="S29" t="s">
-        <v>60</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D30">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F30" s="2">
         <v>1</v>
       </c>
       <c r="G30" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H30" s="3">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
       </c>
       <c r="K30">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L30">
         <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N30">
         <v>1600</v>
       </c>
       <c r="O30">
-        <v>2.7</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P30">
-        <v>5.0999999999999996</v>
+        <v>5.28</v>
       </c>
       <c r="Q30">
-        <v>10.8</v>
+        <v>10.6</v>
       </c>
       <c r="R30">
-        <v>21.5</v>
+        <v>25.18</v>
+      </c>
+      <c r="S30" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -2455,22 +2467,19 @@
         <v>1</v>
       </c>
       <c r="G31" s="3">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="H31" s="3">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
-      <c r="J31" t="s">
-        <v>12</v>
-      </c>
       <c r="K31">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M31" t="s">
         <v>27</v>
@@ -2479,86 +2488,86 @@
         <v>1600</v>
       </c>
       <c r="O31">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="P31">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q31">
-        <v>12.3</v>
+        <v>10.8</v>
       </c>
       <c r="R31">
-        <v>23.9</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A32" s="7" t="s">
+      <c r="A32" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D32">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F32" s="2">
         <v>1</v>
       </c>
       <c r="G32" s="3">
-        <v>2.2000000000000002</v>
+        <v>1.6</v>
       </c>
       <c r="H32" s="3">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="I32" t="s">
         <v>11</v>
       </c>
+      <c r="J32" t="s">
+        <v>12</v>
+      </c>
       <c r="K32">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N32">
         <v>1600</v>
       </c>
       <c r="O32">
-        <v>3.56</v>
+        <v>2.9</v>
       </c>
       <c r="P32">
-        <v>8.07</v>
+        <v>6.4</v>
       </c>
       <c r="Q32">
-        <v>15.55</v>
+        <v>12.3</v>
       </c>
       <c r="R32">
-        <v>34.93</v>
-      </c>
-      <c r="S32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A33" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="2">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D33">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -2567,149 +2576,152 @@
         <v>1</v>
       </c>
       <c r="G33" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H33" s="3">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
       </c>
       <c r="K33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L33">
         <v>2</v>
       </c>
       <c r="M33" t="s">
+        <v>13</v>
+      </c>
+      <c r="N33">
+        <v>1600</v>
+      </c>
+      <c r="O33">
+        <v>3.56</v>
+      </c>
+      <c r="P33">
+        <v>8.07</v>
+      </c>
+      <c r="Q33">
+        <v>15.55</v>
+      </c>
+      <c r="R33">
+        <v>34.93</v>
+      </c>
+      <c r="S33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34">
+        <v>34</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2</v>
+      </c>
+      <c r="H34" s="3">
+        <v>2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+      <c r="L34">
+        <v>2</v>
+      </c>
+      <c r="M34" t="s">
         <v>38</v>
       </c>
-      <c r="N33">
+      <c r="N34">
         <v>667</v>
       </c>
-      <c r="O33">
+      <c r="O34">
         <v>3.8</v>
       </c>
-      <c r="P33">
+      <c r="P34">
         <v>7.8</v>
       </c>
-      <c r="Q33">
+      <c r="Q34">
         <v>15.9</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="E34">
-        <v>8</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H34" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I34" t="s">
-        <v>48</v>
-      </c>
-      <c r="J34" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34">
-        <v>6</v>
-      </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-      <c r="M34" t="s">
-        <v>46</v>
-      </c>
-      <c r="N34">
-        <v>1866</v>
-      </c>
-      <c r="O34">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="P34">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="Q34">
-        <v>33.799999999999997</v>
       </c>
       <c r="R34" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3.5</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
       </c>
       <c r="G35" s="3">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H35" s="3">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I35" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J35" t="s">
+        <v>34</v>
       </c>
       <c r="K35">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L35">
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N35">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O35">
-        <v>10.45</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P35">
-        <v>23.55</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>39</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q35">
+        <v>33.799999999999997</v>
       </c>
       <c r="R35" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -2738,7 +2750,7 @@
         <v>41</v>
       </c>
       <c r="K36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L36">
         <v>1</v>
@@ -2750,19 +2762,19 @@
         <v>1333</v>
       </c>
       <c r="O36">
-        <v>11.8</v>
+        <v>10.45</v>
       </c>
       <c r="P36">
-        <v>23.2</v>
-      </c>
-      <c r="Q36">
-        <v>62</v>
+        <v>23.55</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="R36" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -2770,31 +2782,28 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
       </c>
       <c r="G37" s="3">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H37" s="3">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I37" t="s">
-        <v>11</v>
-      </c>
-      <c r="J37" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K37">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L37">
         <v>1</v>
@@ -2803,18 +2812,74 @@
         <v>27</v>
       </c>
       <c r="N37">
+        <v>1333</v>
+      </c>
+      <c r="O37">
+        <v>11.8</v>
+      </c>
+      <c r="P37">
+        <v>23.2</v>
+      </c>
+      <c r="Q37">
+        <v>62</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H38" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38">
+        <v>8</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38" t="s">
+        <v>27</v>
+      </c>
+      <c r="N38">
         <v>1600</v>
       </c>
-      <c r="O37">
+      <c r="O38">
         <v>13.1</v>
       </c>
-      <c r="P37">
+      <c r="P38">
         <v>27.2</v>
       </c>
-      <c r="Q37">
+      <c r="Q38">
         <v>56.8</v>
       </c>
-      <c r="R37">
+      <c r="R38">
         <v>117.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added results for quad-channel ThreadRipper 1950X and a couple of older laptops
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07BA66-8F11-45ED-B748-A01C632E07AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D03A94-5526-4B6D-B639-CD8565F8E4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="83">
   <si>
     <t>Cores</t>
   </si>
@@ -252,7 +252,31 @@
     <t>Ryzen 9 5950X</t>
   </si>
   <si>
-    <t>16-17-16-34-52-1T</t>
+    <t>Core2Duo SP9600</t>
+  </si>
+  <si>
+    <t>16-17-16-34-52 1T</t>
+  </si>
+  <si>
+    <t>16-17-17-35 1T</t>
+  </si>
+  <si>
+    <t>Latitude E4300</t>
+  </si>
+  <si>
+    <t>i7-4712MQ</t>
+  </si>
+  <si>
+    <t>Latitude E6440</t>
+  </si>
+  <si>
+    <t>i5-6200U</t>
+  </si>
+  <si>
+    <t>Latitude E5470</t>
+  </si>
+  <si>
+    <t>ThreadRipper 1950X</t>
   </si>
 </sst>
 </file>
@@ -342,20 +366,63 @@
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="25">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -414,6 +481,77 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -436,18 +574,18 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S42">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="21"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -761,11 +899,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -903,7 +1041,7 @@
         <v>1.38</v>
       </c>
       <c r="S2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
@@ -967,52 +1105,52 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D4">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="3">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="H4" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
       <c r="K4">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M4" t="s">
         <v>13</v>
       </c>
       <c r="N4">
-        <v>3200</v>
+        <v>2933</v>
       </c>
       <c r="O4">
-        <v>0.31</v>
+        <v>0.26</v>
       </c>
       <c r="P4">
-        <v>0.63</v>
+        <v>0.51</v>
       </c>
       <c r="Q4">
-        <v>1.24</v>
+        <v>0.97</v>
       </c>
       <c r="R4">
-        <v>2.5099999999999998</v>
+        <v>1.96</v>
+      </c>
+      <c r="S4" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
@@ -1044,7 +1182,7 @@
         <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="K5">
         <v>16</v>
@@ -1059,16 +1197,16 @@
         <v>3200</v>
       </c>
       <c r="O5">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="P5">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="Q5">
-        <v>1.3</v>
+        <v>1.24</v>
       </c>
       <c r="R5">
-        <v>2.67</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
@@ -1079,10 +1217,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D6">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -1094,10 +1232,13 @@
         <v>3.2</v>
       </c>
       <c r="H6" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
       </c>
       <c r="K6">
         <v>16</v>
@@ -1109,22 +1250,19 @@
         <v>13</v>
       </c>
       <c r="N6">
-        <v>2400</v>
+        <v>3200</v>
       </c>
       <c r="O6">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="P6">
-        <v>0.76</v>
+        <v>0.66</v>
       </c>
       <c r="Q6">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="R6">
-        <v>3.03</v>
-      </c>
-      <c r="S6" t="s">
-        <v>63</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
@@ -1135,10 +1273,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D7">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -1147,16 +1285,13 @@
         <v>2</v>
       </c>
       <c r="G7" s="3">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="H7" s="3">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
       </c>
       <c r="K7">
         <v>16</v>
@@ -1168,19 +1303,22 @@
         <v>13</v>
       </c>
       <c r="N7">
-        <v>3333</v>
+        <v>2400</v>
       </c>
       <c r="O7">
-        <v>0.46</v>
+        <v>0.36</v>
       </c>
       <c r="P7">
-        <v>0.91</v>
+        <v>0.76</v>
       </c>
       <c r="Q7">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="R7">
-        <v>3.59</v>
+        <v>3.03</v>
+      </c>
+      <c r="S7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -1191,28 +1329,31 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>95</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
       </c>
       <c r="G8" s="3">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="H8" s="3">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
       <c r="K8">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L8">
         <v>2</v>
@@ -1221,19 +1362,19 @@
         <v>13</v>
       </c>
       <c r="N8">
-        <v>3200</v>
+        <v>3333</v>
       </c>
       <c r="O8">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P8">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="Q8">
         <v>1.8</v>
       </c>
       <c r="R8">
-        <v>3.7</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
@@ -1244,10 +1385,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D9">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -1256,16 +1397,13 @@
         <v>2</v>
       </c>
       <c r="G9" s="3">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="H9" s="3">
-        <v>3.46</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
       </c>
       <c r="K9">
         <v>32</v>
@@ -1277,78 +1415,75 @@
         <v>13</v>
       </c>
       <c r="N9">
-        <v>3066</v>
+        <v>3200</v>
       </c>
       <c r="O9">
         <v>0.5</v>
       </c>
       <c r="P9">
-        <v>1.03</v>
+        <v>1</v>
       </c>
       <c r="Q9">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R9">
-        <v>4.05</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D10">
-        <v>280</v>
+        <v>65</v>
       </c>
       <c r="E10">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="3">
-        <v>1.4</v>
+        <v>3.2</v>
       </c>
       <c r="H10" s="3">
-        <v>1.5</v>
+        <v>3.46</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K10">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M10" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N10">
-        <v>7200</v>
+        <v>3066</v>
       </c>
       <c r="O10">
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="P10">
-        <v>1.1599999999999999</v>
+        <v>1.03</v>
       </c>
       <c r="Q10">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="R10">
-        <v>3.57</v>
-      </c>
-      <c r="S10" t="s">
-        <v>56</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
@@ -1359,49 +1494,55 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D11">
-        <v>65</v>
+        <v>280</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="3">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="H11" s="3">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
       <c r="K11">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M11" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="N11">
-        <v>2366</v>
+        <v>7200</v>
       </c>
       <c r="O11">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P11">
-        <v>1.1000000000000001</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q11">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="R11">
-        <v>4.5999999999999996</v>
+        <v>3.57</v>
+      </c>
+      <c r="S11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
@@ -1412,10 +1553,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="D12">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1424,10 +1565,10 @@
         <v>2</v>
       </c>
       <c r="G12" s="3">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="H12" s="3">
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
@@ -1439,39 +1580,36 @@
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N12">
-        <v>1866</v>
+        <v>2366</v>
       </c>
       <c r="O12">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="P12">
-        <v>1.32</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q12">
-        <v>2.68</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R12">
-        <v>5.38</v>
-      </c>
-      <c r="S12" t="s">
-        <v>67</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -1480,51 +1618,51 @@
         <v>2</v>
       </c>
       <c r="G13" s="3">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="H13" s="3">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
       <c r="K13">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L13">
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N13">
-        <v>2400</v>
+        <v>1866</v>
       </c>
       <c r="O13">
-        <v>0.74</v>
+        <v>0.65</v>
       </c>
       <c r="P13">
-        <v>1.53</v>
+        <v>1.32</v>
       </c>
       <c r="Q13">
-        <v>3.17</v>
+        <v>2.68</v>
       </c>
       <c r="R13">
-        <v>6.53</v>
+        <v>5.38</v>
       </c>
       <c r="S13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D14">
         <v>15</v>
@@ -1536,19 +1674,19 @@
         <v>2</v>
       </c>
       <c r="G14" s="3">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="H14" s="3">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
       <c r="K14">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" t="s">
         <v>13</v>
@@ -1557,16 +1695,19 @@
         <v>2400</v>
       </c>
       <c r="O14">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P14">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
       <c r="Q14">
-        <v>3.1</v>
+        <v>3.17</v>
       </c>
       <c r="R14">
-        <v>6.5</v>
+        <v>6.53</v>
+      </c>
+      <c r="S14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
@@ -1577,10 +1718,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1589,7 +1730,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="3">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="H15" s="3">
         <v>3.4</v>
@@ -1598,7 +1739,7 @@
         <v>11</v>
       </c>
       <c r="K15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1613,60 +1754,57 @@
         <v>0.8</v>
       </c>
       <c r="P15">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q15">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R15">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="E16">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="3">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H16" s="3">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
-        <v>12</v>
-      </c>
       <c r="K16">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L16">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N16">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O16">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P16">
         <v>1.7</v>
@@ -1675,7 +1813,7 @@
         <v>3.3</v>
       </c>
       <c r="R16">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
@@ -1686,55 +1824,52 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="D17">
-        <v>215</v>
+        <v>37</v>
       </c>
       <c r="E17">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="F17" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G17" s="3">
-        <v>1.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H17" s="3">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
-      </c>
-      <c r="J17" t="s">
-        <v>34</v>
       </c>
       <c r="K17">
         <v>16</v>
       </c>
       <c r="L17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N17">
-        <v>7200</v>
+        <v>1600</v>
       </c>
       <c r="O17">
-        <v>1.02</v>
+        <v>0.81</v>
       </c>
       <c r="P17">
-        <v>2.0699999999999998</v>
+        <v>1.67</v>
       </c>
       <c r="Q17">
-        <v>4.8899999999999997</v>
+        <v>3.45</v>
       </c>
       <c r="R17">
-        <v>7.92</v>
+        <v>6.87</v>
       </c>
       <c r="S17" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
@@ -1742,52 +1877,55 @@
         <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>125</v>
+        <v>280</v>
       </c>
       <c r="E18">
+        <v>32</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18">
+        <v>64</v>
+      </c>
+      <c r="L18">
         <v>8</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="H18" s="3">
-        <v>4</v>
-      </c>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18">
-        <v>24</v>
-      </c>
-      <c r="L18">
-        <v>2</v>
       </c>
       <c r="M18" t="s">
         <v>27</v>
       </c>
       <c r="N18">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O18">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="P18">
-        <v>1.95</v>
+        <v>1.7</v>
       </c>
       <c r="Q18">
-        <v>4.09</v>
+        <v>3.3</v>
       </c>
       <c r="R18">
-        <v>8.27</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
@@ -1798,49 +1936,55 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D19">
-        <v>77</v>
+        <v>215</v>
       </c>
       <c r="E19">
+        <v>68</v>
+      </c>
+      <c r="F19" s="2">
         <v>4</v>
       </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
       <c r="G19" s="3">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="H19" s="3">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
       </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
       <c r="K19">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L19">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M19" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N19">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O19">
-        <v>1.1000000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="P19">
-        <v>1.7</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q19">
-        <v>3.5</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R19">
-        <v>8</v>
+        <v>7.92</v>
+      </c>
+      <c r="S19" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
@@ -1851,31 +1995,28 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D20">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E20">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="H20" s="3">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
-      <c r="J20" t="s">
-        <v>12</v>
-      </c>
       <c r="K20">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -1884,75 +2025,72 @@
         <v>27</v>
       </c>
       <c r="N20">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O20">
-        <v>1.1200000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P20">
-        <v>2.17</v>
+        <v>1.95</v>
       </c>
       <c r="Q20">
-        <v>4.16</v>
+        <v>4.09</v>
       </c>
       <c r="R20">
-        <v>8.32</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="1">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>77</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21">
+        <v>1600</v>
+      </c>
+      <c r="O21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P21">
+        <v>1.7</v>
+      </c>
+      <c r="Q21">
         <v>3.5</v>
       </c>
-      <c r="E21">
+      <c r="R21">
         <v>8</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H21" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I21" t="s">
-        <v>47</v>
-      </c>
-      <c r="J21" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21">
-        <v>6</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21" t="s">
-        <v>46</v>
-      </c>
-      <c r="N21">
-        <v>1866</v>
-      </c>
-      <c r="O21">
-        <v>1.26</v>
-      </c>
-      <c r="P21">
-        <v>2.57</v>
-      </c>
-      <c r="Q21">
-        <v>5.16</v>
-      </c>
-      <c r="R21">
-        <v>10.47</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
@@ -1963,22 +2101,22 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D22">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="H22" s="3">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
@@ -1987,7 +2125,7 @@
         <v>12</v>
       </c>
       <c r="K22">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -1996,72 +2134,75 @@
         <v>27</v>
       </c>
       <c r="N22">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O22">
-        <v>1.4</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P22">
-        <v>2.78</v>
+        <v>2.17</v>
       </c>
       <c r="Q22">
-        <v>5.76</v>
+        <v>4.16</v>
       </c>
       <c r="R22">
-        <v>11.56</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.5</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H23" s="3">
-        <v>3.5</v>
+        <v>2.4</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="J23" t="s">
+        <v>34</v>
       </c>
       <c r="K23">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N23">
-        <v>2133</v>
+        <v>1866</v>
       </c>
       <c r="O23">
-        <v>1.5</v>
+        <v>1.26</v>
       </c>
       <c r="P23">
-        <v>2.9</v>
+        <v>2.57</v>
       </c>
       <c r="Q23">
-        <v>5.7</v>
+        <v>5.16</v>
       </c>
       <c r="R23">
-        <v>10.6</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
@@ -2072,19 +2213,19 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="D24">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24" s="3">
-        <v>2.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H24" s="3">
         <v>2.8</v>
@@ -2093,7 +2234,7 @@
         <v>11</v>
       </c>
       <c r="K24">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L24">
         <v>2</v>
@@ -2102,19 +2243,22 @@
         <v>13</v>
       </c>
       <c r="N24">
-        <v>2800</v>
+        <v>2133</v>
       </c>
       <c r="O24">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="P24">
-        <v>2.9</v>
+        <v>2.95</v>
       </c>
       <c r="Q24">
-        <v>6.2</v>
+        <v>5.64</v>
       </c>
       <c r="R24">
-        <v>12.4</v>
+        <v>11.92</v>
+      </c>
+      <c r="S24" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
@@ -2122,78 +2266,78 @@
         <v>5</v>
       </c>
       <c r="B25" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="D25">
-        <v>280</v>
+        <v>100</v>
       </c>
       <c r="E25">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
       </c>
       <c r="G25" s="3">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="H25" s="3">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
       </c>
       <c r="J25" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="K25">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L25">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M25" t="s">
         <v>27</v>
       </c>
       <c r="N25">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O25">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="P25">
-        <v>3</v>
+        <v>2.78</v>
       </c>
       <c r="Q25">
-        <v>5.2</v>
+        <v>5.76</v>
       </c>
       <c r="R25">
-        <v>10.9</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D26">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="E26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="3">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="H26" s="3">
         <v>3.5</v>
@@ -2202,28 +2346,28 @@
         <v>11</v>
       </c>
       <c r="K26">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L26">
         <v>2</v>
       </c>
       <c r="M26" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N26">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O26">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P26">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q26">
-        <v>6.6</v>
+        <v>5.7</v>
       </c>
       <c r="R26">
-        <v>13.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
@@ -2234,10 +2378,10 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D27">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -2246,40 +2390,37 @@
         <v>1</v>
       </c>
       <c r="G27" s="3">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H27" s="3">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
       </c>
       <c r="K27">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L27">
         <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N27">
-        <v>1600</v>
+        <v>2800</v>
       </c>
       <c r="O27">
-        <v>1.76</v>
+        <v>1.5</v>
       </c>
       <c r="P27">
-        <v>3.53</v>
+        <v>2.9</v>
       </c>
       <c r="Q27">
-        <v>7.34</v>
+        <v>6.2</v>
       </c>
       <c r="R27">
-        <v>14.74</v>
-      </c>
-      <c r="S27" t="s">
-        <v>66</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
@@ -2287,108 +2428,108 @@
         <v>5</v>
       </c>
       <c r="B28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="D28">
-        <v>155</v>
+        <v>280</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F28" s="2">
         <v>1</v>
       </c>
       <c r="G28" s="3">
-        <v>2.35</v>
+        <v>1.3</v>
       </c>
       <c r="H28" s="3">
-        <v>3.35</v>
+        <v>1.3</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
       </c>
+      <c r="J28" t="s">
+        <v>32</v>
+      </c>
       <c r="K28">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="L28">
         <v>8</v>
       </c>
       <c r="M28" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N28">
+        <v>1333</v>
       </c>
       <c r="O28">
-        <v>2.16</v>
+        <v>1.5</v>
       </c>
       <c r="P28">
-        <v>4.42</v>
+        <v>3</v>
       </c>
       <c r="Q28">
-        <v>9.2899999999999991</v>
+        <v>5.2</v>
       </c>
       <c r="R28">
-        <v>18.75</v>
-      </c>
-      <c r="S28" t="s">
-        <v>58</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D29">
+        <v>95</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
         <v>3.5</v>
       </c>
-      <c r="E29">
-        <v>8</v>
-      </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="3">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="H29" s="3">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="I29" t="s">
-        <v>52</v>
-      </c>
-      <c r="J29" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K29">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N29">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O29">
-        <v>2.41</v>
+        <v>1.7</v>
       </c>
       <c r="P29">
-        <v>4.97</v>
+        <v>3.2</v>
       </c>
       <c r="Q29">
-        <v>10.050000000000001</v>
+        <v>6.6</v>
       </c>
       <c r="R29">
-        <v>21.07</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
@@ -2399,10 +2540,10 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D30">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -2411,40 +2552,40 @@
         <v>1</v>
       </c>
       <c r="G30" s="3">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="H30" s="3">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
       </c>
       <c r="K30">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L30">
         <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N30">
         <v>1600</v>
       </c>
       <c r="O30">
-        <v>2.4900000000000002</v>
+        <v>1.76</v>
       </c>
       <c r="P30">
-        <v>5.28</v>
+        <v>3.53</v>
       </c>
       <c r="Q30">
-        <v>10.6</v>
+        <v>7.34</v>
       </c>
       <c r="R30">
-        <v>25.18</v>
+        <v>14.74</v>
       </c>
       <c r="S30" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
@@ -2455,109 +2596,109 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D31">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="E31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F31" s="2">
         <v>1</v>
       </c>
       <c r="G31" s="3">
-        <v>2</v>
+        <v>2.35</v>
       </c>
       <c r="H31" s="3">
-        <v>2</v>
+        <v>3.35</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
       <c r="K31">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M31" t="s">
-        <v>27</v>
-      </c>
-      <c r="N31">
-        <v>1600</v>
+        <v>13</v>
       </c>
       <c r="O31">
-        <v>2.7</v>
+        <v>2.16</v>
       </c>
       <c r="P31">
-        <v>5.0999999999999996</v>
+        <v>4.42</v>
       </c>
       <c r="Q31">
-        <v>10.8</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R31">
-        <v>21.5</v>
+        <v>18.75</v>
+      </c>
+      <c r="S31" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D32">
+        <v>3.5</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H32" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>52</v>
+      </c>
+      <c r="J32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32">
         <v>6</v>
       </c>
-      <c r="E32">
-        <v>4</v>
-      </c>
-      <c r="F32" s="2">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="H32" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32">
-        <v>8</v>
-      </c>
       <c r="L32">
         <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N32">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O32">
-        <v>2.9</v>
+        <v>2.41</v>
       </c>
       <c r="P32">
-        <v>6.4</v>
+        <v>4.97</v>
       </c>
       <c r="Q32">
-        <v>12.3</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R32">
-        <v>23.9</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A33" s="7" t="s">
+      <c r="A33" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="2">
@@ -2597,36 +2738,36 @@
         <v>1600</v>
       </c>
       <c r="O33">
-        <v>3.56</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P33">
-        <v>8.07</v>
+        <v>5.28</v>
       </c>
       <c r="Q33">
-        <v>15.55</v>
+        <v>10.6</v>
       </c>
       <c r="R33">
-        <v>34.93</v>
+        <v>25.18</v>
       </c>
       <c r="S33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D34">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F34" s="2">
         <v>1</v>
@@ -2641,84 +2782,84 @@
         <v>11</v>
       </c>
       <c r="K34">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="L34">
         <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="N34">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O34">
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
       <c r="P34">
-        <v>7.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q34">
-        <v>15.9</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>39</v>
+        <v>10.8</v>
+      </c>
+      <c r="R34">
+        <v>21.5</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="1">
-        <v>3.5</v>
+        <v>36</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
       </c>
       <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="H35" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35">
         <v>8</v>
       </c>
-      <c r="F35" s="2">
-        <v>1</v>
-      </c>
-      <c r="G35" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H35" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I35" t="s">
-        <v>48</v>
-      </c>
-      <c r="J35" t="s">
-        <v>34</v>
-      </c>
-      <c r="K35">
-        <v>6</v>
-      </c>
       <c r="L35">
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N35">
-        <v>1866</v>
+        <v>1600</v>
       </c>
       <c r="O35">
-        <v>8.3000000000000007</v>
+        <v>2.9</v>
       </c>
       <c r="P35">
-        <v>16.100000000000001</v>
+        <v>6.4</v>
       </c>
       <c r="Q35">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>39</v>
+        <v>12.3</v>
+      </c>
+      <c r="R35">
+        <v>23.9</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.45">
@@ -2729,102 +2870,108 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
       </c>
       <c r="G36" s="3">
-        <v>1.3</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="H36" s="3">
-        <v>1.8</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="I36" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="K36">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M36" t="s">
         <v>27</v>
       </c>
       <c r="N36">
-        <v>1333</v>
+        <v>1066</v>
       </c>
       <c r="O36">
-        <v>10.45</v>
+        <v>3.07</v>
       </c>
       <c r="P36">
-        <v>23.55</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>39</v>
+        <v>6.26</v>
+      </c>
+      <c r="Q36">
+        <v>13.37</v>
+      </c>
+      <c r="R36">
+        <v>26.46</v>
+      </c>
+      <c r="S36" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="A37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H37" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37">
         <v>4</v>
       </c>
-      <c r="F37" s="2">
-        <v>1</v>
-      </c>
-      <c r="G37" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="H37" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="I37" t="s">
-        <v>41</v>
-      </c>
-      <c r="K37">
-        <v>2</v>
-      </c>
       <c r="L37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M37" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N37">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O37">
-        <v>11.8</v>
+        <v>3.56</v>
       </c>
       <c r="P37">
-        <v>23.2</v>
+        <v>8.07</v>
       </c>
       <c r="Q37">
-        <v>62</v>
-      </c>
-      <c r="R37" s="1" t="s">
-        <v>39</v>
+        <v>15.55</v>
+      </c>
+      <c r="R37">
+        <v>34.93</v>
+      </c>
+      <c r="S37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.45">
@@ -2835,78 +2982,293 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>34</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3">
+        <v>2</v>
+      </c>
+      <c r="H38" s="3">
+        <v>2</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>2</v>
+      </c>
+      <c r="M38" t="s">
+        <v>38</v>
+      </c>
+      <c r="N38">
+        <v>667</v>
+      </c>
+      <c r="O38">
+        <v>3.8</v>
+      </c>
+      <c r="P38">
+        <v>7.8</v>
+      </c>
+      <c r="Q38">
+        <v>15.9</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H39" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="I39" t="s">
+        <v>48</v>
+      </c>
+      <c r="J39" t="s">
+        <v>34</v>
+      </c>
+      <c r="K39">
+        <v>6</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" t="s">
+        <v>46</v>
+      </c>
+      <c r="N39">
+        <v>1866</v>
+      </c>
+      <c r="O39">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P39">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q39">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I40" t="s">
+        <v>41</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40" t="s">
+        <v>27</v>
+      </c>
+      <c r="N40">
+        <v>1333</v>
+      </c>
+      <c r="O40">
+        <v>10.45</v>
+      </c>
+      <c r="P40">
+        <v>23.55</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="H41" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I41" t="s">
+        <v>41</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41" t="s">
+        <v>27</v>
+      </c>
+      <c r="N41">
+        <v>1333</v>
+      </c>
+      <c r="O41">
+        <v>11.8</v>
+      </c>
+      <c r="P41">
+        <v>23.2</v>
+      </c>
+      <c r="Q41">
+        <v>62</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
         <v>42</v>
       </c>
-      <c r="D38">
+      <c r="D42">
         <v>5</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2">
-        <v>1</v>
-      </c>
-      <c r="G38" s="3">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3">
         <v>1.4</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H42" s="3">
         <v>1.4</v>
       </c>
-      <c r="I38" t="s">
-        <v>11</v>
-      </c>
-      <c r="J38" t="s">
+      <c r="I42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" t="s">
         <v>12</v>
       </c>
-      <c r="K38">
+      <c r="K42">
         <v>8</v>
       </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
-      <c r="M38" t="s">
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42" t="s">
         <v>27</v>
       </c>
-      <c r="N38">
+      <c r="N42">
         <v>1600</v>
       </c>
-      <c r="O38">
+      <c r="O42">
         <v>13.1</v>
       </c>
-      <c r="P38">
+      <c r="P42">
         <v>27.2</v>
       </c>
-      <c r="Q38">
+      <c r="Q42">
         <v>56.8</v>
       </c>
-      <c r="R38">
+      <c r="R42">
         <v>117.2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B1048575">
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1048575">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"x86-32"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:R1048575">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"OOM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K1048575">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2920,7 +3282,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048575">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2934,7 +3296,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048575">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2948,7 +3310,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048575">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2962,20 +3324,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575 L2:L1048575">
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="greaterThan">
-      <formula>1</formula>
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="greaterThan">
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048575">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"DDR4"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"DDR2"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048575">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2989,6 +3351,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048575">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048575">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3000,7 +3374,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048575">
+  <conditionalFormatting sqref="Q1:Q1048575">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3012,7 +3386,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1048575">
+  <conditionalFormatting sqref="R1:R1048575">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3024,15 +3398,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1048575">
+  <conditionalFormatting sqref="L1:L1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
+        <color theme="2"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color theme="9"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add results for Epyc 7232P and 7402, and Atom D2550
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D03A94-5526-4B6D-B639-CD8565F8E4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F8D047-3834-46D4-863E-3D8BDBA16810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="86">
   <si>
     <t>Cores</t>
   </si>
@@ -277,15 +277,21 @@
   </si>
   <si>
     <t>ThreadRipper 1950X</t>
+  </si>
+  <si>
+    <t>Epyc 7232P</t>
+  </si>
+  <si>
+    <t>Epyc 7402</t>
+  </si>
+  <si>
+    <t>Atom D2550</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,79 +356,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="11">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2A6A6"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -481,77 +444,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2A6A6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -574,18 +466,18 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S45">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -899,11 +791,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -914,8 +806,8 @@
     <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.265625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.86328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.265625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.86328125" style="7" customWidth="1"/>
     <col min="9" max="9" width="12.3984375" customWidth="1"/>
     <col min="10" max="10" width="20.1328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
@@ -926,23 +818,23 @@
     <col min="19" max="19" width="42.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="19.5" x14ac:dyDescent="0.6">
+      <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -951,37 +843,37 @@
       <c r="H1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1004,10 +896,10 @@
       <c r="F2" s="2">
         <v>2</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="7">
         <v>3.4</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="7">
         <v>4.9000000000000004</v>
       </c>
       <c r="I2" t="s">
@@ -1063,10 +955,10 @@
       <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="7">
         <v>3.7</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="7">
         <v>4.8</v>
       </c>
       <c r="I3" t="s">
@@ -1116,10 +1008,10 @@
       <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="7">
         <v>3.4</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="7">
         <v>4.2</v>
       </c>
       <c r="I4" t="s">
@@ -1172,10 +1064,10 @@
       <c r="F5" s="2">
         <v>2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="7">
         <v>3.2</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="I5" t="s">
@@ -1228,10 +1120,10 @@
       <c r="F6" s="2">
         <v>2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="7">
         <v>3.2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="I6" t="s">
@@ -1284,10 +1176,10 @@
       <c r="F7" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="7">
         <v>3.2</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="7">
         <v>4.0999999999999996</v>
       </c>
       <c r="I7" t="s">
@@ -1340,10 +1232,10 @@
       <c r="F8" s="2">
         <v>2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="7">
         <v>3.6</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="7">
         <v>4</v>
       </c>
       <c r="I8" t="s">
@@ -1396,10 +1288,10 @@
       <c r="F9" s="2">
         <v>2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="7">
         <v>3.8</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="I9" t="s">
@@ -1449,10 +1341,10 @@
       <c r="F10" s="2">
         <v>2</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="7">
         <v>3.2</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="7">
         <v>3.46</v>
       </c>
       <c r="I10" t="s">
@@ -1505,10 +1397,10 @@
       <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="7">
         <v>1.4</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="7">
         <v>1.5</v>
       </c>
       <c r="I11" t="s">
@@ -1564,10 +1456,10 @@
       <c r="F12" s="2">
         <v>2</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="7">
         <v>3.6</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="7">
         <v>4.2</v>
       </c>
       <c r="I12" t="s">
@@ -1617,10 +1509,10 @@
       <c r="F13" s="2">
         <v>2</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="7">
         <v>2.8</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="7">
         <v>3.8</v>
       </c>
       <c r="I13" t="s">
@@ -1662,119 +1554,116 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="H14" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14">
+        <v>32</v>
+      </c>
+      <c r="L14">
         <v>4</v>
-      </c>
-      <c r="F14" s="2">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="H14" s="3">
-        <v>3.7</v>
-      </c>
-      <c r="I14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14">
-        <v>16</v>
-      </c>
-      <c r="L14">
-        <v>2</v>
       </c>
       <c r="M14" t="s">
         <v>13</v>
       </c>
       <c r="N14">
-        <v>2400</v>
+        <v>2667</v>
       </c>
       <c r="O14">
-        <v>0.74</v>
+        <v>0.66</v>
       </c>
       <c r="P14">
-        <v>1.53</v>
+        <v>1.26</v>
       </c>
       <c r="Q14">
-        <v>3.17</v>
+        <v>2.44</v>
       </c>
       <c r="R14">
-        <v>6.53</v>
-      </c>
-      <c r="S14" t="s">
-        <v>70</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="D15">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2">
         <v>2</v>
       </c>
-      <c r="G15" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="H15" s="3">
-        <v>3.4</v>
+      <c r="G15" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="H15" s="7">
+        <v>3.35</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
       <c r="K15">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M15" t="s">
         <v>13</v>
       </c>
       <c r="N15">
-        <v>2400</v>
+        <v>2667</v>
       </c>
       <c r="O15">
-        <v>0.8</v>
+        <v>0.66</v>
       </c>
       <c r="P15">
-        <v>1.5</v>
+        <v>1.26</v>
       </c>
       <c r="Q15">
-        <v>3.1</v>
+        <v>1.91</v>
       </c>
       <c r="R15">
-        <v>6.5</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D16">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1782,20 +1671,20 @@
       <c r="F16" s="2">
         <v>2</v>
       </c>
-      <c r="G16" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="H16" s="3">
-        <v>3.4</v>
+      <c r="G16" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="H16" s="7">
+        <v>3.7</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
       <c r="K16">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" t="s">
         <v>13</v>
@@ -1804,16 +1693,19 @@
         <v>2400</v>
       </c>
       <c r="O16">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P16">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="Q16">
-        <v>3.3</v>
+        <v>3.17</v>
       </c>
       <c r="R16">
-        <v>6.7</v>
+        <v>6.53</v>
+      </c>
+      <c r="S16" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
@@ -1824,10 +1716,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="D17">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1835,88 +1727,82 @@
       <c r="F17" s="2">
         <v>2</v>
       </c>
-      <c r="G17" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H17" s="3">
-        <v>3.3</v>
+      <c r="G17" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="H17" s="7">
+        <v>3.4</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
       <c r="K17">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N17">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="O17">
-        <v>0.81</v>
+        <v>0.8</v>
       </c>
       <c r="P17">
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="Q17">
-        <v>3.45</v>
+        <v>3.1</v>
       </c>
       <c r="R17">
-        <v>6.87</v>
-      </c>
-      <c r="S17" t="s">
-        <v>79</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="E18">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="H18" s="3">
-        <v>2.9</v>
+        <v>2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="H18" s="7">
+        <v>3.4</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
       </c>
-      <c r="J18" t="s">
-        <v>12</v>
-      </c>
       <c r="K18">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L18">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N18">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O18">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P18">
         <v>1.7</v>
@@ -1925,7 +1811,7 @@
         <v>3.3</v>
       </c>
       <c r="R18">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
@@ -1936,55 +1822,52 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="D19">
-        <v>215</v>
+        <v>37</v>
       </c>
       <c r="E19">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="F19" s="2">
-        <v>4</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1.5</v>
+        <v>2</v>
+      </c>
+      <c r="G19" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H19" s="7">
+        <v>3.3</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
-      </c>
-      <c r="J19" t="s">
-        <v>34</v>
       </c>
       <c r="K19">
         <v>16</v>
       </c>
       <c r="L19">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M19" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N19">
-        <v>7200</v>
+        <v>1600</v>
       </c>
       <c r="O19">
-        <v>1.02</v>
+        <v>0.81</v>
       </c>
       <c r="P19">
-        <v>2.0699999999999998</v>
+        <v>1.67</v>
       </c>
       <c r="Q19">
-        <v>4.8899999999999997</v>
+        <v>3.45</v>
       </c>
       <c r="R19">
-        <v>7.92</v>
+        <v>6.87</v>
       </c>
       <c r="S19" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
@@ -1992,52 +1875,55 @@
         <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>125</v>
+        <v>280</v>
       </c>
       <c r="E20">
+        <v>32</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="H20" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20">
+        <v>64</v>
+      </c>
+      <c r="L20">
         <v>8</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="H20" s="3">
-        <v>4</v>
-      </c>
-      <c r="I20" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20">
-        <v>24</v>
-      </c>
-      <c r="L20">
-        <v>2</v>
       </c>
       <c r="M20" t="s">
         <v>27</v>
       </c>
       <c r="N20">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O20">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="P20">
-        <v>1.95</v>
+        <v>1.7</v>
       </c>
       <c r="Q20">
-        <v>4.09</v>
+        <v>3.3</v>
       </c>
       <c r="R20">
-        <v>8.27</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
@@ -2048,49 +1934,55 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D21">
-        <v>77</v>
+        <v>215</v>
       </c>
       <c r="E21">
+        <v>68</v>
+      </c>
+      <c r="F21" s="2">
         <v>4</v>
       </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="H21" s="3">
-        <v>3.8</v>
+      <c r="G21" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H21" s="7">
+        <v>1.5</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
       <c r="K21">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L21">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M21" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N21">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O21">
-        <v>1.1000000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="P21">
-        <v>1.7</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q21">
-        <v>3.5</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R21">
-        <v>8</v>
+        <v>7.92</v>
+      </c>
+      <c r="S21" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
@@ -2101,31 +1993,28 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D22">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E22">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
       </c>
-      <c r="G22" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H22" s="3">
-        <v>2.5</v>
+      <c r="G22" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="H22" s="7">
+        <v>4</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
       </c>
-      <c r="J22" t="s">
-        <v>12</v>
-      </c>
       <c r="K22">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -2134,187 +2023,184 @@
         <v>27</v>
       </c>
       <c r="N22">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O22">
-        <v>1.1200000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P22">
-        <v>2.17</v>
+        <v>1.95</v>
       </c>
       <c r="Q22">
-        <v>4.16</v>
+        <v>4.09</v>
       </c>
       <c r="R22">
-        <v>8.32</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="1">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>77</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="H23" s="7">
+        <v>3.8</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23">
+        <v>1600</v>
+      </c>
+      <c r="O23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P23">
+        <v>1.7</v>
+      </c>
+      <c r="Q23">
         <v>3.5</v>
       </c>
-      <c r="E23">
+      <c r="R23">
         <v>8</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H23" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="I23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23">
-        <v>6</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23" t="s">
-        <v>46</v>
-      </c>
-      <c r="N23">
-        <v>1866</v>
-      </c>
-      <c r="O23">
-        <v>1.26</v>
-      </c>
-      <c r="P23">
-        <v>2.57</v>
-      </c>
-      <c r="Q23">
-        <v>5.16</v>
-      </c>
-      <c r="R23">
-        <v>10.47</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="D24">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F24" s="2">
-        <v>2</v>
-      </c>
-      <c r="G24" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H24" s="3">
-        <v>2.8</v>
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="H24" s="7">
+        <v>2.5</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
       </c>
+      <c r="J24" t="s">
+        <v>12</v>
+      </c>
       <c r="K24">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L24">
         <v>2</v>
       </c>
       <c r="M24" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N24">
-        <v>2133</v>
+        <v>1333</v>
       </c>
       <c r="O24">
-        <v>1.3</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P24">
-        <v>2.95</v>
+        <v>2.17</v>
       </c>
       <c r="Q24">
-        <v>5.64</v>
+        <v>4.16</v>
       </c>
       <c r="R24">
-        <v>11.92</v>
-      </c>
-      <c r="S24" t="s">
-        <v>81</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3.5</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
       </c>
-      <c r="G25" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="H25" s="3">
-        <v>2.9</v>
+      <c r="G25" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H25" s="7">
+        <v>2.4</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="J25" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N25">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O25">
-        <v>1.4</v>
+        <v>1.26</v>
       </c>
       <c r="P25">
-        <v>2.78</v>
+        <v>2.57</v>
       </c>
       <c r="Q25">
-        <v>5.76</v>
+        <v>5.16</v>
       </c>
       <c r="R25">
-        <v>11.56</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
@@ -2325,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D26">
         <v>15</v>
@@ -2336,11 +2222,11 @@
       <c r="F26" s="2">
         <v>2</v>
       </c>
-      <c r="G26" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="H26" s="3">
-        <v>3.5</v>
+      <c r="G26" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H26" s="7">
+        <v>2.8</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
@@ -2358,234 +2244,237 @@
         <v>2133</v>
       </c>
       <c r="O26">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="P26">
-        <v>2.9</v>
+        <v>2.95</v>
       </c>
       <c r="Q26">
-        <v>5.7</v>
+        <v>5.64</v>
       </c>
       <c r="R26">
-        <v>10.6</v>
+        <v>11.92</v>
+      </c>
+      <c r="S26" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D27">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
       </c>
-      <c r="G27" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="H27" s="3">
-        <v>2.8</v>
+      <c r="G27" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="H27" s="7">
+        <v>2.9</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
       </c>
+      <c r="J27" t="s">
+        <v>12</v>
+      </c>
       <c r="K27">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L27">
         <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N27">
-        <v>2800</v>
+        <v>1600</v>
       </c>
       <c r="O27">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="P27">
-        <v>2.9</v>
+        <v>2.78</v>
       </c>
       <c r="Q27">
-        <v>6.2</v>
+        <v>5.76</v>
       </c>
       <c r="R27">
-        <v>12.4</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B28" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D28">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E28">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="H28" s="3">
-        <v>1.3</v>
+        <v>2</v>
+      </c>
+      <c r="G28" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="H28" s="7">
+        <v>3.5</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
       </c>
-      <c r="J28" t="s">
-        <v>32</v>
-      </c>
       <c r="K28">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L28">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M28" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N28">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O28">
         <v>1.5</v>
       </c>
       <c r="P28">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q28">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="R28">
-        <v>10.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D29">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F29" s="2">
         <v>1</v>
       </c>
-      <c r="G29" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="H29" s="3">
-        <v>3.5</v>
+      <c r="G29" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="H29" s="7">
+        <v>2.8</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
       </c>
       <c r="K29">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L29">
         <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N29">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O29">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P29">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q29">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="R29">
-        <v>13.6</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B30" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="D30">
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F30" s="2">
         <v>1</v>
       </c>
-      <c r="G30" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="H30" s="3">
-        <v>3.3</v>
+      <c r="G30" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="H30" s="7">
+        <v>1.3</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
       </c>
+      <c r="J30" t="s">
+        <v>32</v>
+      </c>
       <c r="K30">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M30" t="s">
         <v>27</v>
       </c>
       <c r="N30">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O30">
-        <v>1.76</v>
+        <v>1.5</v>
       </c>
       <c r="P30">
-        <v>3.53</v>
+        <v>3</v>
       </c>
       <c r="Q30">
-        <v>7.34</v>
+        <v>5.2</v>
       </c>
       <c r="R30">
-        <v>14.74</v>
-      </c>
-      <c r="S30" t="s">
-        <v>66</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
@@ -2596,119 +2485,119 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="D31">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F31" s="2">
         <v>1</v>
       </c>
-      <c r="G31" s="3">
-        <v>2.35</v>
-      </c>
-      <c r="H31" s="3">
-        <v>3.35</v>
+      <c r="G31" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="H31" s="7">
+        <v>3.5</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
       <c r="K31">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L31">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N31">
+        <v>1333</v>
       </c>
       <c r="O31">
-        <v>2.16</v>
+        <v>1.7</v>
       </c>
       <c r="P31">
-        <v>4.42</v>
+        <v>3.2</v>
       </c>
       <c r="Q31">
-        <v>9.2899999999999991</v>
+        <v>6.6</v>
       </c>
       <c r="R31">
-        <v>18.75</v>
-      </c>
-      <c r="S31" t="s">
-        <v>58</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D32">
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="E32">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2">
         <v>1</v>
       </c>
-      <c r="G32" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H32" s="3">
-        <v>2.4</v>
+      <c r="G32" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="H32" s="7">
+        <v>3.3</v>
       </c>
       <c r="I32" t="s">
-        <v>52</v>
-      </c>
-      <c r="J32" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K32">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N32">
-        <v>1866</v>
+        <v>1600</v>
       </c>
       <c r="O32">
-        <v>2.41</v>
+        <v>1.76</v>
       </c>
       <c r="P32">
-        <v>4.97</v>
+        <v>3.53</v>
       </c>
       <c r="Q32">
-        <v>10.050000000000001</v>
+        <v>7.34</v>
       </c>
       <c r="R32">
-        <v>21.07</v>
+        <v>14.74</v>
+      </c>
+      <c r="S32" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B33" s="2">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D33">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -2716,94 +2605,94 @@
       <c r="F33" s="2">
         <v>1</v>
       </c>
-      <c r="G33" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H33" s="3">
-        <v>3.1</v>
+      <c r="G33" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="H33" s="7">
+        <v>3.35</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
       </c>
       <c r="K33">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M33" t="s">
         <v>13</v>
       </c>
-      <c r="N33">
-        <v>1600</v>
-      </c>
       <c r="O33">
-        <v>2.4900000000000002</v>
+        <v>2.16</v>
       </c>
       <c r="P33">
-        <v>5.28</v>
+        <v>4.42</v>
       </c>
       <c r="Q33">
-        <v>10.6</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R33">
-        <v>25.18</v>
+        <v>18.75</v>
       </c>
       <c r="S33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D34">
-        <v>25</v>
+        <v>3.5</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F34" s="2">
         <v>1</v>
       </c>
-      <c r="G34" s="3">
-        <v>2</v>
-      </c>
-      <c r="H34" s="3">
-        <v>2</v>
+      <c r="G34" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H34" s="7">
+        <v>2.4</v>
       </c>
       <c r="I34" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="J34" t="s">
+        <v>34</v>
       </c>
       <c r="K34">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M34" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N34">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O34">
-        <v>2.7</v>
+        <v>2.41</v>
       </c>
       <c r="P34">
-        <v>5.0999999999999996</v>
+        <v>4.97</v>
       </c>
       <c r="Q34">
-        <v>10.8</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R34">
-        <v>21.5</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.45">
@@ -2814,84 +2703,84 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H35" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35">
         <v>4</v>
       </c>
-      <c r="F35" s="2">
-        <v>1</v>
-      </c>
-      <c r="G35" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="H35" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="I35" t="s">
-        <v>11</v>
-      </c>
-      <c r="J35" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35">
-        <v>8</v>
-      </c>
       <c r="L35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M35" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N35">
         <v>1600</v>
       </c>
       <c r="O35">
-        <v>2.9</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P35">
-        <v>6.4</v>
+        <v>5.28</v>
       </c>
       <c r="Q35">
-        <v>12.3</v>
+        <v>10.6</v>
       </c>
       <c r="R35">
-        <v>23.9</v>
+        <v>25.18</v>
+      </c>
+      <c r="S35" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="D36">
         <v>25</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
       </c>
-      <c r="G36" s="3">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="H36" s="3">
-        <v>2.5299999999999998</v>
+      <c r="G36" s="7">
+        <v>2</v>
+      </c>
+      <c r="H36" s="7">
+        <v>2</v>
       </c>
       <c r="I36" t="s">
         <v>11</v>
       </c>
       <c r="K36">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L36">
         <v>2</v>
@@ -2900,78 +2789,75 @@
         <v>27</v>
       </c>
       <c r="N36">
-        <v>1066</v>
+        <v>1600</v>
       </c>
       <c r="O36">
-        <v>3.07</v>
+        <v>2.7</v>
       </c>
       <c r="P36">
-        <v>6.26</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q36">
-        <v>13.37</v>
+        <v>10.8</v>
       </c>
       <c r="R36">
-        <v>26.46</v>
-      </c>
-      <c r="S36" t="s">
-        <v>77</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A37" s="7" t="s">
+      <c r="A37" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D37">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
       </c>
-      <c r="G37" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H37" s="3">
-        <v>3.1</v>
+      <c r="G37" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="H37" s="7">
+        <v>2.1</v>
       </c>
       <c r="I37" t="s">
         <v>11</v>
       </c>
+      <c r="J37" t="s">
+        <v>12</v>
+      </c>
       <c r="K37">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N37">
         <v>1600</v>
       </c>
       <c r="O37">
-        <v>3.56</v>
+        <v>2.9</v>
       </c>
       <c r="P37">
-        <v>8.07</v>
+        <v>6.4</v>
       </c>
       <c r="Q37">
-        <v>15.55</v>
+        <v>12.3</v>
       </c>
       <c r="R37">
-        <v>34.93</v>
-      </c>
-      <c r="S37" t="s">
-        <v>58</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.45">
@@ -2982,10 +2868,10 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="D38">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -2993,94 +2879,97 @@
       <c r="F38" s="2">
         <v>1</v>
       </c>
-      <c r="G38" s="3">
-        <v>2</v>
-      </c>
-      <c r="H38" s="3">
-        <v>2</v>
+      <c r="G38" s="7">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="H38" s="7">
+        <v>2.5299999999999998</v>
       </c>
       <c r="I38" t="s">
         <v>11</v>
       </c>
       <c r="K38">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L38">
         <v>2</v>
       </c>
       <c r="M38" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="N38">
-        <v>667</v>
+        <v>1066</v>
       </c>
       <c r="O38">
-        <v>3.8</v>
+        <v>3.07</v>
       </c>
       <c r="P38">
-        <v>7.8</v>
+        <v>6.26</v>
       </c>
       <c r="Q38">
-        <v>15.9</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>39</v>
+        <v>13.37</v>
+      </c>
+      <c r="R38">
+        <v>26.46</v>
+      </c>
+      <c r="S38" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>44</v>
+      <c r="A39" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="1">
-        <v>3.5</v>
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>85</v>
       </c>
       <c r="E39">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F39" s="2">
         <v>1</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H39" s="3">
-        <v>2.4</v>
+      <c r="H39" s="7">
+        <v>3.1</v>
       </c>
       <c r="I39" t="s">
-        <v>48</v>
-      </c>
-      <c r="J39" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K39">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M39" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="N39">
-        <v>1866</v>
+        <v>1600</v>
       </c>
       <c r="O39">
-        <v>8.3000000000000007</v>
+        <v>3.56</v>
       </c>
       <c r="P39">
-        <v>16.100000000000001</v>
+        <v>8.07</v>
       </c>
       <c r="Q39">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="R39" s="1" t="s">
-        <v>39</v>
+        <v>15.55</v>
+      </c>
+      <c r="R39">
+        <v>34.93</v>
+      </c>
+      <c r="S39" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.45">
@@ -3091,46 +2980,46 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
       </c>
-      <c r="G40" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="H40" s="3">
-        <v>1.8</v>
+      <c r="G40" s="7">
+        <v>2</v>
+      </c>
+      <c r="H40" s="7">
+        <v>2</v>
       </c>
       <c r="I40" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="K40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M40" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="N40">
-        <v>1333</v>
+        <v>667</v>
       </c>
       <c r="O40">
-        <v>10.45</v>
+        <v>3.8</v>
       </c>
       <c r="P40">
-        <v>23.55</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>39</v>
+        <v>7.8</v>
+      </c>
+      <c r="Q40">
+        <v>15.9</v>
       </c>
       <c r="R40" s="1" t="s">
         <v>39</v>
@@ -3144,28 +3033,31 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F41" s="2">
-        <v>1</v>
-      </c>
-      <c r="G41" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="H41" s="3">
-        <v>1.8</v>
+        <v>2</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1.86</v>
+      </c>
+      <c r="H41" s="7">
+        <v>1.86</v>
       </c>
       <c r="I41" t="s">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="J41" t="s">
+        <v>12</v>
       </c>
       <c r="K41">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L41">
         <v>1</v>
@@ -3174,96 +3066,258 @@
         <v>27</v>
       </c>
       <c r="N41">
-        <v>1333</v>
+        <v>1066</v>
       </c>
       <c r="O41">
-        <v>11.8</v>
+        <v>5.5</v>
       </c>
       <c r="P41">
-        <v>23.2</v>
+        <v>11.55</v>
       </c>
       <c r="Q41">
-        <v>62</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>39</v>
+        <v>26.51</v>
+      </c>
+      <c r="R41">
+        <v>56.61</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H42" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="I42" t="s">
+        <v>48</v>
+      </c>
+      <c r="J42" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42">
+        <v>6</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42" t="s">
+        <v>46</v>
+      </c>
+      <c r="N42">
+        <v>1866</v>
+      </c>
+      <c r="O42">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P42">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q42">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="2">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="H43" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="I43" t="s">
+        <v>41</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N43">
+        <v>1333</v>
+      </c>
+      <c r="O43">
+        <v>10.45</v>
+      </c>
+      <c r="P43">
+        <v>23.55</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="H44" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="I44" t="s">
+        <v>41</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44" t="s">
+        <v>27</v>
+      </c>
+      <c r="N44">
+        <v>1333</v>
+      </c>
+      <c r="O44">
+        <v>11.8</v>
+      </c>
+      <c r="P44">
+        <v>23.2</v>
+      </c>
+      <c r="Q44">
+        <v>62</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
         <v>42</v>
       </c>
-      <c r="D42">
+      <c r="D45">
         <v>5</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2">
-        <v>1</v>
-      </c>
-      <c r="G42" s="3">
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1</v>
+      </c>
+      <c r="G45" s="7">
         <v>1.4</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H45" s="7">
         <v>1.4</v>
       </c>
-      <c r="I42" t="s">
-        <v>11</v>
-      </c>
-      <c r="J42" t="s">
+      <c r="I45" t="s">
+        <v>11</v>
+      </c>
+      <c r="J45" t="s">
         <v>12</v>
       </c>
-      <c r="K42">
+      <c r="K45">
         <v>8</v>
       </c>
-      <c r="L42">
-        <v>1</v>
-      </c>
-      <c r="M42" t="s">
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45" t="s">
         <v>27</v>
       </c>
-      <c r="N42">
+      <c r="N45">
         <v>1600</v>
       </c>
-      <c r="O42">
+      <c r="O45">
         <v>13.1</v>
       </c>
-      <c r="P42">
+      <c r="P45">
         <v>27.2</v>
       </c>
-      <c r="Q42">
+      <c r="Q45">
         <v>56.8</v>
       </c>
-      <c r="R42">
+      <c r="R45">
         <v>117.2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B1048575">
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1048575">
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>"x86-32"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:R1048575">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
       <formula>"OOM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575">
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3324,15 +3378,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575 L2:L1048575">
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048575">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"DDR4"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"DDR2"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixed number of cores for Epyc 7402 (24, not 12)
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F8D047-3834-46D4-863E-3D8BDBA16810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCF0ED1-1DFF-405F-BECE-8814B7D1965D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -795,7 +795,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O41" sqref="O41"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1613,7 +1613,7 @@
         <v>180</v>
       </c>
       <c r="E15">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2">
         <v>2</v>

</xml_diff>

<commit_message>
added result for Atom N270
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCF0ED1-1DFF-405F-BECE-8814B7D1965D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8812624A-0A25-4228-80A7-4AA37F43CF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="87">
   <si>
     <t>Cores</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Atom D2550</t>
+  </si>
+  <si>
+    <t>Atom N270</t>
   </si>
 </sst>
 </file>
@@ -372,20 +375,63 @@
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -444,6 +490,20 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -471,13 +531,13 @@
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="14"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -791,11 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3299,25 +3359,78 @@
         <v>117.2</v>
       </c>
     </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46">
+        <v>2.5</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2">
+        <v>2</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="H46" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="I46" t="s">
+        <v>41</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46" t="s">
+        <v>38</v>
+      </c>
+      <c r="N46">
+        <v>533</v>
+      </c>
+      <c r="O46">
+        <v>40.65</v>
+      </c>
+      <c r="P46">
+        <v>83.55</v>
+      </c>
+      <c r="Q46">
+        <v>221.53</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B1048575">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1048575">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"x86-32"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:R1048575">
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"OOM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3378,15 +3491,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575 L2:L1048575">
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048575">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"DDR4"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"DDR2"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3407,9 +3520,9 @@
   <conditionalFormatting sqref="P1:P1048575">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="90"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
@@ -3419,9 +3532,9 @@
   <conditionalFormatting sqref="O1:O1048575">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="90"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
@@ -3431,9 +3544,9 @@
   <conditionalFormatting sqref="Q1:Q1048575">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="90"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
@@ -3443,9 +3556,9 @@
   <conditionalFormatting sqref="R1:R1048575">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="90"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>

</xml_diff>

<commit_message>
added results for Ryzen 3950X and Athlon 200GE
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8812624A-0A25-4228-80A7-4AA37F43CF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7338BC33-0BC9-42AA-8775-5F681D2A41DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="90">
   <si>
     <t>Cores</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>Atom N270</t>
+  </si>
+  <si>
+    <t>Athlon 200GE</t>
+  </si>
+  <si>
+    <t>Ryzen Balanced</t>
+  </si>
+  <si>
+    <t>Ryzen 9 3950X</t>
   </si>
 </sst>
 </file>
@@ -375,63 +384,20 @@
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="11">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2A6A6"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -490,20 +456,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -526,18 +478,18 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S49">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -851,11 +803,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N47" sqref="N47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1004,28 +956,31 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="D3">
         <v>105</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="7">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="H3" s="7">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
       </c>
+      <c r="J3" t="s">
+        <v>88</v>
+      </c>
       <c r="K3">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -1034,19 +989,19 @@
         <v>13</v>
       </c>
       <c r="N3">
-        <v>3600</v>
+        <v>3200</v>
       </c>
       <c r="O3">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="P3">
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
       <c r="Q3">
-        <v>0.98</v>
+        <v>0.86</v>
       </c>
       <c r="R3">
-        <v>2.13</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
@@ -1057,52 +1012,49 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D4">
-        <v>180</v>
+        <v>105</v>
       </c>
       <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="7">
+        <v>3.7</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4">
         <v>16</v>
       </c>
-      <c r="F4" s="2">
-        <v>2</v>
-      </c>
-      <c r="G4" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="H4" s="7">
-        <v>4.2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4">
-        <v>64</v>
-      </c>
       <c r="L4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M4" t="s">
         <v>13</v>
       </c>
       <c r="N4">
-        <v>2933</v>
+        <v>3600</v>
       </c>
       <c r="O4">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="P4">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="Q4">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="R4">
-        <v>1.96</v>
-      </c>
-      <c r="S4" t="s">
-        <v>76</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
@@ -1113,52 +1065,52 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D5">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
       </c>
       <c r="G5" s="7">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="H5" s="7">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
       </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
       <c r="K5">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M5" t="s">
         <v>13</v>
       </c>
       <c r="N5">
-        <v>3200</v>
+        <v>2933</v>
       </c>
       <c r="O5">
-        <v>0.31</v>
+        <v>0.26</v>
       </c>
       <c r="P5">
-        <v>0.63</v>
+        <v>0.51</v>
       </c>
       <c r="Q5">
-        <v>1.24</v>
+        <v>0.97</v>
       </c>
       <c r="R5">
-        <v>2.5099999999999998</v>
+        <v>1.96</v>
+      </c>
+      <c r="S5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
@@ -1190,7 +1142,7 @@
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="K6">
         <v>16</v>
@@ -1205,16 +1157,16 @@
         <v>3200</v>
       </c>
       <c r="O6">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="P6">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="Q6">
-        <v>1.3</v>
+        <v>1.24</v>
       </c>
       <c r="R6">
-        <v>2.67</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
@@ -1225,10 +1177,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D7">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -1240,10 +1192,13 @@
         <v>3.2</v>
       </c>
       <c r="H7" s="7">
-        <v>4.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
       </c>
       <c r="K7">
         <v>16</v>
@@ -1255,22 +1210,19 @@
         <v>13</v>
       </c>
       <c r="N7">
-        <v>2400</v>
+        <v>3200</v>
       </c>
       <c r="O7">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="P7">
-        <v>0.76</v>
+        <v>0.66</v>
       </c>
       <c r="Q7">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="R7">
-        <v>3.03</v>
-      </c>
-      <c r="S7" t="s">
-        <v>63</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -1281,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D8">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -1293,16 +1245,13 @@
         <v>2</v>
       </c>
       <c r="G8" s="7">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="H8" s="7">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
-      </c>
-      <c r="J8" t="s">
-        <v>12</v>
       </c>
       <c r="K8">
         <v>16</v>
@@ -1314,19 +1263,22 @@
         <v>13</v>
       </c>
       <c r="N8">
-        <v>3333</v>
+        <v>2400</v>
       </c>
       <c r="O8">
-        <v>0.46</v>
+        <v>0.36</v>
       </c>
       <c r="P8">
-        <v>0.91</v>
+        <v>0.76</v>
       </c>
       <c r="Q8">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="R8">
-        <v>3.59</v>
+        <v>3.03</v>
+      </c>
+      <c r="S8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
@@ -1337,28 +1289,31 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>95</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2">
         <v>2</v>
       </c>
       <c r="G9" s="7">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="H9" s="7">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
       <c r="K9">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L9">
         <v>2</v>
@@ -1367,19 +1322,19 @@
         <v>13</v>
       </c>
       <c r="N9">
-        <v>3200</v>
+        <v>3333</v>
       </c>
       <c r="O9">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="Q9">
         <v>1.8</v>
       </c>
       <c r="R9">
-        <v>3.7</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
@@ -1390,10 +1345,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D10">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E10">
         <v>6</v>
@@ -1402,16 +1357,13 @@
         <v>2</v>
       </c>
       <c r="G10" s="7">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="H10" s="7">
-        <v>3.46</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>12</v>
       </c>
       <c r="K10">
         <v>32</v>
@@ -1423,78 +1375,75 @@
         <v>13</v>
       </c>
       <c r="N10">
-        <v>3066</v>
+        <v>3200</v>
       </c>
       <c r="O10">
         <v>0.5</v>
       </c>
       <c r="P10">
-        <v>1.03</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R10">
-        <v>4.05</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D11">
-        <v>280</v>
+        <v>65</v>
       </c>
       <c r="E11">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="7">
-        <v>1.4</v>
+        <v>3.2</v>
       </c>
       <c r="H11" s="7">
-        <v>1.5</v>
+        <v>3.46</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K11">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L11">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M11" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N11">
-        <v>7200</v>
+        <v>3066</v>
       </c>
       <c r="O11">
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="P11">
-        <v>1.1599999999999999</v>
+        <v>1.03</v>
       </c>
       <c r="Q11">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="R11">
-        <v>3.57</v>
-      </c>
-      <c r="S11" t="s">
-        <v>56</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
@@ -1505,49 +1454,55 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D12">
-        <v>65</v>
+        <v>280</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="7">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="H12" s="7">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
       <c r="K12">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M12" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="N12">
-        <v>2366</v>
+        <v>7200</v>
       </c>
       <c r="O12">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P12">
-        <v>1.1000000000000001</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q12">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="R12">
-        <v>4.5999999999999996</v>
+        <v>3.57</v>
+      </c>
+      <c r="S12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
@@ -1558,10 +1513,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="D13">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -1570,10 +1525,10 @@
         <v>2</v>
       </c>
       <c r="G13" s="7">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="H13" s="7">
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
@@ -1585,51 +1540,48 @@
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N13">
-        <v>1866</v>
+        <v>2366</v>
       </c>
       <c r="O13">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="P13">
-        <v>1.32</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q13">
-        <v>2.68</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R13">
-        <v>5.38</v>
-      </c>
-      <c r="S13" t="s">
-        <v>67</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D14">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F14" s="2">
         <v>2</v>
       </c>
       <c r="G14" s="7">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="H14" s="7">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
@@ -1638,25 +1590,28 @@
         <v>32</v>
       </c>
       <c r="L14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N14">
-        <v>2667</v>
+        <v>1866</v>
       </c>
       <c r="O14">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="P14">
-        <v>1.26</v>
+        <v>1.32</v>
       </c>
       <c r="Q14">
-        <v>2.44</v>
+        <v>2.68</v>
       </c>
       <c r="R14">
-        <v>4.17</v>
+        <v>5.38</v>
+      </c>
+      <c r="S14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
@@ -1720,63 +1675,60 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="H16" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16">
+        <v>32</v>
+      </c>
+      <c r="L16">
         <v>4</v>
-      </c>
-      <c r="F16" s="2">
-        <v>2</v>
-      </c>
-      <c r="G16" s="7">
-        <v>2.1</v>
-      </c>
-      <c r="H16" s="7">
-        <v>3.7</v>
-      </c>
-      <c r="I16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16">
-        <v>16</v>
-      </c>
-      <c r="L16">
-        <v>2</v>
       </c>
       <c r="M16" t="s">
         <v>13</v>
       </c>
       <c r="N16">
-        <v>2400</v>
+        <v>2667</v>
       </c>
       <c r="O16">
-        <v>0.74</v>
+        <v>0.66</v>
       </c>
       <c r="P16">
-        <v>1.53</v>
+        <v>1.26</v>
       </c>
       <c r="Q16">
-        <v>3.17</v>
+        <v>2.44</v>
       </c>
       <c r="R16">
-        <v>6.53</v>
-      </c>
-      <c r="S16" t="s">
-        <v>70</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D17">
         <v>15</v>
@@ -1788,19 +1740,19 @@
         <v>2</v>
       </c>
       <c r="G17" s="7">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="H17" s="7">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
       <c r="K17">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" t="s">
         <v>13</v>
@@ -1809,16 +1761,19 @@
         <v>2400</v>
       </c>
       <c r="O17">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P17">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
       <c r="Q17">
-        <v>3.1</v>
+        <v>3.17</v>
       </c>
       <c r="R17">
-        <v>6.5</v>
+        <v>6.53</v>
+      </c>
+      <c r="S17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
@@ -1829,10 +1784,10 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1841,7 +1796,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="7">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="H18" s="7">
         <v>3.4</v>
@@ -1850,7 +1805,7 @@
         <v>11</v>
       </c>
       <c r="K18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -1865,13 +1820,13 @@
         <v>0.8</v>
       </c>
       <c r="P18">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q18">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R18">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
@@ -1882,10 +1837,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="D19">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1894,240 +1849,240 @@
         <v>2</v>
       </c>
       <c r="G19" s="7">
-        <v>2.2999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="H19" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>13</v>
+      </c>
+      <c r="N19">
+        <v>2400</v>
+      </c>
+      <c r="O19">
+        <v>0.8</v>
+      </c>
+      <c r="P19">
+        <v>1.7</v>
+      </c>
+      <c r="Q19">
         <v>3.3</v>
       </c>
-      <c r="I19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19">
-        <v>16</v>
-      </c>
-      <c r="L19">
-        <v>2</v>
-      </c>
-      <c r="M19" t="s">
-        <v>27</v>
-      </c>
-      <c r="N19">
-        <v>1600</v>
-      </c>
-      <c r="O19">
-        <v>0.81</v>
-      </c>
-      <c r="P19">
-        <v>1.67</v>
-      </c>
-      <c r="Q19">
-        <v>3.45</v>
-      </c>
       <c r="R19">
-        <v>6.87</v>
-      </c>
-      <c r="S19" t="s">
-        <v>79</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D20">
-        <v>280</v>
+        <v>37</v>
       </c>
       <c r="E20">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" s="7">
-        <v>2.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H20" s="7">
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
-      <c r="J20" t="s">
-        <v>12</v>
-      </c>
       <c r="K20">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M20" t="s">
         <v>27</v>
       </c>
       <c r="N20">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O20">
-        <v>0.9</v>
+        <v>0.81</v>
       </c>
       <c r="P20">
-        <v>1.7</v>
+        <v>1.67</v>
       </c>
       <c r="Q20">
-        <v>3.3</v>
+        <v>3.45</v>
       </c>
       <c r="R20">
-        <v>6.6</v>
+        <v>6.87</v>
+      </c>
+      <c r="S20" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D21">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="E21">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="F21" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G21" s="7">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="H21" s="7">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
       <c r="J21" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K21">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L21">
         <v>8</v>
       </c>
       <c r="M21" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N21">
-        <v>7200</v>
+        <v>1333</v>
       </c>
       <c r="O21">
-        <v>1.02</v>
+        <v>0.9</v>
       </c>
       <c r="P21">
-        <v>2.0699999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="Q21">
-        <v>4.8899999999999997</v>
+        <v>3.3</v>
       </c>
       <c r="R21">
-        <v>7.92</v>
-      </c>
-      <c r="S21" t="s">
-        <v>57</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D22">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="E22">
+        <v>68</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H22" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22">
+        <v>16</v>
+      </c>
+      <c r="L22">
         <v>8</v>
       </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="H22" s="7">
-        <v>4</v>
-      </c>
-      <c r="I22" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22">
-        <v>24</v>
-      </c>
-      <c r="L22">
-        <v>2</v>
-      </c>
       <c r="M22" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N22">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O22">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="P22">
-        <v>1.95</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q22">
-        <v>4.09</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R22">
-        <v>8.27</v>
+        <v>7.92</v>
+      </c>
+      <c r="S22" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D23">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="H23" s="7">
         <v>4</v>
       </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="H23" s="7">
-        <v>3.8</v>
-      </c>
       <c r="I23" t="s">
         <v>11</v>
       </c>
       <c r="K23">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -2139,51 +2094,48 @@
         <v>1600</v>
       </c>
       <c r="O23">
-        <v>1.1000000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P23">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="Q23">
-        <v>3.5</v>
+        <v>4.09</v>
       </c>
       <c r="R23">
-        <v>8</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D24">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="E24">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
       </c>
       <c r="G24" s="7">
-        <v>2.5</v>
+        <v>3.4</v>
       </c>
       <c r="H24" s="7">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
       </c>
-      <c r="J24" t="s">
-        <v>12</v>
-      </c>
       <c r="K24">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L24">
         <v>2</v>
@@ -2192,89 +2144,89 @@
         <v>27</v>
       </c>
       <c r="N24">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O24">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P24">
-        <v>2.17</v>
+        <v>1.7</v>
       </c>
       <c r="Q24">
-        <v>4.16</v>
+        <v>3.5</v>
       </c>
       <c r="R24">
-        <v>8.32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="1">
-        <v>3.5</v>
+        <v>51</v>
+      </c>
+      <c r="D25">
+        <v>140</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
       </c>
       <c r="G25" s="7">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="H25" s="7">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="I25" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="J25" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K25">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M25" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N25">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O25">
-        <v>1.26</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P25">
-        <v>2.57</v>
+        <v>2.17</v>
       </c>
       <c r="Q25">
-        <v>5.16</v>
+        <v>4.16</v>
       </c>
       <c r="R25">
-        <v>10.47</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D26">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -2283,16 +2235,16 @@
         <v>2</v>
       </c>
       <c r="G26" s="7">
-        <v>2.2999999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="H26" s="7">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
       </c>
       <c r="K26">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L26">
         <v>2</v>
@@ -2301,78 +2253,75 @@
         <v>13</v>
       </c>
       <c r="N26">
-        <v>2133</v>
+        <v>3000</v>
       </c>
       <c r="O26">
-        <v>1.3</v>
+        <v>1.19</v>
       </c>
       <c r="P26">
-        <v>2.95</v>
+        <v>2.48</v>
       </c>
       <c r="Q26">
-        <v>5.64</v>
+        <v>5.13</v>
       </c>
       <c r="R26">
-        <v>11.92</v>
-      </c>
-      <c r="S26" t="s">
-        <v>81</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3.5</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
       </c>
       <c r="G27" s="7">
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H27" s="7">
-        <v>2.9</v>
+        <v>2.4</v>
       </c>
       <c r="I27" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="J27" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N27">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O27">
-        <v>1.4</v>
+        <v>1.26</v>
       </c>
       <c r="P27">
-        <v>2.78</v>
+        <v>2.57</v>
       </c>
       <c r="Q27">
-        <v>5.76</v>
+        <v>5.16</v>
       </c>
       <c r="R27">
-        <v>11.56</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
@@ -2383,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D28">
         <v>15</v>
@@ -2395,10 +2344,10 @@
         <v>2</v>
       </c>
       <c r="G28" s="7">
-        <v>2.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H28" s="7">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
@@ -2416,125 +2365,128 @@
         <v>2133</v>
       </c>
       <c r="O28">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="P28">
-        <v>2.9</v>
+        <v>2.95</v>
       </c>
       <c r="Q28">
-        <v>5.7</v>
+        <v>5.64</v>
       </c>
       <c r="R28">
-        <v>10.6</v>
+        <v>11.92</v>
+      </c>
+      <c r="S28" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D29">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F29" s="2">
         <v>1</v>
       </c>
       <c r="G29" s="7">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="H29" s="7">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
       </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
       <c r="K29">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L29">
         <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N29">
-        <v>2800</v>
+        <v>1600</v>
       </c>
       <c r="O29">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="P29">
-        <v>2.9</v>
+        <v>2.78</v>
       </c>
       <c r="Q29">
-        <v>6.2</v>
+        <v>5.76</v>
       </c>
       <c r="R29">
-        <v>12.4</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D30">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E30">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F30" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30" s="7">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="H30" s="7">
-        <v>1.3</v>
+        <v>3.5</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
       </c>
-      <c r="J30" t="s">
-        <v>32</v>
-      </c>
       <c r="K30">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L30">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N30">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O30">
         <v>1.5</v>
       </c>
       <c r="P30">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q30">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="R30">
-        <v>10.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
@@ -2542,34 +2494,37 @@
         <v>5</v>
       </c>
       <c r="B31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D31">
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F31" s="2">
         <v>1</v>
       </c>
       <c r="G31" s="7">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="H31" s="7">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
+      <c r="J31" t="s">
+        <v>32</v>
+      </c>
       <c r="K31">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="L31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M31" t="s">
         <v>27</v>
@@ -2578,16 +2533,16 @@
         <v>1333</v>
       </c>
       <c r="O31">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P31">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Q31">
-        <v>6.6</v>
+        <v>5.2</v>
       </c>
       <c r="R31">
-        <v>13.6</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
@@ -2598,10 +2553,10 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D32">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -2610,40 +2565,37 @@
         <v>1</v>
       </c>
       <c r="G32" s="7">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H32" s="7">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="I32" t="s">
         <v>11</v>
       </c>
       <c r="K32">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L32">
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N32">
-        <v>1600</v>
+        <v>2800</v>
       </c>
       <c r="O32">
-        <v>1.76</v>
+        <v>1.5</v>
       </c>
       <c r="P32">
-        <v>3.53</v>
+        <v>2.9</v>
       </c>
       <c r="Q32">
-        <v>7.34</v>
+        <v>6.2</v>
       </c>
       <c r="R32">
-        <v>14.74</v>
-      </c>
-      <c r="S32" t="s">
-        <v>66</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.45">
@@ -2654,119 +2606,119 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="D33">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F33" s="2">
         <v>1</v>
       </c>
       <c r="G33" s="7">
-        <v>2.35</v>
+        <v>3.5</v>
       </c>
       <c r="H33" s="7">
-        <v>3.35</v>
+        <v>3.5</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
       </c>
       <c r="K33">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L33">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M33" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N33">
+        <v>1333</v>
       </c>
       <c r="O33">
-        <v>2.16</v>
+        <v>1.7</v>
       </c>
       <c r="P33">
-        <v>4.42</v>
+        <v>3.2</v>
       </c>
       <c r="Q33">
-        <v>9.2899999999999991</v>
+        <v>6.6</v>
       </c>
       <c r="R33">
-        <v>18.75</v>
-      </c>
-      <c r="S33" t="s">
-        <v>58</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D34">
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="E34">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F34" s="2">
         <v>1</v>
       </c>
       <c r="G34" s="7">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="H34" s="7">
-        <v>2.4</v>
+        <v>3.3</v>
       </c>
       <c r="I34" t="s">
-        <v>52</v>
-      </c>
-      <c r="J34" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K34">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N34">
-        <v>1866</v>
+        <v>1600</v>
       </c>
       <c r="O34">
-        <v>2.41</v>
+        <v>1.76</v>
       </c>
       <c r="P34">
-        <v>4.97</v>
+        <v>3.53</v>
       </c>
       <c r="Q34">
-        <v>10.050000000000001</v>
+        <v>7.34</v>
       </c>
       <c r="R34">
-        <v>21.07</v>
+        <v>14.74</v>
+      </c>
+      <c r="S34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D35">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -2775,93 +2727,93 @@
         <v>1</v>
       </c>
       <c r="G35" s="7">
-        <v>2.2000000000000002</v>
+        <v>2.35</v>
       </c>
       <c r="H35" s="7">
-        <v>3.1</v>
+        <v>3.35</v>
       </c>
       <c r="I35" t="s">
         <v>11</v>
       </c>
       <c r="K35">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L35">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M35" t="s">
         <v>13</v>
       </c>
-      <c r="N35">
-        <v>1600</v>
-      </c>
       <c r="O35">
-        <v>2.4900000000000002</v>
+        <v>2.16</v>
       </c>
       <c r="P35">
-        <v>5.28</v>
+        <v>4.42</v>
       </c>
       <c r="Q35">
-        <v>10.6</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R35">
-        <v>25.18</v>
+        <v>18.75</v>
       </c>
       <c r="S35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D36">
-        <v>25</v>
+        <v>3.5</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
       </c>
       <c r="G36" s="7">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H36" s="7">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="I36" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="J36" t="s">
+        <v>34</v>
       </c>
       <c r="K36">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M36" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N36">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O36">
-        <v>2.7</v>
+        <v>2.41</v>
       </c>
       <c r="P36">
-        <v>5.0999999999999996</v>
+        <v>4.97</v>
       </c>
       <c r="Q36">
-        <v>10.8</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R36">
-        <v>21.5</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.45">
@@ -2872,84 +2824,84 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H37" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37">
         <v>4</v>
       </c>
-      <c r="F37" s="2">
-        <v>1</v>
-      </c>
-      <c r="G37" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="H37" s="7">
-        <v>2.1</v>
-      </c>
-      <c r="I37" t="s">
-        <v>11</v>
-      </c>
-      <c r="J37" t="s">
-        <v>12</v>
-      </c>
-      <c r="K37">
-        <v>8</v>
-      </c>
       <c r="L37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M37" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N37">
         <v>1600</v>
       </c>
       <c r="O37">
-        <v>2.9</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P37">
-        <v>6.4</v>
+        <v>5.28</v>
       </c>
       <c r="Q37">
-        <v>12.3</v>
+        <v>10.6</v>
       </c>
       <c r="R37">
-        <v>23.9</v>
+        <v>25.18</v>
+      </c>
+      <c r="S37" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="D38">
         <v>25</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
       </c>
       <c r="G38" s="7">
-        <v>2.5299999999999998</v>
+        <v>2</v>
       </c>
       <c r="H38" s="7">
-        <v>2.5299999999999998</v>
+        <v>2</v>
       </c>
       <c r="I38" t="s">
         <v>11</v>
       </c>
       <c r="K38">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L38">
         <v>2</v>
@@ -2958,78 +2910,75 @@
         <v>27</v>
       </c>
       <c r="N38">
-        <v>1066</v>
+        <v>1600</v>
       </c>
       <c r="O38">
-        <v>3.07</v>
+        <v>2.7</v>
       </c>
       <c r="P38">
-        <v>6.26</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q38">
-        <v>13.37</v>
+        <v>10.8</v>
       </c>
       <c r="R38">
-        <v>26.46</v>
-      </c>
-      <c r="S38" t="s">
-        <v>77</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A39" s="5" t="s">
+      <c r="A39" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D39">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F39" s="2">
         <v>1</v>
       </c>
       <c r="G39" s="7">
-        <v>2.2000000000000002</v>
+        <v>1.6</v>
       </c>
       <c r="H39" s="7">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="I39" t="s">
         <v>11</v>
       </c>
+      <c r="J39" t="s">
+        <v>12</v>
+      </c>
       <c r="K39">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N39">
         <v>1600</v>
       </c>
       <c r="O39">
-        <v>3.56</v>
+        <v>2.9</v>
       </c>
       <c r="P39">
-        <v>8.07</v>
+        <v>6.4</v>
       </c>
       <c r="Q39">
-        <v>15.55</v>
+        <v>12.3</v>
       </c>
       <c r="R39">
-        <v>34.93</v>
-      </c>
-      <c r="S39" t="s">
-        <v>58</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.45">
@@ -3040,10 +2989,10 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="D40">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -3052,146 +3001,146 @@
         <v>1</v>
       </c>
       <c r="G40" s="7">
-        <v>2</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="H40" s="7">
-        <v>2</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="I40" t="s">
         <v>11</v>
       </c>
       <c r="K40">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L40">
         <v>2</v>
       </c>
       <c r="M40" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="N40">
-        <v>667</v>
+        <v>1066</v>
       </c>
       <c r="O40">
-        <v>3.8</v>
+        <v>3.07</v>
       </c>
       <c r="P40">
-        <v>7.8</v>
+        <v>6.26</v>
       </c>
       <c r="Q40">
-        <v>15.9</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>39</v>
+        <v>13.37</v>
+      </c>
+      <c r="R40">
+        <v>26.46</v>
+      </c>
+      <c r="S40" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+      <c r="A41" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41">
         <v>85</v>
       </c>
-      <c r="D41">
-        <v>10</v>
-      </c>
       <c r="E41">
         <v>2</v>
       </c>
       <c r="F41" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" s="7">
-        <v>1.86</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H41" s="7">
-        <v>1.86</v>
+        <v>3.1</v>
       </c>
       <c r="I41" t="s">
         <v>11</v>
       </c>
-      <c r="J41" t="s">
-        <v>12</v>
-      </c>
       <c r="K41">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M41" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N41">
-        <v>1066</v>
+        <v>1600</v>
       </c>
       <c r="O41">
-        <v>5.5</v>
+        <v>3.56</v>
       </c>
       <c r="P41">
-        <v>11.55</v>
+        <v>8.07</v>
       </c>
       <c r="Q41">
-        <v>26.51</v>
+        <v>15.55</v>
       </c>
       <c r="R41">
-        <v>56.61</v>
+        <v>34.93</v>
+      </c>
+      <c r="S41" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B42" s="2">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="1">
-        <v>3.5</v>
+        <v>37</v>
+      </c>
+      <c r="D42">
+        <v>34</v>
       </c>
       <c r="E42">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F42" s="2">
         <v>1</v>
       </c>
       <c r="G42" s="7">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H42" s="7">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="I42" t="s">
-        <v>48</v>
-      </c>
-      <c r="J42" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K42">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M42" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N42">
-        <v>1866</v>
+        <v>667</v>
       </c>
       <c r="O42">
-        <v>8.3000000000000007</v>
+        <v>3.8</v>
       </c>
       <c r="P42">
-        <v>16.100000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="Q42">
-        <v>33.799999999999997</v>
+        <v>15.9</v>
       </c>
       <c r="R42" s="1" t="s">
         <v>39</v>
@@ -3205,28 +3154,31 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F43" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" s="7">
-        <v>1.3</v>
+        <v>1.86</v>
       </c>
       <c r="H43" s="7">
-        <v>1.8</v>
+        <v>1.86</v>
       </c>
       <c r="I43" t="s">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="J43" t="s">
+        <v>12</v>
       </c>
       <c r="K43">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -3235,69 +3187,72 @@
         <v>27</v>
       </c>
       <c r="N43">
-        <v>1333</v>
+        <v>1066</v>
       </c>
       <c r="O43">
-        <v>10.45</v>
+        <v>5.5</v>
       </c>
       <c r="P43">
-        <v>23.55</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>39</v>
+        <v>11.55</v>
+      </c>
+      <c r="Q43">
+        <v>26.51</v>
+      </c>
+      <c r="R43">
+        <v>56.61</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B44" s="2">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3.5</v>
       </c>
       <c r="E44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F44" s="2">
         <v>1</v>
       </c>
       <c r="G44" s="7">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H44" s="7">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I44" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J44" t="s">
+        <v>34</v>
       </c>
       <c r="K44">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L44">
         <v>1</v>
       </c>
       <c r="M44" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N44">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O44">
-        <v>11.8</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P44">
-        <v>23.2</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="Q44">
-        <v>62</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="R44" s="1" t="s">
         <v>39</v>
@@ -3311,31 +3266,28 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F45" s="2">
         <v>1</v>
       </c>
       <c r="G45" s="7">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H45" s="7">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I45" t="s">
-        <v>11</v>
-      </c>
-      <c r="J45" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K45">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L45">
         <v>1</v>
@@ -3344,19 +3296,19 @@
         <v>27</v>
       </c>
       <c r="N45">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O45">
-        <v>13.1</v>
+        <v>10.45</v>
       </c>
       <c r="P45">
-        <v>27.2</v>
-      </c>
-      <c r="Q45">
-        <v>56.8</v>
-      </c>
-      <c r="R45">
-        <v>117.2</v>
+        <v>23.55</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.45">
@@ -3367,70 +3319,179 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="D46">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F46" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G46" s="7">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="H46" s="7">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="I46" t="s">
         <v>41</v>
       </c>
       <c r="K46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L46">
         <v>1</v>
       </c>
       <c r="M46" t="s">
+        <v>27</v>
+      </c>
+      <c r="N46">
+        <v>1333</v>
+      </c>
+      <c r="O46">
+        <v>11.8</v>
+      </c>
+      <c r="P46">
+        <v>23.2</v>
+      </c>
+      <c r="Q46">
+        <v>62</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1</v>
+      </c>
+      <c r="G47" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H47" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="I47" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47">
+        <v>8</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47" t="s">
+        <v>27</v>
+      </c>
+      <c r="N47">
+        <v>1600</v>
+      </c>
+      <c r="O47">
+        <v>13.1</v>
+      </c>
+      <c r="P47">
+        <v>27.2</v>
+      </c>
+      <c r="Q47">
+        <v>56.8</v>
+      </c>
+      <c r="R47">
+        <v>117.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48">
+        <v>2.5</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2">
+        <v>2</v>
+      </c>
+      <c r="G48" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="H48" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="I48" t="s">
+        <v>41</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48" t="s">
         <v>38</v>
       </c>
-      <c r="N46">
+      <c r="N48">
         <v>533</v>
       </c>
-      <c r="O46">
+      <c r="O48">
         <v>40.65</v>
       </c>
-      <c r="P46">
+      <c r="P48">
         <v>83.55</v>
       </c>
-      <c r="Q46">
+      <c r="Q48">
         <v>221.53</v>
       </c>
-      <c r="R46" s="1" t="s">
+      <c r="R48" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B1048575">
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1048575">
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>"x86-32"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:R1048575">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
       <formula>"OOM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575">
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3491,15 +3552,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048575 L2:L1048575">
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048575">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"DDR4"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"DDR2"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added results for more mobile Ryzen 5's
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7338BC33-0BC9-42AA-8775-5F681D2A41DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA12B2A9-B9B5-4EAB-AEE2-E9412A9992DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="94">
   <si>
     <t>Cores</t>
   </si>
@@ -298,6 +298,18 @@
   </si>
   <si>
     <t>Ryzen 9 3950X</t>
+  </si>
+  <si>
+    <t>Ryzen 5 PRO 4650U</t>
+  </si>
+  <si>
+    <t>ThinkPad T14s</t>
+  </si>
+  <si>
+    <t>Ryzen 5 4500U</t>
+  </si>
+  <si>
+    <t>ThinkPad L14</t>
   </si>
 </sst>
 </file>
@@ -478,7 +490,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
   <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S49">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S50">
     <sortCondition ref="O1:O1048575"/>
   </sortState>
   <tableColumns count="19">
@@ -803,11 +815,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S9" sqref="S9"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1345,22 +1357,22 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="D10">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>6</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="7">
-        <v>3.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H10" s="7">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
@@ -1378,16 +1390,19 @@
         <v>3200</v>
       </c>
       <c r="O10">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="Q10">
-        <v>1.8</v>
+        <v>1.88</v>
       </c>
       <c r="R10">
-        <v>3.7</v>
+        <v>3.75</v>
+      </c>
+      <c r="S10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
@@ -1398,10 +1413,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D11">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -1410,16 +1425,13 @@
         <v>2</v>
       </c>
       <c r="G11" s="7">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="H11" s="7">
-        <v>3.46</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>12</v>
       </c>
       <c r="K11">
         <v>32</v>
@@ -1431,110 +1443,107 @@
         <v>13</v>
       </c>
       <c r="N11">
-        <v>3066</v>
+        <v>3200</v>
       </c>
       <c r="O11">
         <v>0.5</v>
       </c>
       <c r="P11">
-        <v>1.03</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R11">
-        <v>4.05</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D12">
-        <v>280</v>
+        <v>65</v>
       </c>
       <c r="E12">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="7">
-        <v>1.4</v>
+        <v>3.2</v>
       </c>
       <c r="H12" s="7">
-        <v>1.5</v>
+        <v>3.46</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K12">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N12">
-        <v>7200</v>
+        <v>3066</v>
       </c>
       <c r="O12">
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="P12">
-        <v>1.1599999999999999</v>
+        <v>1.03</v>
       </c>
       <c r="Q12">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="R12">
-        <v>3.57</v>
-      </c>
-      <c r="S12" t="s">
-        <v>56</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="D13">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="H13" s="7">
         <v>4</v>
       </c>
-      <c r="F13" s="2">
-        <v>2</v>
-      </c>
-      <c r="G13" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="H13" s="7">
-        <v>4.2</v>
-      </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
       <c r="K13">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -1543,19 +1552,22 @@
         <v>13</v>
       </c>
       <c r="N13">
-        <v>2366</v>
+        <v>3200</v>
       </c>
       <c r="O13">
-        <v>0.6</v>
+        <v>0.51</v>
       </c>
       <c r="P13">
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="Q13">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="R13">
-        <v>4.5999999999999996</v>
+        <v>4.32</v>
+      </c>
+      <c r="S13" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
@@ -1566,131 +1578,134 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>280</v>
+      </c>
+      <c r="E14">
         <v>68</v>
       </c>
-      <c r="D14">
-        <v>45</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
       <c r="F14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="7">
-        <v>2.8</v>
+        <v>1.4</v>
       </c>
       <c r="H14" s="7">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
       <c r="K14">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M14" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N14">
-        <v>1866</v>
+        <v>7200</v>
       </c>
       <c r="O14">
-        <v>0.65</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P14">
-        <v>1.32</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q14">
-        <v>2.68</v>
+        <v>1.9</v>
       </c>
       <c r="R14">
-        <v>5.38</v>
+        <v>3.57</v>
       </c>
       <c r="S14" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="D15">
-        <v>180</v>
+        <v>65</v>
       </c>
       <c r="E15">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F15" s="2">
         <v>2</v>
       </c>
       <c r="G15" s="7">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="H15" s="7">
-        <v>3.35</v>
+        <v>4.2</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
       <c r="K15">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="L15">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M15" t="s">
         <v>13</v>
       </c>
       <c r="N15">
-        <v>2667</v>
+        <v>2366</v>
       </c>
       <c r="O15">
-        <v>0.66</v>
+        <v>0.6</v>
       </c>
       <c r="P15">
-        <v>1.26</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q15">
-        <v>1.91</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R15">
-        <v>3.81</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D16">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="E16">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F16" s="2">
         <v>2</v>
       </c>
       <c r="G16" s="7">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="H16" s="7">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
@@ -1699,25 +1714,28 @@
         <v>32</v>
       </c>
       <c r="L16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N16">
-        <v>2667</v>
+        <v>1866</v>
       </c>
       <c r="O16">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="P16">
-        <v>1.26</v>
+        <v>1.32</v>
       </c>
       <c r="Q16">
-        <v>2.44</v>
+        <v>2.68</v>
       </c>
       <c r="R16">
-        <v>4.17</v>
+        <v>5.38</v>
+      </c>
+      <c r="S16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
@@ -1728,119 +1746,116 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D17">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2">
         <v>2</v>
       </c>
       <c r="G17" s="7">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="H17" s="7">
-        <v>3.7</v>
+        <v>3.35</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
       <c r="K17">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M17" t="s">
         <v>13</v>
       </c>
       <c r="N17">
-        <v>2400</v>
+        <v>2667</v>
       </c>
       <c r="O17">
-        <v>0.74</v>
+        <v>0.66</v>
       </c>
       <c r="P17">
-        <v>1.53</v>
+        <v>1.26</v>
       </c>
       <c r="Q17">
-        <v>3.17</v>
+        <v>1.91</v>
       </c>
       <c r="R17">
-        <v>6.53</v>
-      </c>
-      <c r="S17" t="s">
-        <v>70</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="D18">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="H18" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18">
+        <v>32</v>
+      </c>
+      <c r="L18">
         <v>4</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2</v>
-      </c>
-      <c r="G18" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="H18" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18">
-        <v>4</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
       </c>
       <c r="M18" t="s">
         <v>13</v>
       </c>
       <c r="N18">
-        <v>2400</v>
+        <v>2667</v>
       </c>
       <c r="O18">
-        <v>0.8</v>
+        <v>0.66</v>
       </c>
       <c r="P18">
-        <v>1.5</v>
+        <v>1.26</v>
       </c>
       <c r="Q18">
-        <v>3.1</v>
+        <v>2.44</v>
       </c>
       <c r="R18">
-        <v>6.5</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D19">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1849,19 +1864,19 @@
         <v>2</v>
       </c>
       <c r="G19" s="7">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
       <c r="H19" s="7">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
       </c>
       <c r="K19">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M19" t="s">
         <v>13</v>
@@ -1870,16 +1885,19 @@
         <v>2400</v>
       </c>
       <c r="O19">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P19">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="Q19">
-        <v>3.3</v>
+        <v>3.17</v>
       </c>
       <c r="R19">
-        <v>6.7</v>
+        <v>6.53</v>
+      </c>
+      <c r="S19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
@@ -1890,10 +1908,10 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1902,87 +1920,81 @@
         <v>2</v>
       </c>
       <c r="G20" s="7">
-        <v>2.2999999999999998</v>
+        <v>1.6</v>
       </c>
       <c r="H20" s="7">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
       <c r="K20">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N20">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="O20">
-        <v>0.81</v>
+        <v>0.8</v>
       </c>
       <c r="P20">
-        <v>1.67</v>
+        <v>1.5</v>
       </c>
       <c r="Q20">
-        <v>3.45</v>
+        <v>3.1</v>
       </c>
       <c r="R20">
-        <v>6.87</v>
-      </c>
-      <c r="S20" t="s">
-        <v>79</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="E21">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" s="7">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H21" s="7">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
-      <c r="J21" t="s">
-        <v>12</v>
-      </c>
       <c r="K21">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N21">
-        <v>1333</v>
+        <v>2400</v>
       </c>
       <c r="O21">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P21">
         <v>1.7</v>
@@ -1991,7 +2003,7 @@
         <v>3.3</v>
       </c>
       <c r="R21">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
@@ -2002,55 +2014,52 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="D22">
-        <v>215</v>
+        <v>37</v>
       </c>
       <c r="E22">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="F22" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G22" s="7">
-        <v>1.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H22" s="7">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
-      </c>
-      <c r="J22" t="s">
-        <v>34</v>
       </c>
       <c r="K22">
         <v>16</v>
       </c>
       <c r="L22">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N22">
-        <v>7200</v>
+        <v>1600</v>
       </c>
       <c r="O22">
-        <v>1.02</v>
+        <v>0.81</v>
       </c>
       <c r="P22">
-        <v>2.0699999999999998</v>
+        <v>1.67</v>
       </c>
       <c r="Q22">
-        <v>4.8899999999999997</v>
+        <v>3.45</v>
       </c>
       <c r="R22">
-        <v>7.92</v>
+        <v>6.87</v>
       </c>
       <c r="S22" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
@@ -2058,52 +2067,55 @@
         <v>5</v>
       </c>
       <c r="B23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23">
-        <v>125</v>
+        <v>280</v>
       </c>
       <c r="E23">
+        <v>32</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="H23" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23">
+        <v>64</v>
+      </c>
+      <c r="L23">
         <v>8</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="H23" s="7">
-        <v>4</v>
-      </c>
-      <c r="I23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23">
-        <v>24</v>
-      </c>
-      <c r="L23">
-        <v>2</v>
       </c>
       <c r="M23" t="s">
         <v>27</v>
       </c>
       <c r="N23">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O23">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="P23">
-        <v>1.95</v>
+        <v>1.7</v>
       </c>
       <c r="Q23">
-        <v>4.09</v>
+        <v>3.3</v>
       </c>
       <c r="R23">
-        <v>8.27</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
@@ -2114,49 +2126,55 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D24">
-        <v>77</v>
+        <v>215</v>
       </c>
       <c r="E24">
+        <v>68</v>
+      </c>
+      <c r="F24" s="2">
         <v>4</v>
       </c>
-      <c r="F24" s="2">
-        <v>1</v>
-      </c>
       <c r="G24" s="7">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="H24" s="7">
-        <v>3.8</v>
+        <v>1.5</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
       </c>
+      <c r="J24" t="s">
+        <v>34</v>
+      </c>
       <c r="K24">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M24" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N24">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O24">
-        <v>1.1000000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="P24">
-        <v>1.7</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q24">
-        <v>3.5</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R24">
-        <v>8</v>
+        <v>7.92</v>
+      </c>
+      <c r="S24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
@@ -2167,31 +2185,28 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D25">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E25">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
       </c>
       <c r="G25" s="7">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="H25" s="7">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
       </c>
-      <c r="J25" t="s">
-        <v>12</v>
-      </c>
       <c r="K25">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L25">
         <v>2</v>
@@ -2200,142 +2215,142 @@
         <v>27</v>
       </c>
       <c r="N25">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O25">
-        <v>1.1200000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P25">
-        <v>2.17</v>
+        <v>1.95</v>
       </c>
       <c r="Q25">
-        <v>4.16</v>
+        <v>4.09</v>
       </c>
       <c r="R25">
-        <v>8.32</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="D26">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="7">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="H26" s="7">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
       </c>
       <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26">
+        <v>1600</v>
+      </c>
+      <c r="O26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P26">
+        <v>1.7</v>
+      </c>
+      <c r="Q26">
+        <v>3.5</v>
+      </c>
+      <c r="R26">
         <v>8</v>
-      </c>
-      <c r="L26">
-        <v>2</v>
-      </c>
-      <c r="M26" t="s">
-        <v>13</v>
-      </c>
-      <c r="N26">
-        <v>3000</v>
-      </c>
-      <c r="O26">
-        <v>1.19</v>
-      </c>
-      <c r="P26">
-        <v>2.48</v>
-      </c>
-      <c r="Q26">
-        <v>5.13</v>
-      </c>
-      <c r="R26">
-        <v>10.52</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="1">
-        <v>3.5</v>
+        <v>51</v>
+      </c>
+      <c r="D27">
+        <v>140</v>
       </c>
       <c r="E27">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
       </c>
       <c r="G27" s="7">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="H27" s="7">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="I27" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="J27" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K27">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N27">
-        <v>1866</v>
+        <v>1333</v>
       </c>
       <c r="O27">
-        <v>1.26</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P27">
-        <v>2.57</v>
+        <v>2.17</v>
       </c>
       <c r="Q27">
-        <v>5.16</v>
+        <v>4.16</v>
       </c>
       <c r="R27">
-        <v>10.47</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D28">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -2344,16 +2359,16 @@
         <v>2</v>
       </c>
       <c r="G28" s="7">
-        <v>2.2999999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="H28" s="7">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
       </c>
       <c r="K28">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L28">
         <v>2</v>
@@ -2362,78 +2377,75 @@
         <v>13</v>
       </c>
       <c r="N28">
-        <v>2133</v>
+        <v>3000</v>
       </c>
       <c r="O28">
-        <v>1.3</v>
+        <v>1.19</v>
       </c>
       <c r="P28">
-        <v>2.95</v>
+        <v>2.48</v>
       </c>
       <c r="Q28">
-        <v>5.64</v>
+        <v>5.13</v>
       </c>
       <c r="R28">
-        <v>11.92</v>
-      </c>
-      <c r="S28" t="s">
-        <v>81</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3.5</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F29" s="2">
         <v>1</v>
       </c>
       <c r="G29" s="7">
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H29" s="7">
-        <v>2.9</v>
+        <v>2.4</v>
       </c>
       <c r="I29" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="J29" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K29">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N29">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O29">
-        <v>1.4</v>
+        <v>1.26</v>
       </c>
       <c r="P29">
-        <v>2.78</v>
+        <v>2.57</v>
       </c>
       <c r="Q29">
-        <v>5.76</v>
+        <v>5.16</v>
       </c>
       <c r="R29">
-        <v>11.56</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
@@ -2444,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D30">
         <v>15</v>
@@ -2456,10 +2468,10 @@
         <v>2</v>
       </c>
       <c r="G30" s="7">
-        <v>2.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H30" s="7">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
@@ -2477,16 +2489,19 @@
         <v>2133</v>
       </c>
       <c r="O30">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="P30">
-        <v>2.9</v>
+        <v>2.95</v>
       </c>
       <c r="Q30">
-        <v>5.7</v>
+        <v>5.64</v>
       </c>
       <c r="R30">
-        <v>10.6</v>
+        <v>11.92</v>
+      </c>
+      <c r="S30" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
@@ -2494,55 +2509,55 @@
         <v>5</v>
       </c>
       <c r="B31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="D31">
-        <v>280</v>
+        <v>100</v>
       </c>
       <c r="E31">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F31" s="2">
         <v>1</v>
       </c>
       <c r="G31" s="7">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="H31" s="7">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
       <c r="J31" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="K31">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="L31">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M31" t="s">
         <v>27</v>
       </c>
       <c r="N31">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O31">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="P31">
-        <v>3</v>
+        <v>2.78</v>
       </c>
       <c r="Q31">
-        <v>5.2</v>
+        <v>5.76</v>
       </c>
       <c r="R31">
-        <v>10.9</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
@@ -2553,28 +2568,28 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E32">
         <v>2</v>
       </c>
       <c r="F32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32" s="7">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="H32" s="7">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="I32" t="s">
         <v>11</v>
       </c>
       <c r="K32">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L32">
         <v>2</v>
@@ -2583,7 +2598,7 @@
         <v>13</v>
       </c>
       <c r="N32">
-        <v>2800</v>
+        <v>2133</v>
       </c>
       <c r="O32">
         <v>1.5</v>
@@ -2592,10 +2607,10 @@
         <v>2.9</v>
       </c>
       <c r="Q32">
-        <v>6.2</v>
+        <v>5.7</v>
       </c>
       <c r="R32">
-        <v>12.4</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.45">
@@ -2603,34 +2618,37 @@
         <v>5</v>
       </c>
       <c r="B33" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D33">
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="E33">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F33" s="2">
         <v>1</v>
       </c>
       <c r="G33" s="7">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="H33" s="7">
-        <v>3.5</v>
+        <v>1.3</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
       </c>
+      <c r="J33" t="s">
+        <v>32</v>
+      </c>
       <c r="K33">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="L33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M33" t="s">
         <v>27</v>
@@ -2639,16 +2657,16 @@
         <v>1333</v>
       </c>
       <c r="O33">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P33">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Q33">
-        <v>6.6</v>
+        <v>5.2</v>
       </c>
       <c r="R33">
-        <v>13.6</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.45">
@@ -2659,10 +2677,10 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D34">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -2671,40 +2689,37 @@
         <v>1</v>
       </c>
       <c r="G34" s="7">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="H34" s="7">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="I34" t="s">
         <v>11</v>
       </c>
       <c r="K34">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L34">
         <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N34">
-        <v>1600</v>
+        <v>2800</v>
       </c>
       <c r="O34">
-        <v>1.76</v>
+        <v>1.5</v>
       </c>
       <c r="P34">
-        <v>3.53</v>
+        <v>2.9</v>
       </c>
       <c r="Q34">
-        <v>7.34</v>
+        <v>6.2</v>
       </c>
       <c r="R34">
-        <v>14.74</v>
-      </c>
-      <c r="S34" t="s">
-        <v>66</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.45">
@@ -2715,119 +2730,119 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="D35">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
       </c>
       <c r="G35" s="7">
-        <v>2.35</v>
+        <v>3.5</v>
       </c>
       <c r="H35" s="7">
-        <v>3.35</v>
+        <v>3.5</v>
       </c>
       <c r="I35" t="s">
         <v>11</v>
       </c>
       <c r="K35">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L35">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M35" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N35">
+        <v>1333</v>
       </c>
       <c r="O35">
-        <v>2.16</v>
+        <v>1.7</v>
       </c>
       <c r="P35">
-        <v>4.42</v>
+        <v>3.2</v>
       </c>
       <c r="Q35">
-        <v>9.2899999999999991</v>
+        <v>6.6</v>
       </c>
       <c r="R35">
-        <v>18.75</v>
-      </c>
-      <c r="S35" t="s">
-        <v>58</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D36">
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="E36">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
       </c>
       <c r="G36" s="7">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="H36" s="7">
-        <v>2.4</v>
+        <v>3.3</v>
       </c>
       <c r="I36" t="s">
-        <v>52</v>
-      </c>
-      <c r="J36" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K36">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M36" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N36">
-        <v>1866</v>
+        <v>1600</v>
       </c>
       <c r="O36">
-        <v>2.41</v>
+        <v>1.76</v>
       </c>
       <c r="P36">
-        <v>4.97</v>
+        <v>3.53</v>
       </c>
       <c r="Q36">
-        <v>10.050000000000001</v>
+        <v>7.34</v>
       </c>
       <c r="R36">
-        <v>21.07</v>
+        <v>14.74</v>
+      </c>
+      <c r="S36" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D37">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -2836,93 +2851,93 @@
         <v>1</v>
       </c>
       <c r="G37" s="7">
-        <v>2.2000000000000002</v>
+        <v>2.35</v>
       </c>
       <c r="H37" s="7">
-        <v>3.1</v>
+        <v>3.35</v>
       </c>
       <c r="I37" t="s">
         <v>11</v>
       </c>
       <c r="K37">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L37">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M37" t="s">
         <v>13</v>
       </c>
-      <c r="N37">
-        <v>1600</v>
-      </c>
       <c r="O37">
-        <v>2.4900000000000002</v>
+        <v>2.16</v>
       </c>
       <c r="P37">
-        <v>5.28</v>
+        <v>4.42</v>
       </c>
       <c r="Q37">
-        <v>10.6</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R37">
-        <v>25.18</v>
+        <v>18.75</v>
       </c>
       <c r="S37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D38">
-        <v>25</v>
+        <v>3.5</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
       </c>
       <c r="G38" s="7">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H38" s="7">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="I38" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="J38" t="s">
+        <v>34</v>
       </c>
       <c r="K38">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M38" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N38">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O38">
-        <v>2.7</v>
+        <v>2.41</v>
       </c>
       <c r="P38">
-        <v>5.0999999999999996</v>
+        <v>4.97</v>
       </c>
       <c r="Q38">
-        <v>10.8</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R38">
-        <v>21.5</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.45">
@@ -2933,84 +2948,84 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D39">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H39" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39">
         <v>4</v>
       </c>
-      <c r="F39" s="2">
-        <v>1</v>
-      </c>
-      <c r="G39" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="H39" s="7">
-        <v>2.1</v>
-      </c>
-      <c r="I39" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" t="s">
-        <v>12</v>
-      </c>
-      <c r="K39">
-        <v>8</v>
-      </c>
       <c r="L39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M39" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N39">
         <v>1600</v>
       </c>
       <c r="O39">
-        <v>2.9</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P39">
-        <v>6.4</v>
+        <v>5.28</v>
       </c>
       <c r="Q39">
-        <v>12.3</v>
+        <v>10.6</v>
       </c>
       <c r="R39">
-        <v>23.9</v>
+        <v>25.18</v>
+      </c>
+      <c r="S39" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B40" s="2">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="D40">
         <v>25</v>
       </c>
       <c r="E40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
       </c>
       <c r="G40" s="7">
-        <v>2.5299999999999998</v>
+        <v>2</v>
       </c>
       <c r="H40" s="7">
-        <v>2.5299999999999998</v>
+        <v>2</v>
       </c>
       <c r="I40" t="s">
         <v>11</v>
       </c>
       <c r="K40">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L40">
         <v>2</v>
@@ -3019,78 +3034,75 @@
         <v>27</v>
       </c>
       <c r="N40">
-        <v>1066</v>
+        <v>1600</v>
       </c>
       <c r="O40">
-        <v>3.07</v>
+        <v>2.7</v>
       </c>
       <c r="P40">
-        <v>6.26</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q40">
-        <v>13.37</v>
+        <v>10.8</v>
       </c>
       <c r="R40">
-        <v>26.46</v>
-      </c>
-      <c r="S40" t="s">
-        <v>77</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A41" s="5" t="s">
+      <c r="A41" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D41">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F41" s="2">
         <v>1</v>
       </c>
       <c r="G41" s="7">
-        <v>2.2000000000000002</v>
+        <v>1.6</v>
       </c>
       <c r="H41" s="7">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="I41" t="s">
         <v>11</v>
       </c>
+      <c r="J41" t="s">
+        <v>12</v>
+      </c>
       <c r="K41">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M41" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N41">
         <v>1600</v>
       </c>
       <c r="O41">
-        <v>3.56</v>
+        <v>2.9</v>
       </c>
       <c r="P41">
-        <v>8.07</v>
+        <v>6.4</v>
       </c>
       <c r="Q41">
-        <v>15.55</v>
+        <v>12.3</v>
       </c>
       <c r="R41">
-        <v>34.93</v>
-      </c>
-      <c r="S41" t="s">
-        <v>58</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.45">
@@ -3101,10 +3113,10 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="D42">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -3113,146 +3125,146 @@
         <v>1</v>
       </c>
       <c r="G42" s="7">
-        <v>2</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="H42" s="7">
-        <v>2</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="I42" t="s">
         <v>11</v>
       </c>
       <c r="K42">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L42">
         <v>2</v>
       </c>
       <c r="M42" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="N42">
-        <v>667</v>
+        <v>1066</v>
       </c>
       <c r="O42">
-        <v>3.8</v>
+        <v>3.07</v>
       </c>
       <c r="P42">
-        <v>7.8</v>
+        <v>6.26</v>
       </c>
       <c r="Q42">
-        <v>15.9</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>39</v>
+        <v>13.37</v>
+      </c>
+      <c r="R42">
+        <v>26.46</v>
+      </c>
+      <c r="S42" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B43" s="2">
         <v>1</v>
       </c>
       <c r="C43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43">
         <v>85</v>
       </c>
-      <c r="D43">
-        <v>10</v>
-      </c>
       <c r="E43">
         <v>2</v>
       </c>
       <c r="F43" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="7">
-        <v>1.86</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H43" s="7">
-        <v>1.86</v>
+        <v>3.1</v>
       </c>
       <c r="I43" t="s">
         <v>11</v>
       </c>
-      <c r="J43" t="s">
-        <v>12</v>
-      </c>
       <c r="K43">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M43" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N43">
-        <v>1066</v>
+        <v>1600</v>
       </c>
       <c r="O43">
-        <v>5.5</v>
+        <v>3.56</v>
       </c>
       <c r="P43">
-        <v>11.55</v>
+        <v>8.07</v>
       </c>
       <c r="Q43">
-        <v>26.51</v>
+        <v>15.55</v>
       </c>
       <c r="R43">
-        <v>56.61</v>
+        <v>34.93</v>
+      </c>
+      <c r="S43" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B44" s="2">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D44" s="1">
-        <v>3.5</v>
+        <v>37</v>
+      </c>
+      <c r="D44">
+        <v>34</v>
       </c>
       <c r="E44">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F44" s="2">
         <v>1</v>
       </c>
       <c r="G44" s="7">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="H44" s="7">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>48</v>
-      </c>
-      <c r="J44" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K44">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M44" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N44">
-        <v>1866</v>
+        <v>667</v>
       </c>
       <c r="O44">
-        <v>8.3000000000000007</v>
+        <v>3.8</v>
       </c>
       <c r="P44">
-        <v>16.100000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="Q44">
-        <v>33.799999999999997</v>
+        <v>15.9</v>
       </c>
       <c r="R44" s="1" t="s">
         <v>39</v>
@@ -3266,28 +3278,31 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F45" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G45" s="7">
-        <v>1.3</v>
+        <v>1.86</v>
       </c>
       <c r="H45" s="7">
-        <v>1.8</v>
+        <v>1.86</v>
       </c>
       <c r="I45" t="s">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="J45" t="s">
+        <v>12</v>
       </c>
       <c r="K45">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L45">
         <v>1</v>
@@ -3296,69 +3311,72 @@
         <v>27</v>
       </c>
       <c r="N45">
-        <v>1333</v>
+        <v>1066</v>
       </c>
       <c r="O45">
-        <v>10.45</v>
+        <v>5.5</v>
       </c>
       <c r="P45">
-        <v>23.55</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R45" s="1" t="s">
-        <v>39</v>
+        <v>11.55</v>
+      </c>
+      <c r="Q45">
+        <v>26.51</v>
+      </c>
+      <c r="R45">
+        <v>56.61</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3.5</v>
       </c>
       <c r="E46">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F46" s="2">
         <v>1</v>
       </c>
       <c r="G46" s="7">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H46" s="7">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I46" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J46" t="s">
+        <v>34</v>
       </c>
       <c r="K46">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L46">
         <v>1</v>
       </c>
       <c r="M46" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N46">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O46">
-        <v>11.8</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P46">
-        <v>23.2</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="Q46">
-        <v>62</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="R46" s="1" t="s">
         <v>39</v>
@@ -3372,31 +3390,28 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F47" s="2">
         <v>1</v>
       </c>
       <c r="G47" s="7">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H47" s="7">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I47" t="s">
-        <v>11</v>
-      </c>
-      <c r="J47" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K47">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L47">
         <v>1</v>
@@ -3405,19 +3420,19 @@
         <v>27</v>
       </c>
       <c r="N47">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O47">
-        <v>13.1</v>
+        <v>10.45</v>
       </c>
       <c r="P47">
-        <v>27.2</v>
-      </c>
-      <c r="Q47">
-        <v>56.8</v>
-      </c>
-      <c r="R47">
-        <v>117.2</v>
+        <v>23.55</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.45">
@@ -3428,48 +3443,157 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="D48">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F48" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48" s="7">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="H48" s="7">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="I48" t="s">
         <v>41</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L48">
         <v>1</v>
       </c>
       <c r="M48" t="s">
+        <v>27</v>
+      </c>
+      <c r="N48">
+        <v>1333</v>
+      </c>
+      <c r="O48">
+        <v>11.8</v>
+      </c>
+      <c r="P48">
+        <v>23.2</v>
+      </c>
+      <c r="Q48">
+        <v>62</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="2">
+        <v>1</v>
+      </c>
+      <c r="G49" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H49" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="I49" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49">
+        <v>8</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49" t="s">
+        <v>27</v>
+      </c>
+      <c r="N49">
+        <v>1600</v>
+      </c>
+      <c r="O49">
+        <v>13.1</v>
+      </c>
+      <c r="P49">
+        <v>27.2</v>
+      </c>
+      <c r="Q49">
+        <v>56.8</v>
+      </c>
+      <c r="R49">
+        <v>117.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50">
+        <v>2.5</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2">
+        <v>2</v>
+      </c>
+      <c r="G50" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="H50" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="I50" t="s">
+        <v>41</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50" t="s">
         <v>38</v>
       </c>
-      <c r="N48">
+      <c r="N50">
         <v>533</v>
       </c>
-      <c r="O48">
+      <c r="O50">
         <v>40.65</v>
       </c>
-      <c r="P48">
+      <c r="P50">
         <v>83.55</v>
       </c>
-      <c r="Q48">
+      <c r="Q50">
         <v>221.53</v>
       </c>
-      <c r="R48" s="1" t="s">
+      <c r="R50" s="1" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed some hw details
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA12B2A9-B9B5-4EAB-AEE2-E9412A9992DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60C30FB-63EE-4EF7-941F-22988C77C767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -818,8 +818,8 @@
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3025,7 +3025,7 @@
         <v>11</v>
       </c>
       <c r="K40">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L40">
         <v>2</v>

</xml_diff>

<commit_message>
added results for Epyc 7402 with 1TB RAM
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60C30FB-63EE-4EF7-941F-22988C77C767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57CD3BE-EC6E-4A40-AD02-70CC38DFEEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="95">
   <si>
     <t>Cores</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>ThinkPad L14</t>
+  </si>
+  <si>
+    <t>`1024</t>
   </si>
 </sst>
 </file>
@@ -396,20 +399,63 @@
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="25">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -468,6 +514,77 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -488,20 +605,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048575" totalsRowShown="0">
-  <autoFilter ref="A1:S1048575" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S50">
-    <sortCondition ref="O1:O1048575"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048576" totalsRowShown="0">
+  <autoFilter ref="A1:S1048576" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S51">
+    <sortCondition ref="O1:O1048576"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="21"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -815,11 +932,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K39" sqref="K39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1189,34 +1306,31 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D7">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="H7" s="7">
+        <v>3.35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7">
         <v>8</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2</v>
-      </c>
-      <c r="G7" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="H7" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7">
-        <v>16</v>
-      </c>
-      <c r="L7">
-        <v>2</v>
       </c>
       <c r="M7" t="s">
         <v>13</v>
@@ -1225,16 +1339,16 @@
         <v>3200</v>
       </c>
       <c r="O7">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="P7">
-        <v>0.66</v>
+        <v>0.59</v>
       </c>
       <c r="Q7">
-        <v>1.3</v>
+        <v>0.92</v>
       </c>
       <c r="R7">
-        <v>2.67</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -1245,10 +1359,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D8">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -1260,10 +1374,13 @@
         <v>3.2</v>
       </c>
       <c r="H8" s="7">
-        <v>4.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>32</v>
       </c>
       <c r="K8">
         <v>16</v>
@@ -1275,22 +1392,19 @@
         <v>13</v>
       </c>
       <c r="N8">
-        <v>2400</v>
+        <v>3200</v>
       </c>
       <c r="O8">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="P8">
-        <v>0.76</v>
+        <v>0.66</v>
       </c>
       <c r="Q8">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="R8">
-        <v>3.03</v>
-      </c>
-      <c r="S8" t="s">
-        <v>63</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
@@ -1301,10 +1415,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D9">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1313,16 +1427,13 @@
         <v>2</v>
       </c>
       <c r="G9" s="7">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="H9" s="7">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
       </c>
       <c r="K9">
         <v>16</v>
@@ -1334,19 +1445,22 @@
         <v>13</v>
       </c>
       <c r="N9">
-        <v>3333</v>
+        <v>2400</v>
       </c>
       <c r="O9">
-        <v>0.46</v>
+        <v>0.36</v>
       </c>
       <c r="P9">
-        <v>0.91</v>
+        <v>0.76</v>
       </c>
       <c r="Q9">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="R9">
-        <v>3.59</v>
+        <v>3.03</v>
+      </c>
+      <c r="S9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
@@ -1357,19 +1471,19 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="7">
-        <v>2.2999999999999998</v>
+        <v>3.6</v>
       </c>
       <c r="H10" s="7">
         <v>4</v>
@@ -1377,8 +1491,11 @@
       <c r="I10" t="s">
         <v>11</v>
       </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
       <c r="K10">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -1387,7 +1504,7 @@
         <v>13</v>
       </c>
       <c r="N10">
-        <v>3200</v>
+        <v>3333</v>
       </c>
       <c r="O10">
         <v>0.46</v>
@@ -1396,13 +1513,10 @@
         <v>0.91</v>
       </c>
       <c r="Q10">
-        <v>1.88</v>
+        <v>1.8</v>
       </c>
       <c r="R10">
-        <v>3.75</v>
-      </c>
-      <c r="S10" t="s">
-        <v>93</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
@@ -1413,22 +1527,22 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="D11">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>6</v>
       </c>
       <c r="F11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="7">
-        <v>3.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H11" s="7">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -1446,16 +1560,19 @@
         <v>3200</v>
       </c>
       <c r="O11">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P11">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="Q11">
-        <v>1.8</v>
+        <v>1.88</v>
       </c>
       <c r="R11">
-        <v>3.7</v>
+        <v>3.75</v>
+      </c>
+      <c r="S11" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
@@ -1466,10 +1583,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D12">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -1478,16 +1595,13 @@
         <v>2</v>
       </c>
       <c r="G12" s="7">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="H12" s="7">
-        <v>3.46</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
-      </c>
-      <c r="J12" t="s">
-        <v>12</v>
       </c>
       <c r="K12">
         <v>32</v>
@@ -1499,19 +1613,19 @@
         <v>13</v>
       </c>
       <c r="N12">
-        <v>3066</v>
+        <v>3200</v>
       </c>
       <c r="O12">
         <v>0.5</v>
       </c>
       <c r="P12">
-        <v>1.03</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R12">
-        <v>4.05</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
@@ -1522,10 +1636,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="D13">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -1534,16 +1648,19 @@
         <v>2</v>
       </c>
       <c r="G13" s="7">
-        <v>2.1</v>
+        <v>3.2</v>
       </c>
       <c r="H13" s="7">
-        <v>4</v>
+        <v>3.46</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
       <c r="K13">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -1552,81 +1669,75 @@
         <v>13</v>
       </c>
       <c r="N13">
-        <v>3200</v>
+        <v>3066</v>
       </c>
       <c r="O13">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="P13">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="Q13">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="R13">
-        <v>4.32</v>
-      </c>
-      <c r="S13" t="s">
-        <v>91</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="D14">
-        <v>280</v>
+        <v>25</v>
       </c>
       <c r="E14">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="7">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="H14" s="7">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
-      </c>
-      <c r="J14" t="s">
-        <v>34</v>
       </c>
       <c r="K14">
         <v>16</v>
       </c>
       <c r="L14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N14">
-        <v>7200</v>
+        <v>3200</v>
       </c>
       <c r="O14">
-        <v>0.57999999999999996</v>
+        <v>0.51</v>
       </c>
       <c r="P14">
-        <v>1.1599999999999999</v>
+        <v>1.05</v>
       </c>
       <c r="Q14">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="R14">
-        <v>3.57</v>
+        <v>4.32</v>
       </c>
       <c r="S14" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
@@ -1637,49 +1748,55 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D15">
-        <v>65</v>
+        <v>280</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="7">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="H15" s="7">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
       <c r="K15">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M15" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="N15">
-        <v>2366</v>
+        <v>7200</v>
       </c>
       <c r="O15">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P15">
-        <v>1.1000000000000001</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q15">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="R15">
-        <v>4.5999999999999996</v>
+        <v>3.57</v>
+      </c>
+      <c r="S15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
@@ -1690,10 +1807,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="D16">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1702,10 +1819,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="7">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="H16" s="7">
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
@@ -1717,42 +1834,39 @@
         <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N16">
-        <v>1866</v>
+        <v>2366</v>
       </c>
       <c r="O16">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="P16">
-        <v>1.32</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q16">
-        <v>2.68</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R16">
-        <v>5.38</v>
-      </c>
-      <c r="S16" t="s">
-        <v>67</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D17">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="E17">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F17" s="2">
         <v>2</v>
@@ -1761,34 +1875,37 @@
         <v>2.8</v>
       </c>
       <c r="H17" s="7">
-        <v>3.35</v>
+        <v>3.8</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
       <c r="K17">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="L17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N17">
-        <v>2667</v>
+        <v>1866</v>
       </c>
       <c r="O17">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="P17">
-        <v>1.26</v>
+        <v>1.32</v>
       </c>
       <c r="Q17">
-        <v>1.91</v>
+        <v>2.68</v>
       </c>
       <c r="R17">
-        <v>3.81</v>
+        <v>5.38</v>
+      </c>
+      <c r="S17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
@@ -1799,31 +1916,31 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D18">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="E18">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="H18" s="7">
+        <v>3.35</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18">
+        <v>64</v>
+      </c>
+      <c r="L18">
         <v>8</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2</v>
-      </c>
-      <c r="G18" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="H18" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18">
-        <v>32</v>
-      </c>
-      <c r="L18">
-        <v>4</v>
       </c>
       <c r="M18" t="s">
         <v>13</v>
@@ -1838,10 +1955,10 @@
         <v>1.26</v>
       </c>
       <c r="Q18">
-        <v>2.44</v>
+        <v>1.91</v>
       </c>
       <c r="R18">
-        <v>4.17</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
@@ -1852,63 +1969,60 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D19">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="H19" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19">
+        <v>32</v>
+      </c>
+      <c r="L19">
         <v>4</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7">
-        <v>2.1</v>
-      </c>
-      <c r="H19" s="7">
-        <v>3.7</v>
-      </c>
-      <c r="I19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19">
-        <v>16</v>
-      </c>
-      <c r="L19">
-        <v>2</v>
       </c>
       <c r="M19" t="s">
         <v>13</v>
       </c>
       <c r="N19">
-        <v>2400</v>
+        <v>2667</v>
       </c>
       <c r="O19">
-        <v>0.74</v>
+        <v>0.66</v>
       </c>
       <c r="P19">
-        <v>1.53</v>
+        <v>1.26</v>
       </c>
       <c r="Q19">
-        <v>3.17</v>
+        <v>2.44</v>
       </c>
       <c r="R19">
-        <v>6.53</v>
-      </c>
-      <c r="S19" t="s">
-        <v>70</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D20">
         <v>15</v>
@@ -1920,19 +2034,19 @@
         <v>2</v>
       </c>
       <c r="G20" s="7">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="H20" s="7">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
       <c r="K20">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" t="s">
         <v>13</v>
@@ -1941,16 +2055,19 @@
         <v>2400</v>
       </c>
       <c r="O20">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P20">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
       <c r="Q20">
-        <v>3.1</v>
+        <v>3.17</v>
       </c>
       <c r="R20">
-        <v>6.5</v>
+        <v>6.53</v>
+      </c>
+      <c r="S20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
@@ -1961,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -1973,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="7">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="H21" s="7">
         <v>3.4</v>
@@ -1982,7 +2099,7 @@
         <v>11</v>
       </c>
       <c r="K21">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -1997,13 +2114,13 @@
         <v>0.8</v>
       </c>
       <c r="P21">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q21">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R21">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
@@ -2014,10 +2131,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="D22">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -2026,240 +2143,240 @@
         <v>2</v>
       </c>
       <c r="G22" s="7">
-        <v>2.2999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="H22" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22">
+        <v>8</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22">
+        <v>2400</v>
+      </c>
+      <c r="O22">
+        <v>0.8</v>
+      </c>
+      <c r="P22">
+        <v>1.7</v>
+      </c>
+      <c r="Q22">
         <v>3.3</v>
       </c>
-      <c r="I22" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22">
-        <v>16</v>
-      </c>
-      <c r="L22">
-        <v>2</v>
-      </c>
-      <c r="M22" t="s">
-        <v>27</v>
-      </c>
-      <c r="N22">
-        <v>1600</v>
-      </c>
-      <c r="O22">
-        <v>0.81</v>
-      </c>
-      <c r="P22">
-        <v>1.67</v>
-      </c>
-      <c r="Q22">
-        <v>3.45</v>
-      </c>
       <c r="R22">
-        <v>6.87</v>
-      </c>
-      <c r="S22" t="s">
-        <v>79</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D23">
-        <v>280</v>
+        <v>37</v>
       </c>
       <c r="E23">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="7">
-        <v>2.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H23" s="7">
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
       </c>
-      <c r="J23" t="s">
-        <v>12</v>
-      </c>
       <c r="K23">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M23" t="s">
         <v>27</v>
       </c>
       <c r="N23">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O23">
-        <v>0.9</v>
+        <v>0.81</v>
       </c>
       <c r="P23">
-        <v>1.7</v>
+        <v>1.67</v>
       </c>
       <c r="Q23">
-        <v>3.3</v>
+        <v>3.45</v>
       </c>
       <c r="R23">
-        <v>6.6</v>
+        <v>6.87</v>
+      </c>
+      <c r="S23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D24">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="E24">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="F24" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G24" s="7">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="H24" s="7">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K24">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L24">
         <v>8</v>
       </c>
       <c r="M24" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N24">
-        <v>7200</v>
+        <v>1333</v>
       </c>
       <c r="O24">
-        <v>1.02</v>
+        <v>0.9</v>
       </c>
       <c r="P24">
-        <v>2.0699999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="Q24">
-        <v>4.8899999999999997</v>
+        <v>3.3</v>
       </c>
       <c r="R24">
-        <v>7.92</v>
-      </c>
-      <c r="S24" t="s">
-        <v>57</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D25">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="E25">
+        <v>68</v>
+      </c>
+      <c r="F25" s="2">
+        <v>4</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H25" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25">
+        <v>16</v>
+      </c>
+      <c r="L25">
         <v>8</v>
       </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="H25" s="7">
-        <v>4</v>
-      </c>
-      <c r="I25" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25">
-        <v>24</v>
-      </c>
-      <c r="L25">
-        <v>2</v>
-      </c>
       <c r="M25" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N25">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O25">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="P25">
-        <v>1.95</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q25">
-        <v>4.09</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R25">
-        <v>8.27</v>
+        <v>7.92</v>
+      </c>
+      <c r="S25" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="H26" s="7">
         <v>4</v>
       </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="H26" s="7">
-        <v>3.8</v>
-      </c>
       <c r="I26" t="s">
         <v>11</v>
       </c>
       <c r="K26">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="L26">
         <v>2</v>
@@ -2271,51 +2388,48 @@
         <v>1600</v>
       </c>
       <c r="O26">
-        <v>1.1000000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P26">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="Q26">
-        <v>3.5</v>
+        <v>4.09</v>
       </c>
       <c r="R26">
-        <v>8</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D27">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="E27">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F27" s="2">
         <v>1</v>
       </c>
       <c r="G27" s="7">
-        <v>2.5</v>
+        <v>3.4</v>
       </c>
       <c r="H27" s="7">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
       </c>
-      <c r="J27" t="s">
-        <v>12</v>
-      </c>
       <c r="K27">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L27">
         <v>2</v>
@@ -2324,19 +2438,19 @@
         <v>27</v>
       </c>
       <c r="N27">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O27">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P27">
-        <v>2.17</v>
+        <v>1.7</v>
       </c>
       <c r="Q27">
-        <v>4.16</v>
+        <v>3.5</v>
       </c>
       <c r="R27">
-        <v>8.32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
@@ -2347,464 +2461,467 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="D28">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F28" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" s="7">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="H28" s="7">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
       </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
       <c r="K28">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L28">
         <v>2</v>
       </c>
       <c r="M28" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N28">
-        <v>3000</v>
+        <v>1333</v>
       </c>
       <c r="O28">
-        <v>1.19</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P28">
-        <v>2.48</v>
+        <v>2.17</v>
       </c>
       <c r="Q28">
-        <v>5.13</v>
+        <v>4.16</v>
       </c>
       <c r="R28">
-        <v>10.52</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="1">
-        <v>3.5</v>
+        <v>87</v>
+      </c>
+      <c r="D29">
+        <v>35</v>
       </c>
       <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2</v>
+      </c>
+      <c r="G29" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="H29" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29">
         <v>8</v>
       </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H29" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="I29" t="s">
-        <v>47</v>
-      </c>
-      <c r="J29" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29">
-        <v>6</v>
-      </c>
       <c r="L29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="N29">
-        <v>1866</v>
+        <v>3000</v>
       </c>
       <c r="O29">
-        <v>1.26</v>
+        <v>1.19</v>
       </c>
       <c r="P29">
-        <v>2.57</v>
+        <v>2.48</v>
       </c>
       <c r="Q29">
-        <v>5.16</v>
+        <v>5.13</v>
       </c>
       <c r="R29">
-        <v>10.47</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3.5</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" s="7">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H30" s="7">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="I30" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="J30" t="s">
+        <v>34</v>
       </c>
       <c r="K30">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N30">
-        <v>2133</v>
+        <v>1866</v>
       </c>
       <c r="O30">
-        <v>1.3</v>
+        <v>1.26</v>
       </c>
       <c r="P30">
-        <v>2.95</v>
+        <v>2.57</v>
       </c>
       <c r="Q30">
-        <v>5.64</v>
+        <v>5.16</v>
       </c>
       <c r="R30">
-        <v>11.92</v>
-      </c>
-      <c r="S30" t="s">
-        <v>81</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D31">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="E31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" s="7">
-        <v>2.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H31" s="7">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
-      <c r="J31" t="s">
-        <v>12</v>
-      </c>
       <c r="K31">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L31">
         <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N31">
-        <v>1600</v>
+        <v>2133</v>
       </c>
       <c r="O31">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="P31">
-        <v>2.78</v>
+        <v>2.95</v>
       </c>
       <c r="Q31">
-        <v>5.76</v>
+        <v>5.64</v>
       </c>
       <c r="R31">
-        <v>11.56</v>
+        <v>11.92</v>
+      </c>
+      <c r="S31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="D32">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" s="7">
         <v>2.9</v>
       </c>
       <c r="H32" s="7">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="I32" t="s">
         <v>11</v>
       </c>
+      <c r="J32" t="s">
+        <v>12</v>
+      </c>
       <c r="K32">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L32">
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N32">
-        <v>2133</v>
+        <v>1600</v>
       </c>
       <c r="O32">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="P32">
-        <v>2.9</v>
+        <v>2.78</v>
       </c>
       <c r="Q32">
-        <v>5.7</v>
+        <v>5.76</v>
       </c>
       <c r="R32">
-        <v>10.6</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B33" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D33">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E33">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F33" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" s="7">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="H33" s="7">
-        <v>1.3</v>
+        <v>3.5</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
       </c>
-      <c r="J33" t="s">
-        <v>32</v>
-      </c>
       <c r="K33">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L33">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M33" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N33">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O33">
         <v>1.5</v>
       </c>
       <c r="P33">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q33">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="R33">
-        <v>10.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B34" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D34">
-        <v>51</v>
+        <v>280</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F34" s="2">
         <v>1</v>
       </c>
       <c r="G34" s="7">
-        <v>2.8</v>
+        <v>1.3</v>
       </c>
       <c r="H34" s="7">
-        <v>2.8</v>
+        <v>1.3</v>
       </c>
       <c r="I34" t="s">
         <v>11</v>
       </c>
+      <c r="J34" t="s">
+        <v>32</v>
+      </c>
       <c r="K34">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="L34">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M34" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N34">
-        <v>2800</v>
+        <v>1333</v>
       </c>
       <c r="O34">
         <v>1.5</v>
       </c>
       <c r="P34">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="Q34">
-        <v>6.2</v>
+        <v>5.2</v>
       </c>
       <c r="R34">
-        <v>12.4</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D35">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E35">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
       </c>
       <c r="G35" s="7">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="H35" s="7">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="I35" t="s">
         <v>11</v>
       </c>
       <c r="K35">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L35">
         <v>2</v>
       </c>
       <c r="M35" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N35">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O35">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P35">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q35">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="R35">
-        <v>13.6</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D36">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
       </c>
       <c r="G36" s="7">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
       <c r="H36" s="7">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="I36" t="s">
         <v>11</v>
       </c>
       <c r="K36">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L36">
         <v>2</v>
@@ -2813,36 +2930,33 @@
         <v>27</v>
       </c>
       <c r="N36">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O36">
-        <v>1.76</v>
+        <v>1.7</v>
       </c>
       <c r="P36">
-        <v>3.53</v>
+        <v>3.2</v>
       </c>
       <c r="Q36">
-        <v>7.34</v>
+        <v>6.6</v>
       </c>
       <c r="R36">
-        <v>14.74</v>
-      </c>
-      <c r="S36" t="s">
-        <v>66</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D37">
-        <v>155</v>
+        <v>35</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -2851,110 +2965,110 @@
         <v>1</v>
       </c>
       <c r="G37" s="7">
-        <v>2.35</v>
+        <v>2.6</v>
       </c>
       <c r="H37" s="7">
-        <v>3.35</v>
+        <v>3.3</v>
       </c>
       <c r="I37" t="s">
         <v>11</v>
       </c>
       <c r="K37">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L37">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M37" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N37">
+        <v>1600</v>
       </c>
       <c r="O37">
-        <v>2.16</v>
+        <v>1.76</v>
       </c>
       <c r="P37">
-        <v>4.42</v>
+        <v>3.53</v>
       </c>
       <c r="Q37">
-        <v>9.2899999999999991</v>
+        <v>7.34</v>
       </c>
       <c r="R37">
-        <v>18.75</v>
+        <v>14.74</v>
       </c>
       <c r="S37" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D38">
-        <v>3.5</v>
+        <v>155</v>
       </c>
       <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="H38" s="7">
+        <v>3.35</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38">
         <v>8</v>
       </c>
-      <c r="F38" s="2">
-        <v>1</v>
-      </c>
-      <c r="G38" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H38" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="I38" t="s">
-        <v>52</v>
-      </c>
-      <c r="J38" t="s">
-        <v>34</v>
-      </c>
-      <c r="K38">
-        <v>6</v>
-      </c>
       <c r="L38">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M38" t="s">
-        <v>46</v>
-      </c>
-      <c r="N38">
-        <v>1866</v>
+        <v>13</v>
       </c>
       <c r="O38">
-        <v>2.41</v>
+        <v>2.16</v>
       </c>
       <c r="P38">
-        <v>4.97</v>
+        <v>4.42</v>
       </c>
       <c r="Q38">
-        <v>10.050000000000001</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R38">
-        <v>21.07</v>
+        <v>18.75</v>
+      </c>
+      <c r="S38" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D39">
-        <v>85</v>
+        <v>3.5</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F39" s="2">
         <v>1</v>
@@ -2963,104 +3077,107 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H39" s="7">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="I39" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="J39" t="s">
+        <v>34</v>
       </c>
       <c r="K39">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N39">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O39">
-        <v>2.4900000000000002</v>
+        <v>2.41</v>
       </c>
       <c r="P39">
-        <v>5.28</v>
+        <v>4.97</v>
       </c>
       <c r="Q39">
-        <v>10.6</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R39">
-        <v>25.18</v>
-      </c>
-      <c r="S39" t="s">
-        <v>60</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B40" s="2">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D40">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+      <c r="G40" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H40" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40">
         <v>4</v>
       </c>
-      <c r="F40" s="2">
-        <v>1</v>
-      </c>
-      <c r="G40" s="7">
-        <v>2</v>
-      </c>
-      <c r="H40" s="7">
-        <v>2</v>
-      </c>
-      <c r="I40" t="s">
-        <v>11</v>
-      </c>
-      <c r="K40">
-        <v>8</v>
-      </c>
       <c r="L40">
         <v>2</v>
       </c>
       <c r="M40" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N40">
         <v>1600</v>
       </c>
       <c r="O40">
-        <v>2.7</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P40">
-        <v>5.0999999999999996</v>
+        <v>5.28</v>
       </c>
       <c r="Q40">
-        <v>10.8</v>
+        <v>10.6</v>
       </c>
       <c r="R40">
-        <v>21.5</v>
+        <v>25.18</v>
+      </c>
+      <c r="S40" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -3069,22 +3186,19 @@
         <v>1</v>
       </c>
       <c r="G41" s="7">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="H41" s="7">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="I41" t="s">
         <v>11</v>
-      </c>
-      <c r="J41" t="s">
-        <v>12</v>
       </c>
       <c r="K41">
         <v>8</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M41" t="s">
         <v>27</v>
@@ -3093,16 +3207,16 @@
         <v>1600</v>
       </c>
       <c r="O41">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="P41">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q41">
-        <v>12.3</v>
+        <v>10.8</v>
       </c>
       <c r="R41">
-        <v>23.9</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.45">
@@ -3113,161 +3227,164 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D42">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F42" s="2">
         <v>1</v>
       </c>
       <c r="G42" s="7">
-        <v>2.5299999999999998</v>
+        <v>1.6</v>
       </c>
       <c r="H42" s="7">
-        <v>2.5299999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="I42" t="s">
         <v>11</v>
+      </c>
+      <c r="J42" t="s">
+        <v>12</v>
       </c>
       <c r="K42">
         <v>8</v>
       </c>
       <c r="L42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M42" t="s">
         <v>27</v>
       </c>
       <c r="N42">
+        <v>1600</v>
+      </c>
+      <c r="O42">
+        <v>2.9</v>
+      </c>
+      <c r="P42">
+        <v>6.4</v>
+      </c>
+      <c r="Q42">
+        <v>12.3</v>
+      </c>
+      <c r="R42">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43">
+        <v>25</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="H43" s="7">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43">
+        <v>8</v>
+      </c>
+      <c r="L43">
+        <v>2</v>
+      </c>
+      <c r="M43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N43">
         <v>1066</v>
       </c>
-      <c r="O42">
+      <c r="O43">
         <v>3.07</v>
       </c>
-      <c r="P42">
+      <c r="P43">
         <v>6.26</v>
       </c>
-      <c r="Q42">
+      <c r="Q43">
         <v>13.37</v>
       </c>
-      <c r="R42">
+      <c r="R43">
         <v>26.46</v>
       </c>
-      <c r="S42" t="s">
+      <c r="S43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A44" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="2">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
         <v>50</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <v>85</v>
       </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
-      <c r="F43" s="2">
-        <v>1</v>
-      </c>
-      <c r="G43" s="7">
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H43" s="7">
+      <c r="H44" s="7">
         <v>3.1</v>
       </c>
-      <c r="I43" t="s">
-        <v>11</v>
-      </c>
-      <c r="K43">
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44">
         <v>4</v>
       </c>
-      <c r="L43">
-        <v>2</v>
-      </c>
-      <c r="M43" t="s">
+      <c r="L44">
+        <v>2</v>
+      </c>
+      <c r="M44" t="s">
         <v>13</v>
       </c>
-      <c r="N43">
+      <c r="N44">
         <v>1600</v>
       </c>
-      <c r="O43">
+      <c r="O44">
         <v>3.56</v>
       </c>
-      <c r="P43">
+      <c r="P44">
         <v>8.07</v>
       </c>
-      <c r="Q43">
+      <c r="Q44">
         <v>15.55</v>
       </c>
-      <c r="R43">
+      <c r="R44">
         <v>34.93</v>
       </c>
-      <c r="S43" t="s">
+      <c r="S44" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44">
-        <v>34</v>
-      </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-      <c r="F44" s="2">
-        <v>1</v>
-      </c>
-      <c r="G44" s="7">
-        <v>2</v>
-      </c>
-      <c r="H44" s="7">
-        <v>2</v>
-      </c>
-      <c r="I44" t="s">
-        <v>11</v>
-      </c>
-      <c r="K44">
-        <v>2</v>
-      </c>
-      <c r="L44">
-        <v>2</v>
-      </c>
-      <c r="M44" t="s">
-        <v>38</v>
-      </c>
-      <c r="N44">
-        <v>667</v>
-      </c>
-      <c r="O44">
-        <v>3.8</v>
-      </c>
-      <c r="P44">
-        <v>7.8</v>
-      </c>
-      <c r="Q44">
-        <v>15.9</v>
-      </c>
-      <c r="R44" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.45">
@@ -3278,158 +3395,158 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="D45">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E45">
         <v>2</v>
       </c>
       <c r="F45" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45" s="7">
-        <v>1.86</v>
+        <v>2</v>
       </c>
       <c r="H45" s="7">
-        <v>1.86</v>
+        <v>2</v>
       </c>
       <c r="I45" t="s">
         <v>11</v>
       </c>
-      <c r="J45" t="s">
-        <v>12</v>
-      </c>
       <c r="K45">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M45" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="N45">
-        <v>1066</v>
+        <v>667</v>
       </c>
       <c r="O45">
-        <v>5.5</v>
+        <v>3.8</v>
       </c>
       <c r="P45">
-        <v>11.55</v>
+        <v>7.8</v>
       </c>
       <c r="Q45">
-        <v>26.51</v>
-      </c>
-      <c r="R45">
-        <v>56.61</v>
+        <v>15.9</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B46" s="2">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" s="1">
-        <v>3.5</v>
+        <v>85</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
       </c>
       <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" s="2">
+        <v>2</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1.86</v>
+      </c>
+      <c r="H46" s="7">
+        <v>1.86</v>
+      </c>
+      <c r="I46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46">
         <v>8</v>
       </c>
-      <c r="F46" s="2">
-        <v>1</v>
-      </c>
-      <c r="G46" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H46" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="I46" t="s">
-        <v>48</v>
-      </c>
-      <c r="J46" t="s">
-        <v>34</v>
-      </c>
-      <c r="K46">
-        <v>6</v>
-      </c>
       <c r="L46">
         <v>1</v>
       </c>
       <c r="M46" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N46">
-        <v>1866</v>
+        <v>1066</v>
       </c>
       <c r="O46">
-        <v>8.3000000000000007</v>
+        <v>5.5</v>
       </c>
       <c r="P46">
-        <v>16.100000000000001</v>
+        <v>11.55</v>
       </c>
       <c r="Q46">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="R46" s="1" t="s">
-        <v>39</v>
+        <v>26.51</v>
+      </c>
+      <c r="R46">
+        <v>56.61</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B47" s="2">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D47" s="1">
+        <v>3.5</v>
       </c>
       <c r="E47">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F47" s="2">
         <v>1</v>
       </c>
       <c r="G47" s="7">
-        <v>1.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H47" s="7">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="I47" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J47" t="s">
+        <v>34</v>
       </c>
       <c r="K47">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L47">
         <v>1</v>
       </c>
       <c r="M47" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N47">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O47">
-        <v>10.45</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P47">
-        <v>23.55</v>
-      </c>
-      <c r="Q47" s="1" t="s">
-        <v>39</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q47">
+        <v>33.799999999999997</v>
       </c>
       <c r="R47" s="1" t="s">
         <v>39</v>
@@ -3464,7 +3581,7 @@
         <v>41</v>
       </c>
       <c r="K48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L48">
         <v>1</v>
@@ -3476,13 +3593,13 @@
         <v>1333</v>
       </c>
       <c r="O48">
-        <v>11.8</v>
+        <v>10.45</v>
       </c>
       <c r="P48">
-        <v>23.2</v>
-      </c>
-      <c r="Q48">
-        <v>62</v>
+        <v>23.55</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>39</v>
@@ -3496,31 +3613,28 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F49" s="2">
         <v>1</v>
       </c>
       <c r="G49" s="7">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H49" s="7">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="I49" t="s">
-        <v>11</v>
-      </c>
-      <c r="J49" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K49">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L49">
         <v>1</v>
@@ -3529,19 +3643,19 @@
         <v>27</v>
       </c>
       <c r="N49">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O49">
-        <v>13.1</v>
+        <v>11.8</v>
       </c>
       <c r="P49">
-        <v>27.2</v>
+        <v>23.2</v>
       </c>
       <c r="Q49">
-        <v>56.8</v>
-      </c>
-      <c r="R49">
-        <v>117.2</v>
+        <v>62</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.45">
@@ -3552,74 +3666,130 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1</v>
+      </c>
+      <c r="G50" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H50" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="I50" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" t="s">
+        <v>12</v>
+      </c>
+      <c r="K50">
+        <v>8</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50" t="s">
+        <v>27</v>
+      </c>
+      <c r="N50">
+        <v>1600</v>
+      </c>
+      <c r="O50">
+        <v>13.1</v>
+      </c>
+      <c r="P50">
+        <v>27.2</v>
+      </c>
+      <c r="Q50">
+        <v>56.8</v>
+      </c>
+      <c r="R50">
+        <v>117.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
         <v>86</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <v>2.5</v>
       </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2">
-        <v>2</v>
-      </c>
-      <c r="G50" s="7">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="2">
+        <v>2</v>
+      </c>
+      <c r="G51" s="7">
         <v>1.6</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H51" s="7">
         <v>1.6</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I51" t="s">
         <v>41</v>
       </c>
-      <c r="K50">
-        <v>1</v>
-      </c>
-      <c r="L50">
-        <v>1</v>
-      </c>
-      <c r="M50" t="s">
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51" t="s">
         <v>38</v>
       </c>
-      <c r="N50">
+      <c r="N51">
         <v>533</v>
       </c>
-      <c r="O50">
+      <c r="O51">
         <v>40.65</v>
       </c>
-      <c r="P50">
+      <c r="P51">
         <v>83.55</v>
       </c>
-      <c r="Q50">
+      <c r="Q51">
         <v>221.53</v>
       </c>
-      <c r="R50" s="1" t="s">
+      <c r="R51" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B1048575">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="cellIs" dxfId="6" priority="19" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I1048575">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+  <conditionalFormatting sqref="I2:I1048576">
+    <cfRule type="cellIs" dxfId="5" priority="18" operator="equal">
       <formula>"x86-32"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:R1048575">
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
+  <conditionalFormatting sqref="O2:R1048576">
+    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>"OOM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048575">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="cellIs" dxfId="3" priority="16" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K1048575">
+  <conditionalFormatting sqref="K1:K1048576">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
@@ -3633,7 +3803,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048575">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
@@ -3647,7 +3817,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048575">
+  <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
@@ -3661,7 +3831,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1048575">
+  <conditionalFormatting sqref="G1:H1048576">
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
@@ -3675,20 +3845,20 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048575 L2:L1048575">
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="F2:F1048576 L2:L1048576">
+    <cfRule type="cellIs" dxfId="2" priority="15" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1048575">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+  <conditionalFormatting sqref="M1:M1048576">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>"DDR4"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>"DDR2"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048575">
+  <conditionalFormatting sqref="N1:N1048576">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -3702,7 +3872,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048575">
+  <conditionalFormatting sqref="P1:P1048576">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="percentile" val="10"/>
@@ -3714,7 +3884,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048575">
+  <conditionalFormatting sqref="O1:O1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="percentile" val="10"/>
@@ -3726,7 +3896,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1048575">
+  <conditionalFormatting sqref="Q1:Q1048576">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="percentile" val="10"/>
@@ -3738,7 +3908,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1048575">
+  <conditionalFormatting sqref="R1:R1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="percentile" val="10"/>
@@ -3772,14 +3942,14 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0367AC6D-DDF3-42AF-AC1A-A8D437802C33}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0" direction="leftToRight">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K2:K1048575</xm:sqref>
+          <xm:sqref>K1:K1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{769BD0BC-E3E0-4DCC-B1ED-8FCB849998EF}">
@@ -3790,7 +3960,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D1:D1048575</xm:sqref>
+          <xm:sqref>D1:D1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4F31A67C-5F53-4BA7-A05C-64FCDA72461D}">
@@ -3801,7 +3971,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E1:E1048575</xm:sqref>
+          <xm:sqref>E1:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B3B407FB-2D4D-463A-AD8A-DEC691552228}">
@@ -3812,7 +3982,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G1:H1048575</xm:sqref>
+          <xm:sqref>G1:H1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{463BE009-64FC-4160-9507-16F4AF063486}">
@@ -3823,7 +3993,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N1:N1048575</xm:sqref>
+          <xm:sqref>N1:N1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
added results for Ryzen 7 7700X with 32GB of DDR5
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\raddi.net\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57CD3BE-EC6E-4A40-AD02-70CC38DFEEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A459216-66AD-4528-BA6C-5E25AC0827A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0FBA9384-5EF6-42B8-A1DF-DF2292C35582}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="97">
   <si>
     <t>Cores</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>`1024</t>
+  </si>
+  <si>
+    <t>DDR5</t>
+  </si>
+  <si>
+    <t>Ryzen 7 7700X</t>
   </si>
 </sst>
 </file>
@@ -375,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -387,7 +393,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -399,63 +404,20 @@
     <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="11">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2A6A6"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -514,77 +476,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2A6A6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -607,18 +498,18 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08A46E77-DE31-4947-AB12-B13E0A176F26}" name="Tabulka1" displayName="Tabulka1" ref="A1:S1048576" totalsRowShown="0">
   <autoFilter ref="A1:S1048576" xr:uid="{32AF2267-AEC1-4754-8A50-CBC7ADB168FB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S51">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S52">
     <sortCondition ref="O1:O1048576"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{D916E857-8E67-4CCF-A189-3239FF92D1EF}" name="Manufacturer"/>
-    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{854A30F5-0EAC-49C5-9B1B-A5FE51A057DD}" name="#" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{9CA5BEBB-DF19-41A0-B193-FD1F3F02BB93}" name="CPU Model"/>
     <tableColumn id="3" xr3:uid="{45352AFB-3190-4015-B63B-4F1506C77556}" name="TDP (W)"/>
     <tableColumn id="4" xr3:uid="{0C87E181-3276-456E-94FF-1764A5DD338E}" name="Cores"/>
-    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{B9034861-4CB4-4B99-8D43-368AC05ED78C}" name="SMT" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{BD5DC32B-3569-44C0-A686-1084EDBD2441}" name="Base (GHz)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{B795F37E-43A3-4CAF-94ED-7611DE36D3F4}" name="Turbo (GHz)" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{0876323E-EF6B-4465-9C59-7D1ADF60370B}" name="OS Architecture"/>
     <tableColumn id="9" xr3:uid="{ED459F27-D629-4F70-8FCD-63211A9B7F7F}" name="Power profile"/>
     <tableColumn id="10" xr3:uid="{706A6B35-E968-4B58-A4D9-528BAF5EFB2D}" name="RAM Amount (GB)"/>
@@ -932,11 +823,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA8CAA5-6B51-4AA2-BBFE-A72866FB553F}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -947,8 +838,8 @@
     <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.265625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.86328125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.265625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.86328125" style="6" customWidth="1"/>
     <col min="9" max="9" width="12.3984375" customWidth="1"/>
     <col min="10" max="10" width="20.1328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
@@ -978,10 +869,10 @@
       <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -1026,28 +917,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="D2">
         <v>105</v>
       </c>
       <c r="E2">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2">
         <v>2</v>
       </c>
-      <c r="G2" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="H2" s="7">
-        <v>4.9000000000000004</v>
+      <c r="G2" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="H2" s="6">
+        <v>5.4</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
       </c>
       <c r="K2">
         <v>32</v>
@@ -1056,25 +944,22 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="N2">
-        <v>3761</v>
+        <v>6000</v>
       </c>
       <c r="O2">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="P2">
-        <v>0.42</v>
+        <v>0.36</v>
       </c>
       <c r="Q2">
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
       <c r="R2">
-        <v>1.38</v>
-      </c>
-      <c r="S2" t="s">
-        <v>75</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
@@ -1085,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>105</v>
@@ -1096,20 +981,20 @@
       <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="G3" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="H3" s="7">
-        <v>4.7</v>
+      <c r="G3" s="6">
+        <v>3.4</v>
+      </c>
+      <c r="H3" s="6">
+        <v>4.9000000000000004</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="K3">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -1118,19 +1003,22 @@
         <v>13</v>
       </c>
       <c r="N3">
-        <v>3200</v>
+        <v>3761</v>
       </c>
       <c r="O3">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="P3">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="Q3">
-        <v>0.86</v>
+        <v>0.72</v>
       </c>
       <c r="R3">
-        <v>1.76</v>
+        <v>1.38</v>
+      </c>
+      <c r="S3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
@@ -1141,28 +1029,31 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>105</v>
       </c>
       <c r="E4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="7">
-        <v>3.7</v>
-      </c>
-      <c r="H4" s="7">
-        <v>4.8</v>
+      <c r="G4" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H4" s="6">
+        <v>4.7</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
       </c>
+      <c r="J4" t="s">
+        <v>88</v>
+      </c>
       <c r="K4">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -1171,19 +1062,19 @@
         <v>13</v>
       </c>
       <c r="N4">
-        <v>3600</v>
+        <v>3200</v>
       </c>
       <c r="O4">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="P4">
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
       <c r="Q4">
-        <v>0.98</v>
+        <v>0.86</v>
       </c>
       <c r="R4">
-        <v>2.13</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
@@ -1194,52 +1085,49 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D5">
-        <v>180</v>
+        <v>105</v>
       </c>
       <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3.7</v>
+      </c>
+      <c r="H5" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5">
         <v>16</v>
       </c>
-      <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="H5" s="7">
-        <v>4.2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5">
-        <v>64</v>
-      </c>
       <c r="L5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M5" t="s">
         <v>13</v>
       </c>
       <c r="N5">
-        <v>2933</v>
+        <v>3600</v>
       </c>
       <c r="O5">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="P5">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="Q5">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="R5">
-        <v>1.96</v>
-      </c>
-      <c r="S5" t="s">
-        <v>76</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
@@ -1250,52 +1138,52 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D6">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F6" s="2">
         <v>2</v>
       </c>
-      <c r="G6" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="H6" s="7">
-        <v>4.4000000000000004</v>
+      <c r="G6" s="6">
+        <v>3.4</v>
+      </c>
+      <c r="H6" s="6">
+        <v>4.2</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
       </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
       <c r="K6">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M6" t="s">
         <v>13</v>
       </c>
       <c r="N6">
-        <v>3200</v>
+        <v>2933</v>
       </c>
       <c r="O6">
-        <v>0.31</v>
+        <v>0.26</v>
       </c>
       <c r="P6">
-        <v>0.63</v>
+        <v>0.51</v>
       </c>
       <c r="Q6">
-        <v>1.24</v>
+        <v>0.97</v>
       </c>
       <c r="R6">
-        <v>2.5099999999999998</v>
+        <v>1.96</v>
+      </c>
+      <c r="S6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
@@ -1306,31 +1194,34 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D7">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="E7">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="7">
-        <v>2.8</v>
-      </c>
-      <c r="H7" s="7">
-        <v>3.35</v>
+      <c r="G7" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="H7" s="6">
+        <v>4.4000000000000004</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>94</v>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7">
+        <v>16</v>
       </c>
       <c r="L7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M7" t="s">
         <v>13</v>
@@ -1342,13 +1233,13 @@
         <v>0.31</v>
       </c>
       <c r="P7">
-        <v>0.59</v>
+        <v>0.63</v>
       </c>
       <c r="Q7">
-        <v>0.92</v>
+        <v>1.24</v>
       </c>
       <c r="R7">
-        <v>1.77</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -1359,34 +1250,31 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D8">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="E8">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="H8" s="6">
+        <v>3.35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L8">
         <v>8</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2</v>
-      </c>
-      <c r="G8" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="H8" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8">
-        <v>16</v>
-      </c>
-      <c r="L8">
-        <v>2</v>
       </c>
       <c r="M8" t="s">
         <v>13</v>
@@ -1395,16 +1283,16 @@
         <v>3200</v>
       </c>
       <c r="O8">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="P8">
-        <v>0.66</v>
+        <v>0.59</v>
       </c>
       <c r="Q8">
-        <v>1.3</v>
+        <v>0.92</v>
       </c>
       <c r="R8">
-        <v>2.67</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
@@ -1415,10 +1303,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D9">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1426,14 +1314,17 @@
       <c r="F9" s="2">
         <v>2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>3.2</v>
       </c>
-      <c r="H9" s="7">
-        <v>4.0999999999999996</v>
+      <c r="H9" s="6">
+        <v>4.4000000000000004</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
       </c>
       <c r="K9">
         <v>16</v>
@@ -1445,22 +1336,19 @@
         <v>13</v>
       </c>
       <c r="N9">
-        <v>2400</v>
+        <v>3200</v>
       </c>
       <c r="O9">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="P9">
-        <v>0.76</v>
+        <v>0.66</v>
       </c>
       <c r="Q9">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="R9">
-        <v>3.03</v>
-      </c>
-      <c r="S9" t="s">
-        <v>63</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
@@ -1471,10 +1359,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D10">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -1482,17 +1370,14 @@
       <c r="F10" s="2">
         <v>2</v>
       </c>
-      <c r="G10" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="H10" s="7">
-        <v>4</v>
+      <c r="G10" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="H10" s="6">
+        <v>4.0999999999999996</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>12</v>
       </c>
       <c r="K10">
         <v>16</v>
@@ -1504,19 +1389,22 @@
         <v>13</v>
       </c>
       <c r="N10">
-        <v>3333</v>
+        <v>2400</v>
       </c>
       <c r="O10">
-        <v>0.46</v>
+        <v>0.36</v>
       </c>
       <c r="P10">
-        <v>0.91</v>
+        <v>0.76</v>
       </c>
       <c r="Q10">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="R10">
-        <v>3.59</v>
+        <v>3.03</v>
+      </c>
+      <c r="S10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
@@ -1527,28 +1415,31 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H11" s="7">
+        <v>2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="H11" s="6">
         <v>4</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
       </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
       <c r="K11">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -1557,7 +1448,7 @@
         <v>13</v>
       </c>
       <c r="N11">
-        <v>3200</v>
+        <v>3333</v>
       </c>
       <c r="O11">
         <v>0.46</v>
@@ -1566,13 +1457,10 @@
         <v>0.91</v>
       </c>
       <c r="Q11">
-        <v>1.88</v>
+        <v>1.8</v>
       </c>
       <c r="R11">
-        <v>3.75</v>
-      </c>
-      <c r="S11" t="s">
-        <v>93</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
@@ -1583,22 +1471,22 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="D12">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>6</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
-      </c>
-      <c r="G12" s="7">
-        <v>3.8</v>
-      </c>
-      <c r="H12" s="7">
-        <v>4.4000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H12" s="6">
+        <v>4</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
@@ -1616,16 +1504,19 @@
         <v>3200</v>
       </c>
       <c r="O12">
-        <v>0.5</v>
+        <v>0.46</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="Q12">
-        <v>1.8</v>
+        <v>1.88</v>
       </c>
       <c r="R12">
-        <v>3.7</v>
+        <v>3.75</v>
+      </c>
+      <c r="S12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.45">
@@ -1636,10 +1527,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D13">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -1647,17 +1538,14 @@
       <c r="F13" s="2">
         <v>2</v>
       </c>
-      <c r="G13" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="H13" s="7">
-        <v>3.46</v>
+      <c r="G13" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="H13" s="6">
+        <v>4.4000000000000004</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
-      </c>
-      <c r="J13" t="s">
-        <v>12</v>
       </c>
       <c r="K13">
         <v>32</v>
@@ -1669,19 +1557,19 @@
         <v>13</v>
       </c>
       <c r="N13">
-        <v>3066</v>
+        <v>3200</v>
       </c>
       <c r="O13">
         <v>0.5</v>
       </c>
       <c r="P13">
-        <v>1.03</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R13">
-        <v>4.05</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
@@ -1692,10 +1580,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -1703,17 +1591,20 @@
       <c r="F14" s="2">
         <v>2</v>
       </c>
-      <c r="G14" s="7">
-        <v>2.1</v>
-      </c>
-      <c r="H14" s="7">
-        <v>4</v>
+      <c r="G14" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="H14" s="6">
+        <v>3.46</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
+      <c r="J14" t="s">
+        <v>12</v>
+      </c>
       <c r="K14">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L14">
         <v>2</v>
@@ -1722,81 +1613,75 @@
         <v>13</v>
       </c>
       <c r="N14">
-        <v>3200</v>
+        <v>3066</v>
       </c>
       <c r="O14">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="P14">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="Q14">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="R14">
-        <v>4.32</v>
-      </c>
-      <c r="S14" t="s">
-        <v>91</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="D15">
-        <v>280</v>
+        <v>25</v>
       </c>
       <c r="E15">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="H15" s="7">
-        <v>1.5</v>
+        <v>2</v>
+      </c>
+      <c r="G15" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="H15" s="6">
+        <v>4</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
-      </c>
-      <c r="J15" t="s">
-        <v>34</v>
       </c>
       <c r="K15">
         <v>16</v>
       </c>
       <c r="L15">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M15" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="N15">
-        <v>7200</v>
+        <v>3200</v>
       </c>
       <c r="O15">
-        <v>0.57999999999999996</v>
+        <v>0.51</v>
       </c>
       <c r="P15">
-        <v>1.1599999999999999</v>
+        <v>1.05</v>
       </c>
       <c r="Q15">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="R15">
-        <v>3.57</v>
+        <v>4.32</v>
       </c>
       <c r="S15" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
@@ -1807,49 +1692,55 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D16">
-        <v>65</v>
+        <v>280</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F16" s="2">
-        <v>2</v>
-      </c>
-      <c r="G16" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="H16" s="7">
-        <v>4.2</v>
+        <v>1</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.5</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
       <c r="K16">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M16" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="N16">
-        <v>2366</v>
+        <v>7200</v>
       </c>
       <c r="O16">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P16">
-        <v>1.1000000000000001</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q16">
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="R16">
-        <v>4.5999999999999996</v>
+        <v>3.57</v>
+      </c>
+      <c r="S16" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.45">
@@ -1860,10 +1751,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="D17">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1871,11 +1762,11 @@
       <c r="F17" s="2">
         <v>2</v>
       </c>
-      <c r="G17" s="7">
-        <v>2.8</v>
-      </c>
-      <c r="H17" s="7">
-        <v>3.8</v>
+      <c r="G17" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="H17" s="6">
+        <v>4.2</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
@@ -1887,78 +1778,78 @@
         <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N17">
-        <v>1866</v>
+        <v>2366</v>
       </c>
       <c r="O17">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="P17">
-        <v>1.32</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q17">
-        <v>2.68</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R17">
-        <v>5.38</v>
-      </c>
-      <c r="S17" t="s">
-        <v>67</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D18">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="E18">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F18" s="2">
         <v>2</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>2.8</v>
       </c>
-      <c r="H18" s="7">
-        <v>3.35</v>
+      <c r="H18" s="6">
+        <v>3.8</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
       </c>
       <c r="K18">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="L18">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N18">
-        <v>2667</v>
+        <v>1866</v>
       </c>
       <c r="O18">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
       <c r="P18">
-        <v>1.26</v>
+        <v>1.32</v>
       </c>
       <c r="Q18">
-        <v>1.91</v>
+        <v>2.68</v>
       </c>
       <c r="R18">
-        <v>3.81</v>
+        <v>5.38</v>
+      </c>
+      <c r="S18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
@@ -1969,31 +1860,31 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D19">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="E19">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="H19" s="6">
+        <v>3.35</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19">
+        <v>64</v>
+      </c>
+      <c r="L19">
         <v>8</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="H19" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="I19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19">
-        <v>32</v>
-      </c>
-      <c r="L19">
-        <v>4</v>
       </c>
       <c r="M19" t="s">
         <v>13</v>
@@ -2008,10 +1899,10 @@
         <v>1.26</v>
       </c>
       <c r="Q19">
-        <v>2.44</v>
+        <v>1.91</v>
       </c>
       <c r="R19">
-        <v>4.17</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
@@ -2022,63 +1913,60 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D20">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2</v>
+      </c>
+      <c r="G20" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="H20" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20">
+        <v>32</v>
+      </c>
+      <c r="L20">
         <v>4</v>
-      </c>
-      <c r="F20" s="2">
-        <v>2</v>
-      </c>
-      <c r="G20" s="7">
-        <v>2.1</v>
-      </c>
-      <c r="H20" s="7">
-        <v>3.7</v>
-      </c>
-      <c r="I20" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20">
-        <v>16</v>
-      </c>
-      <c r="L20">
-        <v>2</v>
       </c>
       <c r="M20" t="s">
         <v>13</v>
       </c>
       <c r="N20">
-        <v>2400</v>
+        <v>2667</v>
       </c>
       <c r="O20">
-        <v>0.74</v>
+        <v>0.66</v>
       </c>
       <c r="P20">
-        <v>1.53</v>
+        <v>1.26</v>
       </c>
       <c r="Q20">
-        <v>3.17</v>
+        <v>2.44</v>
       </c>
       <c r="R20">
-        <v>6.53</v>
-      </c>
-      <c r="S20" t="s">
-        <v>70</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D21">
         <v>15</v>
@@ -2089,20 +1977,20 @@
       <c r="F21" s="2">
         <v>2</v>
       </c>
-      <c r="G21" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="H21" s="7">
-        <v>3.4</v>
+      <c r="G21" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="H21" s="6">
+        <v>3.7</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
       <c r="K21">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M21" t="s">
         <v>13</v>
@@ -2111,16 +1999,19 @@
         <v>2400</v>
       </c>
       <c r="O21">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="P21">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
       <c r="Q21">
-        <v>3.1</v>
+        <v>3.17</v>
       </c>
       <c r="R21">
-        <v>6.5</v>
+        <v>6.53</v>
+      </c>
+      <c r="S21" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
@@ -2131,10 +2022,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -2142,17 +2033,17 @@
       <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="G22" s="7">
-        <v>2.8</v>
-      </c>
-      <c r="H22" s="7">
+      <c r="G22" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="H22" s="6">
         <v>3.4</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
       </c>
       <c r="K22">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -2167,13 +2058,13 @@
         <v>0.8</v>
       </c>
       <c r="P22">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="Q22">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="R22">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.45">
@@ -2184,10 +2075,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="D23">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -2195,241 +2086,241 @@
       <c r="F23" s="2">
         <v>2</v>
       </c>
-      <c r="G23" s="7">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H23" s="7">
+      <c r="G23" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="H23" s="6">
+        <v>3.4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23">
+        <v>8</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23">
+        <v>2400</v>
+      </c>
+      <c r="O23">
+        <v>0.8</v>
+      </c>
+      <c r="P23">
+        <v>1.7</v>
+      </c>
+      <c r="Q23">
         <v>3.3</v>
       </c>
-      <c r="I23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23">
-        <v>16</v>
-      </c>
-      <c r="L23">
-        <v>2</v>
-      </c>
-      <c r="M23" t="s">
-        <v>27</v>
-      </c>
-      <c r="N23">
-        <v>1600</v>
-      </c>
-      <c r="O23">
-        <v>0.81</v>
-      </c>
-      <c r="P23">
-        <v>1.67</v>
-      </c>
-      <c r="Q23">
-        <v>3.45</v>
-      </c>
       <c r="R23">
-        <v>6.87</v>
-      </c>
-      <c r="S23" t="s">
-        <v>79</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D24">
-        <v>280</v>
+        <v>37</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
-      </c>
-      <c r="G24" s="7">
-        <v>2.6</v>
-      </c>
-      <c r="H24" s="7">
-        <v>2.9</v>
+        <v>2</v>
+      </c>
+      <c r="G24" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H24" s="6">
+        <v>3.3</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
       </c>
-      <c r="J24" t="s">
-        <v>12</v>
-      </c>
       <c r="K24">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L24">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M24" t="s">
         <v>27</v>
       </c>
       <c r="N24">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O24">
-        <v>0.9</v>
+        <v>0.81</v>
       </c>
       <c r="P24">
-        <v>1.7</v>
+        <v>1.67</v>
       </c>
       <c r="Q24">
-        <v>3.3</v>
+        <v>3.45</v>
       </c>
       <c r="R24">
-        <v>6.6</v>
+        <v>6.87</v>
+      </c>
+      <c r="S24" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D25">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="E25">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="F25" s="2">
-        <v>4</v>
-      </c>
-      <c r="G25" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="H25" s="7">
-        <v>1.5</v>
+        <v>1</v>
+      </c>
+      <c r="G25" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="H25" s="6">
+        <v>2.9</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
       </c>
       <c r="J25" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K25">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="L25">
         <v>8</v>
       </c>
       <c r="M25" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="N25">
-        <v>7200</v>
+        <v>1333</v>
       </c>
       <c r="O25">
-        <v>1.02</v>
+        <v>0.9</v>
       </c>
       <c r="P25">
-        <v>2.0699999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="Q25">
-        <v>4.8899999999999997</v>
+        <v>3.3</v>
       </c>
       <c r="R25">
-        <v>7.92</v>
-      </c>
-      <c r="S25" t="s">
-        <v>57</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D26">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="E26">
+        <v>68</v>
+      </c>
+      <c r="F26" s="2">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26">
+        <v>16</v>
+      </c>
+      <c r="L26">
         <v>8</v>
       </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="H26" s="7">
-        <v>4</v>
-      </c>
-      <c r="I26" t="s">
-        <v>11</v>
-      </c>
-      <c r="K26">
-        <v>24</v>
-      </c>
-      <c r="L26">
-        <v>2</v>
-      </c>
       <c r="M26" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="N26">
-        <v>1600</v>
+        <v>7200</v>
       </c>
       <c r="O26">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="P26">
-        <v>1.95</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Q26">
-        <v>4.09</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="R26">
-        <v>8.27</v>
+        <v>7.92</v>
+      </c>
+      <c r="S26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D27">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="H27" s="6">
         <v>4</v>
       </c>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="H27" s="7">
-        <v>3.8</v>
-      </c>
       <c r="I27" t="s">
         <v>11</v>
       </c>
       <c r="K27">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="L27">
         <v>2</v>
@@ -2441,51 +2332,48 @@
         <v>1600</v>
       </c>
       <c r="O27">
-        <v>1.1000000000000001</v>
+        <v>1.03</v>
       </c>
       <c r="P27">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="Q27">
-        <v>3.5</v>
+        <v>4.09</v>
       </c>
       <c r="R27">
-        <v>8</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D28">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="E28">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F28" s="2">
         <v>1</v>
       </c>
-      <c r="G28" s="7">
-        <v>2.5</v>
-      </c>
-      <c r="H28" s="7">
-        <v>2.5</v>
+      <c r="G28" s="6">
+        <v>3.4</v>
+      </c>
+      <c r="H28" s="6">
+        <v>3.8</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
       </c>
-      <c r="J28" t="s">
-        <v>12</v>
-      </c>
       <c r="K28">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L28">
         <v>2</v>
@@ -2494,19 +2382,19 @@
         <v>27</v>
       </c>
       <c r="N28">
-        <v>1333</v>
+        <v>1600</v>
       </c>
       <c r="O28">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P28">
-        <v>2.17</v>
+        <v>1.7</v>
       </c>
       <c r="Q28">
-        <v>4.16</v>
+        <v>3.5</v>
       </c>
       <c r="R28">
-        <v>8.32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.45">
@@ -2517,464 +2405,467 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="D29">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F29" s="2">
-        <v>2</v>
-      </c>
-      <c r="G29" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="H29" s="7">
-        <v>3.2</v>
+        <v>1</v>
+      </c>
+      <c r="G29" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="H29" s="6">
+        <v>2.5</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
       </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
       <c r="K29">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L29">
         <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N29">
-        <v>3000</v>
+        <v>1333</v>
       </c>
       <c r="O29">
-        <v>1.19</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="P29">
-        <v>2.48</v>
+        <v>2.17</v>
       </c>
       <c r="Q29">
-        <v>5.13</v>
+        <v>4.16</v>
       </c>
       <c r="R29">
-        <v>10.52</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="1">
-        <v>3.5</v>
+        <v>87</v>
+      </c>
+      <c r="D30">
+        <v>35</v>
       </c>
       <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" s="2">
+        <v>2</v>
+      </c>
+      <c r="G30" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="H30" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30">
         <v>8</v>
       </c>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H30" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="I30" t="s">
-        <v>47</v>
-      </c>
-      <c r="J30" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30">
-        <v>6</v>
-      </c>
       <c r="L30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="N30">
-        <v>1866</v>
+        <v>3000</v>
       </c>
       <c r="O30">
-        <v>1.26</v>
+        <v>1.19</v>
       </c>
       <c r="P30">
-        <v>2.57</v>
+        <v>2.48</v>
       </c>
       <c r="Q30">
-        <v>5.16</v>
+        <v>5.13</v>
       </c>
       <c r="R30">
-        <v>10.47</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3.5</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F31" s="2">
-        <v>2</v>
-      </c>
-      <c r="G31" s="7">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H31" s="7">
-        <v>2.8</v>
+        <v>1</v>
+      </c>
+      <c r="G31" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H31" s="6">
+        <v>2.4</v>
       </c>
       <c r="I31" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="J31" t="s">
+        <v>34</v>
       </c>
       <c r="K31">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M31" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N31">
-        <v>2133</v>
+        <v>1866</v>
       </c>
       <c r="O31">
-        <v>1.3</v>
+        <v>1.26</v>
       </c>
       <c r="P31">
-        <v>2.95</v>
+        <v>2.57</v>
       </c>
       <c r="Q31">
-        <v>5.64</v>
+        <v>5.16</v>
       </c>
       <c r="R31">
-        <v>11.92</v>
-      </c>
-      <c r="S31" t="s">
-        <v>81</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D32">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2">
-        <v>1</v>
-      </c>
-      <c r="G32" s="7">
-        <v>2.9</v>
-      </c>
-      <c r="H32" s="7">
-        <v>2.9</v>
+        <v>2</v>
+      </c>
+      <c r="G32" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H32" s="6">
+        <v>2.8</v>
       </c>
       <c r="I32" t="s">
         <v>11</v>
       </c>
-      <c r="J32" t="s">
-        <v>12</v>
-      </c>
       <c r="K32">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L32">
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N32">
-        <v>1600</v>
+        <v>2133</v>
       </c>
       <c r="O32">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="P32">
-        <v>2.78</v>
+        <v>2.95</v>
       </c>
       <c r="Q32">
-        <v>5.76</v>
+        <v>5.64</v>
       </c>
       <c r="R32">
-        <v>11.56</v>
+        <v>11.92</v>
+      </c>
+      <c r="S32" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B33" s="2">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="D33">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F33" s="2">
-        <v>2</v>
-      </c>
-      <c r="G33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6">
         <v>2.9</v>
       </c>
-      <c r="H33" s="7">
-        <v>3.5</v>
+      <c r="H33" s="6">
+        <v>2.9</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
       </c>
+      <c r="J33" t="s">
+        <v>12</v>
+      </c>
       <c r="K33">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L33">
         <v>2</v>
       </c>
       <c r="M33" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N33">
-        <v>2133</v>
+        <v>1600</v>
       </c>
       <c r="O33">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="P33">
-        <v>2.9</v>
+        <v>2.78</v>
       </c>
       <c r="Q33">
-        <v>5.7</v>
+        <v>5.76</v>
       </c>
       <c r="R33">
-        <v>10.6</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D34">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="E34">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="7">
-        <v>1.3</v>
-      </c>
-      <c r="H34" s="7">
-        <v>1.3</v>
+        <v>2</v>
+      </c>
+      <c r="G34" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="H34" s="6">
+        <v>3.5</v>
       </c>
       <c r="I34" t="s">
         <v>11</v>
       </c>
-      <c r="J34" t="s">
-        <v>32</v>
-      </c>
       <c r="K34">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L34">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N34">
-        <v>1333</v>
+        <v>2133</v>
       </c>
       <c r="O34">
         <v>1.5</v>
       </c>
       <c r="P34">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q34">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
       <c r="R34">
-        <v>10.9</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B35" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D35">
-        <v>51</v>
+        <v>280</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
       </c>
-      <c r="G35" s="7">
-        <v>2.8</v>
-      </c>
-      <c r="H35" s="7">
-        <v>2.8</v>
+      <c r="G35" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1.3</v>
       </c>
       <c r="I35" t="s">
         <v>11</v>
       </c>
+      <c r="J35" t="s">
+        <v>32</v>
+      </c>
       <c r="K35">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="L35">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M35" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="N35">
-        <v>2800</v>
+        <v>1333</v>
       </c>
       <c r="O35">
         <v>1.5</v>
       </c>
       <c r="P35">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="Q35">
-        <v>6.2</v>
+        <v>5.2</v>
       </c>
       <c r="R35">
-        <v>12.4</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D36">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E36">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F36" s="2">
         <v>1</v>
       </c>
-      <c r="G36" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="H36" s="7">
-        <v>3.5</v>
+      <c r="G36" s="6">
+        <v>2.8</v>
+      </c>
+      <c r="H36" s="6">
+        <v>2.8</v>
       </c>
       <c r="I36" t="s">
         <v>11</v>
       </c>
       <c r="K36">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L36">
         <v>2</v>
       </c>
       <c r="M36" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N36">
-        <v>1333</v>
+        <v>2800</v>
       </c>
       <c r="O36">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P36">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q36">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="R36">
-        <v>13.6</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D37">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
       </c>
-      <c r="G37" s="7">
-        <v>2.6</v>
-      </c>
-      <c r="H37" s="7">
-        <v>3.3</v>
+      <c r="G37" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H37" s="6">
+        <v>3.5</v>
       </c>
       <c r="I37" t="s">
         <v>11</v>
       </c>
       <c r="K37">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L37">
         <v>2</v>
@@ -2983,36 +2874,33 @@
         <v>27</v>
       </c>
       <c r="N37">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O37">
-        <v>1.76</v>
+        <v>1.7</v>
       </c>
       <c r="P37">
-        <v>3.53</v>
+        <v>3.2</v>
       </c>
       <c r="Q37">
-        <v>7.34</v>
+        <v>6.6</v>
       </c>
       <c r="R37">
-        <v>14.74</v>
-      </c>
-      <c r="S37" t="s">
-        <v>66</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D38">
-        <v>155</v>
+        <v>35</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -3020,217 +2908,220 @@
       <c r="F38" s="2">
         <v>1</v>
       </c>
-      <c r="G38" s="7">
-        <v>2.35</v>
-      </c>
-      <c r="H38" s="7">
-        <v>3.35</v>
+      <c r="G38" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="H38" s="6">
+        <v>3.3</v>
       </c>
       <c r="I38" t="s">
         <v>11</v>
       </c>
       <c r="K38">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L38">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M38" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="N38">
+        <v>1600</v>
       </c>
       <c r="O38">
-        <v>2.16</v>
+        <v>1.76</v>
       </c>
       <c r="P38">
-        <v>4.42</v>
+        <v>3.53</v>
       </c>
       <c r="Q38">
-        <v>9.2899999999999991</v>
+        <v>7.34</v>
       </c>
       <c r="R38">
-        <v>18.75</v>
+        <v>14.74</v>
       </c>
       <c r="S38" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D39">
-        <v>3.5</v>
+        <v>155</v>
       </c>
       <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="6">
+        <v>2.35</v>
+      </c>
+      <c r="H39" s="6">
+        <v>3.35</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39">
         <v>8</v>
       </c>
-      <c r="F39" s="2">
-        <v>1</v>
-      </c>
-      <c r="G39" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H39" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="I39" t="s">
-        <v>52</v>
-      </c>
-      <c r="J39" t="s">
-        <v>34</v>
-      </c>
-      <c r="K39">
-        <v>6</v>
-      </c>
       <c r="L39">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M39" t="s">
-        <v>46</v>
-      </c>
-      <c r="N39">
-        <v>1866</v>
+        <v>13</v>
       </c>
       <c r="O39">
-        <v>2.41</v>
+        <v>2.16</v>
       </c>
       <c r="P39">
-        <v>4.97</v>
+        <v>4.42</v>
       </c>
       <c r="Q39">
-        <v>10.050000000000001</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="R39">
-        <v>21.07</v>
+        <v>18.75</v>
+      </c>
+      <c r="S39" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B40" s="2">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D40">
-        <v>85</v>
+        <v>3.5</v>
       </c>
       <c r="E40">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H40" s="7">
-        <v>3.1</v>
+      <c r="H40" s="6">
+        <v>2.4</v>
       </c>
       <c r="I40" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="J40" t="s">
+        <v>34</v>
       </c>
       <c r="K40">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="N40">
-        <v>1600</v>
+        <v>1866</v>
       </c>
       <c r="O40">
-        <v>2.4900000000000002</v>
+        <v>2.41</v>
       </c>
       <c r="P40">
-        <v>5.28</v>
+        <v>4.97</v>
       </c>
       <c r="Q40">
-        <v>10.6</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R40">
-        <v>25.18</v>
-      </c>
-      <c r="S40" t="s">
-        <v>60</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D41">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
+      <c r="G41" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H41" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41">
         <v>4</v>
       </c>
-      <c r="F41" s="2">
-        <v>1</v>
-      </c>
-      <c r="G41" s="7">
-        <v>2</v>
-      </c>
-      <c r="H41" s="7">
-        <v>2</v>
-      </c>
-      <c r="I41" t="s">
-        <v>11</v>
-      </c>
-      <c r="K41">
-        <v>8</v>
-      </c>
       <c r="L41">
         <v>2</v>
       </c>
       <c r="M41" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N41">
         <v>1600</v>
       </c>
       <c r="O41">
-        <v>2.7</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="P41">
-        <v>5.0999999999999996</v>
+        <v>5.28</v>
       </c>
       <c r="Q41">
-        <v>10.8</v>
+        <v>10.6</v>
       </c>
       <c r="R41">
-        <v>21.5</v>
+        <v>25.18</v>
+      </c>
+      <c r="S41" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B42" s="2">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E42">
         <v>4</v>
@@ -3238,23 +3129,20 @@
       <c r="F42" s="2">
         <v>1</v>
       </c>
-      <c r="G42" s="7">
-        <v>1.6</v>
-      </c>
-      <c r="H42" s="7">
-        <v>2.1</v>
+      <c r="G42" s="6">
+        <v>2</v>
+      </c>
+      <c r="H42" s="6">
+        <v>2</v>
       </c>
       <c r="I42" t="s">
         <v>11</v>
-      </c>
-      <c r="J42" t="s">
-        <v>12</v>
       </c>
       <c r="K42">
         <v>8</v>
       </c>
       <c r="L42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M42" t="s">
         <v>27</v>
@@ -3263,16 +3151,16 @@
         <v>1600</v>
       </c>
       <c r="O42">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="P42">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q42">
-        <v>12.3</v>
+        <v>10.8</v>
       </c>
       <c r="R42">
-        <v>23.9</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.45">
@@ -3283,108 +3171,108 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D43">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F43" s="2">
         <v>1</v>
       </c>
-      <c r="G43" s="7">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="H43" s="7">
-        <v>2.5299999999999998</v>
+      <c r="G43" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="H43" s="6">
+        <v>2.1</v>
       </c>
       <c r="I43" t="s">
         <v>11</v>
+      </c>
+      <c r="J43" t="s">
+        <v>12</v>
       </c>
       <c r="K43">
         <v>8</v>
       </c>
       <c r="L43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M43" t="s">
         <v>27</v>
       </c>
       <c r="N43">
+        <v>1600</v>
+      </c>
+      <c r="O43">
+        <v>2.9</v>
+      </c>
+      <c r="P43">
+        <v>6.4</v>
+      </c>
+      <c r="Q43">
+        <v>12.3</v>
+      </c>
+      <c r="R43">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44">
+        <v>25</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="6">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="H44" s="6">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44">
+        <v>8</v>
+      </c>
+      <c r="L44">
+        <v>2</v>
+      </c>
+      <c r="M44" t="s">
+        <v>27</v>
+      </c>
+      <c r="N44">
         <v>1066</v>
       </c>
-      <c r="O43">
+      <c r="O44">
         <v>3.07</v>
       </c>
-      <c r="P43">
+      <c r="P44">
         <v>6.26</v>
       </c>
-      <c r="Q43">
+      <c r="Q44">
         <v>13.37</v>
       </c>
-      <c r="R43">
+      <c r="R44">
         <v>26.46</v>
       </c>
-      <c r="S43" t="s">
+      <c r="S44" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A44" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44">
-        <v>85</v>
-      </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-      <c r="F44" s="2">
-        <v>1</v>
-      </c>
-      <c r="G44" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H44" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="I44" t="s">
-        <v>11</v>
-      </c>
-      <c r="K44">
-        <v>4</v>
-      </c>
-      <c r="L44">
-        <v>2</v>
-      </c>
-      <c r="M44" t="s">
-        <v>13</v>
-      </c>
-      <c r="N44">
-        <v>1600</v>
-      </c>
-      <c r="O44">
-        <v>3.56</v>
-      </c>
-      <c r="P44">
-        <v>8.07</v>
-      </c>
-      <c r="Q44">
-        <v>15.55</v>
-      </c>
-      <c r="R44">
-        <v>34.93</v>
-      </c>
-      <c r="S44" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.45">
@@ -3395,10 +3283,10 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D45">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -3406,38 +3294,41 @@
       <c r="F45" s="2">
         <v>1</v>
       </c>
-      <c r="G45" s="7">
-        <v>2</v>
-      </c>
-      <c r="H45" s="7">
-        <v>2</v>
+      <c r="G45" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H45" s="6">
+        <v>3.1</v>
       </c>
       <c r="I45" t="s">
         <v>11</v>
       </c>
       <c r="K45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L45">
         <v>2</v>
       </c>
       <c r="M45" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="N45">
-        <v>667</v>
+        <v>1600</v>
       </c>
       <c r="O45">
-        <v>3.8</v>
+        <v>3.56</v>
       </c>
       <c r="P45">
-        <v>7.8</v>
+        <v>8.07</v>
       </c>
       <c r="Q45">
-        <v>15.9</v>
-      </c>
-      <c r="R45" s="1" t="s">
-        <v>39</v>
+        <v>15.55</v>
+      </c>
+      <c r="R45">
+        <v>34.93</v>
+      </c>
+      <c r="S45" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.45">
@@ -3448,158 +3339,158 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="D46">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E46">
         <v>2</v>
       </c>
       <c r="F46" s="2">
-        <v>2</v>
-      </c>
-      <c r="G46" s="7">
-        <v>1.86</v>
-      </c>
-      <c r="H46" s="7">
-        <v>1.86</v>
+        <v>1</v>
+      </c>
+      <c r="G46" s="6">
+        <v>2</v>
+      </c>
+      <c r="H46" s="6">
+        <v>2</v>
       </c>
       <c r="I46" t="s">
         <v>11</v>
       </c>
-      <c r="J46" t="s">
-        <v>12</v>
-      </c>
       <c r="K46">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M46" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="N46">
-        <v>1066</v>
+        <v>667</v>
       </c>
       <c r="O46">
-        <v>5.5</v>
+        <v>3.8</v>
       </c>
       <c r="P46">
-        <v>11.55</v>
+        <v>7.8</v>
       </c>
       <c r="Q46">
-        <v>26.51</v>
-      </c>
-      <c r="R46">
-        <v>56.61</v>
+        <v>15.9</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B47" s="2">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" s="1">
-        <v>3.5</v>
+        <v>85</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
       </c>
       <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" s="2">
+        <v>2</v>
+      </c>
+      <c r="G47" s="6">
+        <v>1.86</v>
+      </c>
+      <c r="H47" s="6">
+        <v>1.86</v>
+      </c>
+      <c r="I47" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47">
         <v>8</v>
       </c>
-      <c r="F47" s="2">
-        <v>1</v>
-      </c>
-      <c r="G47" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H47" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="I47" t="s">
-        <v>48</v>
-      </c>
-      <c r="J47" t="s">
-        <v>34</v>
-      </c>
-      <c r="K47">
-        <v>6</v>
-      </c>
       <c r="L47">
         <v>1</v>
       </c>
       <c r="M47" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="N47">
-        <v>1866</v>
+        <v>1066</v>
       </c>
       <c r="O47">
-        <v>8.3000000000000007</v>
+        <v>5.5</v>
       </c>
       <c r="P47">
-        <v>16.100000000000001</v>
+        <v>11.55</v>
       </c>
       <c r="Q47">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="R47" s="1" t="s">
-        <v>39</v>
+        <v>26.51</v>
+      </c>
+      <c r="R47">
+        <v>56.61</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B48" s="2">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D48" s="1">
+        <v>3.5</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F48" s="2">
         <v>1</v>
       </c>
-      <c r="G48" s="7">
-        <v>1.3</v>
-      </c>
-      <c r="H48" s="7">
-        <v>1.8</v>
+      <c r="G48" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H48" s="6">
+        <v>2.4</v>
       </c>
       <c r="I48" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="J48" t="s">
+        <v>34</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L48">
         <v>1</v>
       </c>
       <c r="M48" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="N48">
-        <v>1333</v>
+        <v>1866</v>
       </c>
       <c r="O48">
-        <v>10.45</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="P48">
-        <v>23.55</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>39</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q48">
+        <v>33.799999999999997</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>39</v>
@@ -3624,17 +3515,17 @@
       <c r="F49" s="2">
         <v>1</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G49" s="6">
         <v>1.3</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49" s="6">
         <v>1.8</v>
       </c>
       <c r="I49" t="s">
         <v>41</v>
       </c>
       <c r="K49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L49">
         <v>1</v>
@@ -3646,13 +3537,13 @@
         <v>1333</v>
       </c>
       <c r="O49">
-        <v>11.8</v>
+        <v>10.45</v>
       </c>
       <c r="P49">
-        <v>23.2</v>
-      </c>
-      <c r="Q49">
-        <v>62</v>
+        <v>23.55</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="R49" s="1" t="s">
         <v>39</v>
@@ -3666,31 +3557,28 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D50">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F50" s="2">
         <v>1</v>
       </c>
-      <c r="G50" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="H50" s="7">
-        <v>1.4</v>
+      <c r="G50" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="H50" s="6">
+        <v>1.8</v>
       </c>
       <c r="I50" t="s">
-        <v>11</v>
-      </c>
-      <c r="J50" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="K50">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L50">
         <v>1</v>
@@ -3699,19 +3587,19 @@
         <v>27</v>
       </c>
       <c r="N50">
-        <v>1600</v>
+        <v>1333</v>
       </c>
       <c r="O50">
-        <v>13.1</v>
+        <v>11.8</v>
       </c>
       <c r="P50">
-        <v>27.2</v>
+        <v>23.2</v>
       </c>
       <c r="Q50">
-        <v>56.8</v>
-      </c>
-      <c r="R50">
-        <v>117.2</v>
+        <v>62</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.45">
@@ -3722,70 +3610,126 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="2">
+        <v>1</v>
+      </c>
+      <c r="G51" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="H51" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="I51" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51">
+        <v>8</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51" t="s">
+        <v>27</v>
+      </c>
+      <c r="N51">
+        <v>1600</v>
+      </c>
+      <c r="O51">
+        <v>13.1</v>
+      </c>
+      <c r="P51">
+        <v>27.2</v>
+      </c>
+      <c r="Q51">
+        <v>56.8</v>
+      </c>
+      <c r="R51">
+        <v>117.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
         <v>86</v>
       </c>
-      <c r="D51">
+      <c r="D52">
         <v>2.5</v>
       </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2">
-        <v>2</v>
-      </c>
-      <c r="G51" s="7">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2">
+        <v>2</v>
+      </c>
+      <c r="G52" s="6">
         <v>1.6</v>
       </c>
-      <c r="H51" s="7">
+      <c r="H52" s="6">
         <v>1.6</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" t="s">
         <v>41</v>
       </c>
-      <c r="K51">
-        <v>1</v>
-      </c>
-      <c r="L51">
-        <v>1</v>
-      </c>
-      <c r="M51" t="s">
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52" t="s">
         <v>38</v>
       </c>
-      <c r="N51">
+      <c r="N52">
         <v>533</v>
       </c>
-      <c r="O51">
+      <c r="O52">
         <v>40.65</v>
       </c>
-      <c r="P51">
+      <c r="P52">
         <v>83.55</v>
       </c>
-      <c r="Q51">
+      <c r="Q52">
         <v>221.53</v>
       </c>
-      <c r="R51" s="1" t="s">
+      <c r="R52" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="6" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1048576">
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>"x86-32"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:R1048576">
-    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
       <formula>"OOM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3846,15 +3790,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576 L2:L1048576">
-    <cfRule type="cellIs" dxfId="2" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"DDR4"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"DDR2"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>